<commit_message>
Bot5 GUI -v 1.0
</commit_message>
<xml_diff>
--- a/CUENTAS DE CAJA IVSA.xlsx
+++ b/CUENTAS DE CAJA IVSA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{E7FEFFEB-5A09-49B6-9D87-359617FDBFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45CFDE40-E5C2-4738-B778-0AF71508455E}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{E7FEFFEB-5A09-49B6-9D87-359617FDBFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C162C00-A340-4162-BFBA-CC7DE95FA878}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="570" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DISTRIBUIDORAS" sheetId="1" r:id="rId1"/>
@@ -644,7 +644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -800,6 +800,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -815,10 +816,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1120,7 +1117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -1675,9 +1672,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4:F38"/>
     </sheetView>
   </sheetViews>
@@ -1688,7 +1685,7 @@
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
@@ -1699,7 +1696,7 @@
       </c>
       <c r="E1" s="61"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -1714,7 +1711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>6</v>
@@ -1725,7 +1722,7 @@
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>7</v>
       </c>
@@ -1741,8 +1738,9 @@
       <c r="E4" s="15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="63"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>7</v>
       </c>
@@ -1758,8 +1756,9 @@
       <c r="E5" s="15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="63"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
@@ -1775,8 +1774,9 @@
       <c r="E6" s="15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="63"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>7</v>
       </c>
@@ -1792,8 +1792,9 @@
       <c r="E7" s="15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="63"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>18</v>
       </c>
@@ -1809,8 +1810,9 @@
       <c r="E8" s="19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="63"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>7</v>
       </c>
@@ -1826,8 +1828,9 @@
       <c r="E9" s="15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="63"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>7</v>
       </c>
@@ -1843,8 +1846,9 @@
       <c r="E10" s="15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="63"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>7</v>
       </c>
@@ -1860,8 +1864,9 @@
       <c r="E11" s="15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="63"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>7</v>
       </c>
@@ -1877,8 +1882,9 @@
       <c r="E12" s="15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="63"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>7</v>
       </c>
@@ -1894,8 +1900,9 @@
       <c r="E13" s="15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="63"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>7</v>
       </c>
@@ -1911,8 +1918,9 @@
       <c r="E14" s="15" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="63"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>7</v>
       </c>
@@ -1928,8 +1936,9 @@
       <c r="E15" s="15" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="63"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>7</v>
       </c>
@@ -1945,8 +1954,9 @@
       <c r="E16" s="15" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="63"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>7</v>
       </c>
@@ -1962,8 +1972,9 @@
       <c r="E17" s="15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="63"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>7</v>
       </c>
@@ -1979,8 +1990,9 @@
       <c r="E18" s="15" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="63"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>45</v>
       </c>
@@ -1996,8 +2008,9 @@
       <c r="E19" s="15" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="63"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>45</v>
       </c>
@@ -2013,8 +2026,9 @@
       <c r="E20" s="15" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="63"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
       <c r="B21" s="21" t="s">
         <v>50</v>
@@ -2024,8 +2038,9 @@
       </c>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="63"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>7</v>
       </c>
@@ -2041,8 +2056,9 @@
       <c r="E22" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="63"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>7</v>
       </c>
@@ -2058,8 +2074,9 @@
       <c r="E23" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="63"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>7</v>
       </c>
@@ -2075,8 +2092,9 @@
       <c r="E24" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="63"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>7</v>
       </c>
@@ -2092,8 +2110,9 @@
       <c r="E25" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="63"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>18</v>
       </c>
@@ -2109,8 +2128,9 @@
       <c r="E26" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="63"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>7</v>
       </c>
@@ -2126,8 +2146,9 @@
       <c r="E27" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="63"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>7</v>
       </c>
@@ -2143,8 +2164,9 @@
       <c r="E28" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="63"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>7</v>
       </c>
@@ -2160,8 +2182,9 @@
       <c r="E29" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="63"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>7</v>
       </c>
@@ -2177,8 +2200,9 @@
       <c r="E30" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="63"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>7</v>
       </c>
@@ -2194,8 +2218,9 @@
       <c r="E31" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="63"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>7</v>
       </c>
@@ -2211,8 +2236,9 @@
       <c r="E32" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F32" s="63"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>7</v>
       </c>
@@ -2228,8 +2254,9 @@
       <c r="E33" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F33" s="63"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>7</v>
       </c>
@@ -2245,8 +2272,9 @@
       <c r="E34" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F34" s="63"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>7</v>
       </c>
@@ -2262,8 +2290,9 @@
       <c r="E35" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F35" s="63"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>7</v>
       </c>
@@ -2279,8 +2308,9 @@
       <c r="E36" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F36" s="63"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>45</v>
       </c>
@@ -2296,8 +2326,9 @@
       <c r="E37" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F37" s="63"/>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>45</v>
       </c>
@@ -2313,23 +2344,24 @@
       <c r="E38" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="63"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>82</v>
       </c>
@@ -2340,6 +2372,6 @@
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.38" bottom="0.27" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967293"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
últimos ajustes Bot5GUI -v 1.00
</commit_message>
<xml_diff>
--- a/CUENTAS DE CAJA IVSA.xlsx
+++ b/CUENTAS DE CAJA IVSA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="8_{E7FEFFEB-5A09-49B6-9D87-359617FDBFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C162C00-A340-4162-BFBA-CC7DE95FA878}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="8_{E7FEFFEB-5A09-49B6-9D87-359617FDBFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FF3F8E0-DE22-441A-B0DE-26E04F1B1DCF}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DISTRIBUIDORAS" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="88">
   <si>
     <t>CAJAS RECAUDADORAS A NIVEL NACIONAL</t>
   </si>
@@ -291,7 +291,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,8 +357,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,8 +396,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -640,11 +653,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -664,7 +686,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -774,6 +795,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -800,12 +837,105 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1117,537 +1247,537 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="52" customWidth="1"/>
-    <col min="2" max="2" width="47.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="31"/>
+    <col min="1" max="1" width="27.28515625" style="51" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="57" t="s">
+      <c r="B1" s="60"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="56"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="F2" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="H2" s="58" t="s">
+      <c r="H2" s="63" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36" t="s">
+      <c r="A3" s="34"/>
+      <c r="B3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="36">
         <v>101010101</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="40" t="s">
+      <c r="A4" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="40">
         <v>101010102</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="24">
         <v>101020101</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="42">
+      <c r="F4" s="41">
         <v>101044012</v>
       </c>
-      <c r="G4" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="44" t="s">
+      <c r="G4" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="40" t="s">
+      <c r="A5" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="40">
         <v>101010106</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="24">
         <v>101020101</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="45">
+      <c r="F5" s="44">
         <v>101044012</v>
       </c>
-      <c r="G5" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H5" s="44" t="s">
+      <c r="G5" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="40" t="s">
+      <c r="A6" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="40">
         <v>101010107</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="24">
         <v>101020101</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="45">
+      <c r="F6" s="44">
         <v>101044032</v>
       </c>
-      <c r="G6" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H6" s="44" t="s">
+      <c r="G6" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="40">
         <v>101010109</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="24">
         <v>101020101</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="45">
+      <c r="F7" s="44">
         <v>101044072</v>
       </c>
-      <c r="G7" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7" s="44" t="s">
+      <c r="G7" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="40" t="s">
+      <c r="A8" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="40">
         <v>101010111</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="24">
         <v>101020101</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="45">
+      <c r="F8" s="44">
         <v>101044022</v>
       </c>
-      <c r="G8" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H8" s="44" t="s">
+      <c r="G8" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9" s="40">
         <v>101010114</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="24">
         <v>101020101</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="45">
+      <c r="F9" s="44">
         <v>101044052</v>
       </c>
-      <c r="G9" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H9" s="44" t="s">
+      <c r="G9" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="41">
+      <c r="C10" s="40">
         <v>101010117</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="24">
         <v>101020101</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="45">
+      <c r="F10" s="44">
         <v>101044062</v>
       </c>
-      <c r="G10" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H10" s="44" t="s">
+      <c r="G10" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C11" s="40">
         <v>101010119</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="24">
         <v>101020101</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="45">
+      <c r="F11" s="44">
         <v>101044042</v>
       </c>
-      <c r="G11" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H11" s="44" t="s">
+      <c r="G11" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="41">
+      <c r="C12" s="40">
         <v>101010121</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="24">
         <v>101020101</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="45">
+      <c r="F12" s="44">
         <v>101044082</v>
       </c>
-      <c r="G12" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H12" s="44" t="s">
+      <c r="G12" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="40" t="s">
+      <c r="A13" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="45">
         <v>101010202</v>
       </c>
-      <c r="D13" s="47">
+      <c r="D13" s="46">
         <v>101020201</v>
       </c>
-      <c r="E13" s="47" t="s">
+      <c r="E13" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="45">
+      <c r="F13" s="44">
         <v>101052002</v>
       </c>
-      <c r="G13" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H13" s="44" t="s">
+      <c r="G13" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="40" t="s">
+      <c r="A14" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="45">
         <v>101010206</v>
       </c>
-      <c r="D14" s="48">
+      <c r="D14" s="47">
         <v>101020201</v>
       </c>
-      <c r="E14" s="48" t="s">
+      <c r="E14" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="45">
+      <c r="F14" s="44">
         <v>101052002</v>
       </c>
-      <c r="G14" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H14" s="44" t="s">
+      <c r="G14" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="40" t="s">
+      <c r="A15" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="46">
+      <c r="C15" s="45">
         <v>101010207</v>
       </c>
-      <c r="D15" s="48">
+      <c r="D15" s="47">
         <v>101020201</v>
       </c>
-      <c r="E15" s="48" t="s">
+      <c r="E15" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="45">
+      <c r="F15" s="44">
         <v>101052002</v>
       </c>
-      <c r="G15" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H15" s="44" t="s">
+      <c r="G15" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="46">
+      <c r="C16" s="45">
         <v>101010209</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D16" s="47">
         <v>101020201</v>
       </c>
-      <c r="E16" s="48" t="s">
+      <c r="E16" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="45">
+      <c r="F16" s="44">
         <v>101052002</v>
       </c>
-      <c r="G16" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H16" s="44" t="s">
+      <c r="G16" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="40" t="s">
+      <c r="A17" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="46">
+      <c r="C17" s="45">
         <v>101010211</v>
       </c>
-      <c r="D17" s="48">
+      <c r="D17" s="47">
         <v>101020201</v>
       </c>
-      <c r="E17" s="48" t="s">
+      <c r="E17" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="45">
+      <c r="F17" s="44">
         <v>101052002</v>
       </c>
-      <c r="G17" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H17" s="44" t="s">
+      <c r="G17" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="46">
+      <c r="C18" s="45">
         <v>101010214</v>
       </c>
-      <c r="D18" s="48">
+      <c r="D18" s="47">
         <v>101020201</v>
       </c>
-      <c r="E18" s="48" t="s">
+      <c r="E18" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="45">
+      <c r="F18" s="44">
         <v>101052002</v>
       </c>
-      <c r="G18" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H18" s="44" t="s">
+      <c r="G18" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="46">
+      <c r="C19" s="45">
         <v>101010217</v>
       </c>
-      <c r="D19" s="48">
+      <c r="D19" s="47">
         <v>101020201</v>
       </c>
-      <c r="E19" s="48" t="s">
+      <c r="E19" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="45">
+      <c r="F19" s="44">
         <v>101052002</v>
       </c>
-      <c r="G19" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H19" s="44" t="s">
+      <c r="G19" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="46">
+      <c r="C20" s="45">
         <v>101010219</v>
       </c>
-      <c r="D20" s="48">
+      <c r="D20" s="47">
         <v>101020201</v>
       </c>
-      <c r="E20" s="48" t="s">
+      <c r="E20" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="45">
+      <c r="F20" s="44">
         <v>101052002</v>
       </c>
-      <c r="G20" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H20" s="44" t="s">
+      <c r="G20" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H20" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="30">
+      <c r="C21" s="29">
         <v>101010221</v>
       </c>
-      <c r="D21" s="50">
+      <c r="D21" s="49">
         <v>101020201</v>
       </c>
-      <c r="E21" s="50" t="s">
+      <c r="E21" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="45">
+      <c r="F21" s="44">
         <v>101052002</v>
       </c>
-      <c r="G21" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H21" s="44" t="s">
+      <c r="G21" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H21" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
+      <c r="A22" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1657,6 +1787,14 @@
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
   </mergeCells>
+  <conditionalFormatting sqref="G4:G21">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="SI">
+      <formula>NOT(ISERROR(SEARCH("SI",G4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",G4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G21" xr:uid="{36543B51-5247-4ED3-ACAE-69DC0A05FC31}">
       <formula1>"SI,NO"</formula1>
@@ -1674,8 +1812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,15 +1824,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="62" t="s">
+      <c r="B1" s="65"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="61"/>
+      <c r="E1" s="66"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -1720,634 +1858,705 @@
         <v>101010101</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="57" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="6">
         <v>101010103</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <v>101044012</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="63"/>
+      <c r="F4" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="14" t="s">
+      <c r="A5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="6">
         <v>101010104</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>101044012</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="63"/>
+      <c r="F5" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="6">
         <v>101010105</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>101044012</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="63"/>
+      <c r="F6" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="6">
         <v>101010133</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>101041012</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="63"/>
+      <c r="F7" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="17">
         <v>101010108</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="18">
         <v>101044032</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="63"/>
+      <c r="F8" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="14" t="s">
+      <c r="A9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="6">
         <v>101010132</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>101044032</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="63"/>
+      <c r="F9" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="6">
         <v>101010134</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <v>101041082</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="63"/>
+      <c r="F10" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="14" t="s">
+      <c r="A11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="6">
         <v>101010110</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>101041002</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="63"/>
+      <c r="F11" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="14" t="s">
+      <c r="A12" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="6">
         <v>101010112</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="14">
         <v>101044022</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="63"/>
+      <c r="F12" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="14" t="s">
+      <c r="A13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="6">
         <v>101010113</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <v>101044022</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="63"/>
+      <c r="F13" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="14" t="s">
+      <c r="A14" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="6">
         <v>101010115</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="14">
         <v>101044052</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="63"/>
+      <c r="F14" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="14" t="s">
+      <c r="A15" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="6">
         <v>101010116</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <v>101044052</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="63"/>
+      <c r="F15" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="14" t="s">
+      <c r="A16" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="6">
         <v>101010118</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="14">
         <v>101044062</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="63"/>
+      <c r="F16" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="14" t="s">
+      <c r="A17" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>40</v>
       </c>
       <c r="C17" s="6">
         <v>101010120</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="14">
         <v>101044042</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="63"/>
+      <c r="F17" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="14" t="s">
+      <c r="A18" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>43</v>
       </c>
       <c r="C18" s="6">
         <v>101010122</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="14">
         <v>101044082</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="63"/>
+      <c r="F18" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>46</v>
       </c>
       <c r="C19" s="6">
         <v>101010136</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="14">
         <v>101044102</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="63"/>
+      <c r="F19" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>48</v>
       </c>
       <c r="C20" s="6">
         <v>101010137</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="14">
         <v>101044092</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="63"/>
+      <c r="F20" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="21" t="s">
+      <c r="A21" s="19"/>
+      <c r="B21" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="21">
         <v>101010201</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="63"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="68"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="14" t="s">
+      <c r="A22" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="13" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="6">
         <v>101010203</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22" s="23">
         <v>101052002</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="63"/>
+      <c r="F22" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="14" t="s">
+      <c r="A23" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>55</v>
       </c>
       <c r="C23" s="6">
         <v>101010204</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23" s="23">
         <v>101052002</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="63"/>
+      <c r="F23" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="14" t="s">
+      <c r="A24" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>56</v>
       </c>
       <c r="C24" s="6">
         <v>101010205</v>
       </c>
-      <c r="D24" s="24">
+      <c r="D24" s="23">
         <v>101052002</v>
       </c>
-      <c r="E24" s="24" t="s">
+      <c r="E24" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="63"/>
+      <c r="F24" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="14" t="s">
+      <c r="A25" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="13" t="s">
         <v>58</v>
       </c>
       <c r="C25" s="6">
         <v>101010233</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="23">
         <v>101052002</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="63"/>
+      <c r="F25" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="17">
         <v>101010208</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="23">
         <v>101052002</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="E26" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F26" s="63"/>
+      <c r="F26" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="14" t="s">
+      <c r="A27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="13" t="s">
         <v>61</v>
       </c>
       <c r="C27" s="6">
         <v>101010232</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="23">
         <v>101052002</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="E27" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="63"/>
+      <c r="F27" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="14" t="s">
+      <c r="A28" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="13" t="s">
         <v>62</v>
       </c>
       <c r="C28" s="6">
         <v>101010234</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28" s="23">
         <v>101052002</v>
       </c>
-      <c r="E28" s="24" t="s">
+      <c r="E28" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F28" s="63"/>
+      <c r="F28" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="14" t="s">
+      <c r="A29" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="13" t="s">
         <v>64</v>
       </c>
       <c r="C29" s="6">
         <v>101010210</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="23">
         <v>101052002</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="E29" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F29" s="63"/>
+      <c r="F29" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="14" t="s">
+      <c r="A30" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="13" t="s">
         <v>66</v>
       </c>
       <c r="C30" s="6">
         <v>101010212</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="23">
         <v>101052002</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F30" s="63"/>
+      <c r="F30" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="14" t="s">
+      <c r="A31" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="13" t="s">
         <v>67</v>
       </c>
       <c r="C31" s="6">
         <v>101010213</v>
       </c>
-      <c r="D31" s="24">
+      <c r="D31" s="23">
         <v>101052002</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E31" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F31" s="63"/>
+      <c r="F31" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="14" t="s">
+      <c r="A32" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="13" t="s">
         <v>69</v>
       </c>
       <c r="C32" s="6">
         <v>101010215</v>
       </c>
-      <c r="D32" s="24">
+      <c r="D32" s="23">
         <v>101052002</v>
       </c>
-      <c r="E32" s="24" t="s">
+      <c r="E32" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F32" s="63"/>
+      <c r="F32" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="14" t="s">
+      <c r="A33" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="13" t="s">
         <v>70</v>
       </c>
       <c r="C33" s="6">
         <v>101010216</v>
       </c>
-      <c r="D33" s="24">
+      <c r="D33" s="23">
         <v>101052002</v>
       </c>
-      <c r="E33" s="24" t="s">
+      <c r="E33" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F33" s="63"/>
+      <c r="F33" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="14" t="s">
+      <c r="A34" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="13" t="s">
         <v>72</v>
       </c>
       <c r="C34" s="6">
         <v>101010218</v>
       </c>
-      <c r="D34" s="24">
+      <c r="D34" s="23">
         <v>101052002</v>
       </c>
-      <c r="E34" s="24" t="s">
+      <c r="E34" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F34" s="63"/>
+      <c r="F34" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="14" t="s">
+      <c r="A35" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="13" t="s">
         <v>74</v>
       </c>
       <c r="C35" s="6">
         <v>101010220</v>
       </c>
-      <c r="D35" s="24">
+      <c r="D35" s="23">
         <v>101052002</v>
       </c>
-      <c r="E35" s="24" t="s">
+      <c r="E35" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F35" s="63"/>
+      <c r="F35" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="14" t="s">
+      <c r="A36" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="13" t="s">
         <v>76</v>
       </c>
       <c r="C36" s="6">
         <v>101010222</v>
       </c>
-      <c r="D36" s="24">
+      <c r="D36" s="23">
         <v>101052002</v>
       </c>
-      <c r="E36" s="24" t="s">
+      <c r="E36" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F36" s="63"/>
+      <c r="F36" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="13" t="s">
         <v>77</v>
       </c>
       <c r="C37" s="6">
         <v>101010236</v>
       </c>
-      <c r="D37" s="24">
+      <c r="D37" s="23">
         <v>101052002</v>
       </c>
-      <c r="E37" s="24" t="s">
+      <c r="E37" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F37" s="63"/>
+      <c r="F37" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="13" t="s">
         <v>78</v>
       </c>
       <c r="C38" s="6">
         <v>101010237</v>
       </c>
-      <c r="D38" s="24">
+      <c r="D38" s="23">
         <v>101052002</v>
       </c>
-      <c r="E38" s="24" t="s">
+      <c r="E38" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F38" s="63"/>
+      <c r="F38" s="68" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="11" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2371,6 +2580,22 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:E1"/>
   </mergeCells>
+  <conditionalFormatting sqref="F4:F38">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",F4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="SI">
+      <formula>NOT(ISERROR(SEARCH("SI",F4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",F4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F20 F22:F38" xr:uid="{4DDA8D3B-06EF-40B5-B0B2-CBEB1310B5C8}">
+      <formula1>"SI,NO"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.38" bottom="0.27" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Bot5GUI -v1.00 - el siguiente paso es empezar las pruebas
</commit_message>
<xml_diff>
--- a/CUENTAS DE CAJA IVSA.xlsx
+++ b/CUENTAS DE CAJA IVSA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="8_{E7FEFFEB-5A09-49B6-9D87-359617FDBFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FF3F8E0-DE22-441A-B0DE-26E04F1B1DCF}"/>
+  <xr:revisionPtr revIDLastSave="126" documentId="8_{E7FEFFEB-5A09-49B6-9D87-359617FDBFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B5B7978-DF3D-4E6B-8905-1BC76B74D16B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DISTRIBUIDORAS" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="86">
   <si>
     <t>CAJAS RECAUDADORAS A NIVEL NACIONAL</t>
   </si>
@@ -275,13 +275,7 @@
     <t>CTA BANCARIA</t>
   </si>
   <si>
-    <t>DIRECTO</t>
-  </si>
-  <si>
     <t>SI</t>
-  </si>
-  <si>
-    <t>NO</t>
   </si>
   <si>
     <t>EJECUTAR</t>
@@ -350,16 +344,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="8" tint="-0.249977111117893"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -666,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -768,9 +762,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -809,6 +800,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -837,64 +831,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -935,6 +882,16 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -946,6 +903,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1237,7 +1198,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1245,21 +1206,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:BD22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" style="50" customWidth="1"/>
     <col min="2" max="2" width="47.42578125" style="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" style="30" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11.42578125" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
@@ -1270,7 +1231,7 @@
       </c>
       <c r="E1" s="61"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31"/>
       <c r="B2" s="31" t="s">
         <v>2</v>
@@ -1288,13 +1249,59 @@
         <v>83</v>
       </c>
       <c r="G2" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="H2" s="63" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="H2" s="68"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="69"/>
+      <c r="U2" s="69"/>
+      <c r="V2" s="69"/>
+      <c r="W2" s="69"/>
+      <c r="X2" s="69"/>
+      <c r="Y2" s="69"/>
+      <c r="Z2" s="69"/>
+      <c r="AA2" s="69"/>
+      <c r="AB2" s="69"/>
+      <c r="AC2" s="69"/>
+      <c r="AD2" s="69"/>
+      <c r="AE2" s="69"/>
+      <c r="AF2" s="69"/>
+      <c r="AG2" s="69"/>
+      <c r="AH2" s="69"/>
+      <c r="AI2" s="69"/>
+      <c r="AJ2" s="69"/>
+      <c r="AK2" s="69"/>
+      <c r="AL2" s="69"/>
+      <c r="AM2" s="69"/>
+      <c r="AN2" s="69"/>
+      <c r="AO2" s="69"/>
+      <c r="AP2" s="69"/>
+      <c r="AQ2" s="69"/>
+      <c r="AR2" s="69"/>
+      <c r="AS2" s="69"/>
+      <c r="AT2" s="69"/>
+      <c r="AU2" s="69"/>
+      <c r="AV2" s="69"/>
+      <c r="AW2" s="69"/>
+      <c r="AX2" s="69"/>
+      <c r="AY2" s="69"/>
+      <c r="AZ2" s="69"/>
+      <c r="BA2" s="69"/>
+      <c r="BB2" s="69"/>
+      <c r="BC2" s="69"/>
+      <c r="BD2" s="69"/>
+    </row>
+    <row r="3" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34"/>
       <c r="B3" s="35" t="s">
         <v>6</v>
@@ -1306,9 +1313,57 @@
       <c r="E3" s="38"/>
       <c r="F3" s="58"/>
       <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="68"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="69"/>
+      <c r="Q3" s="69"/>
+      <c r="R3" s="69"/>
+      <c r="S3" s="69"/>
+      <c r="T3" s="69"/>
+      <c r="U3" s="69"/>
+      <c r="V3" s="69"/>
+      <c r="W3" s="69"/>
+      <c r="X3" s="69"/>
+      <c r="Y3" s="69"/>
+      <c r="Z3" s="69"/>
+      <c r="AA3" s="69"/>
+      <c r="AB3" s="69"/>
+      <c r="AC3" s="69"/>
+      <c r="AD3" s="69"/>
+      <c r="AE3" s="69"/>
+      <c r="AF3" s="69"/>
+      <c r="AG3" s="69"/>
+      <c r="AH3" s="69"/>
+      <c r="AI3" s="69"/>
+      <c r="AJ3" s="69"/>
+      <c r="AK3" s="69"/>
+      <c r="AL3" s="69"/>
+      <c r="AM3" s="69"/>
+      <c r="AN3" s="69"/>
+      <c r="AO3" s="69"/>
+      <c r="AP3" s="69"/>
+      <c r="AQ3" s="69"/>
+      <c r="AR3" s="69"/>
+      <c r="AS3" s="69"/>
+      <c r="AT3" s="69"/>
+      <c r="AU3" s="69"/>
+      <c r="AV3" s="69"/>
+      <c r="AW3" s="69"/>
+      <c r="AX3" s="69"/>
+      <c r="AY3" s="69"/>
+      <c r="AZ3" s="69"/>
+      <c r="BA3" s="69"/>
+      <c r="BB3" s="69"/>
+      <c r="BC3" s="69"/>
+      <c r="BD3" s="69"/>
+    </row>
+    <row r="4" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>7</v>
       </c>
@@ -1328,13 +1383,59 @@
         <v>101044012</v>
       </c>
       <c r="G4" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="69"/>
+      <c r="N4" s="69"/>
+      <c r="O4" s="69"/>
+      <c r="P4" s="69"/>
+      <c r="Q4" s="69"/>
+      <c r="R4" s="69"/>
+      <c r="S4" s="69"/>
+      <c r="T4" s="69"/>
+      <c r="U4" s="69"/>
+      <c r="V4" s="69"/>
+      <c r="W4" s="69"/>
+      <c r="X4" s="69"/>
+      <c r="Y4" s="69"/>
+      <c r="Z4" s="69"/>
+      <c r="AA4" s="69"/>
+      <c r="AB4" s="69"/>
+      <c r="AC4" s="69"/>
+      <c r="AD4" s="69"/>
+      <c r="AE4" s="69"/>
+      <c r="AF4" s="69"/>
+      <c r="AG4" s="69"/>
+      <c r="AH4" s="69"/>
+      <c r="AI4" s="69"/>
+      <c r="AJ4" s="69"/>
+      <c r="AK4" s="69"/>
+      <c r="AL4" s="69"/>
+      <c r="AM4" s="69"/>
+      <c r="AN4" s="69"/>
+      <c r="AO4" s="69"/>
+      <c r="AP4" s="69"/>
+      <c r="AQ4" s="69"/>
+      <c r="AR4" s="69"/>
+      <c r="AS4" s="69"/>
+      <c r="AT4" s="69"/>
+      <c r="AU4" s="69"/>
+      <c r="AV4" s="69"/>
+      <c r="AW4" s="69"/>
+      <c r="AX4" s="69"/>
+      <c r="AY4" s="69"/>
+      <c r="AZ4" s="69"/>
+      <c r="BA4" s="69"/>
+      <c r="BB4" s="69"/>
+      <c r="BC4" s="69"/>
+      <c r="BD4" s="69"/>
+    </row>
+    <row r="5" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>7</v>
       </c>
@@ -1350,17 +1451,63 @@
       <c r="E5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="44">
+      <c r="F5" s="43">
         <v>101044012</v>
       </c>
       <c r="G5" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H5" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="69"/>
+      <c r="T5" s="69"/>
+      <c r="U5" s="69"/>
+      <c r="V5" s="69"/>
+      <c r="W5" s="69"/>
+      <c r="X5" s="69"/>
+      <c r="Y5" s="69"/>
+      <c r="Z5" s="69"/>
+      <c r="AA5" s="69"/>
+      <c r="AB5" s="69"/>
+      <c r="AC5" s="69"/>
+      <c r="AD5" s="69"/>
+      <c r="AE5" s="69"/>
+      <c r="AF5" s="69"/>
+      <c r="AG5" s="69"/>
+      <c r="AH5" s="69"/>
+      <c r="AI5" s="69"/>
+      <c r="AJ5" s="69"/>
+      <c r="AK5" s="69"/>
+      <c r="AL5" s="69"/>
+      <c r="AM5" s="69"/>
+      <c r="AN5" s="69"/>
+      <c r="AO5" s="69"/>
+      <c r="AP5" s="69"/>
+      <c r="AQ5" s="69"/>
+      <c r="AR5" s="69"/>
+      <c r="AS5" s="69"/>
+      <c r="AT5" s="69"/>
+      <c r="AU5" s="69"/>
+      <c r="AV5" s="69"/>
+      <c r="AW5" s="69"/>
+      <c r="AX5" s="69"/>
+      <c r="AY5" s="69"/>
+      <c r="AZ5" s="69"/>
+      <c r="BA5" s="69"/>
+      <c r="BB5" s="69"/>
+      <c r="BC5" s="69"/>
+      <c r="BD5" s="69"/>
+    </row>
+    <row r="6" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>7</v>
       </c>
@@ -1376,17 +1523,63 @@
       <c r="E6" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="44">
+      <c r="F6" s="43">
         <v>101044032</v>
       </c>
       <c r="G6" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H6" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
+      <c r="O6" s="69"/>
+      <c r="P6" s="69"/>
+      <c r="Q6" s="69"/>
+      <c r="R6" s="69"/>
+      <c r="S6" s="69"/>
+      <c r="T6" s="69"/>
+      <c r="U6" s="69"/>
+      <c r="V6" s="69"/>
+      <c r="W6" s="69"/>
+      <c r="X6" s="69"/>
+      <c r="Y6" s="69"/>
+      <c r="Z6" s="69"/>
+      <c r="AA6" s="69"/>
+      <c r="AB6" s="69"/>
+      <c r="AC6" s="69"/>
+      <c r="AD6" s="69"/>
+      <c r="AE6" s="69"/>
+      <c r="AF6" s="69"/>
+      <c r="AG6" s="69"/>
+      <c r="AH6" s="69"/>
+      <c r="AI6" s="69"/>
+      <c r="AJ6" s="69"/>
+      <c r="AK6" s="69"/>
+      <c r="AL6" s="69"/>
+      <c r="AM6" s="69"/>
+      <c r="AN6" s="69"/>
+      <c r="AO6" s="69"/>
+      <c r="AP6" s="69"/>
+      <c r="AQ6" s="69"/>
+      <c r="AR6" s="69"/>
+      <c r="AS6" s="69"/>
+      <c r="AT6" s="69"/>
+      <c r="AU6" s="69"/>
+      <c r="AV6" s="69"/>
+      <c r="AW6" s="69"/>
+      <c r="AX6" s="69"/>
+      <c r="AY6" s="69"/>
+      <c r="AZ6" s="69"/>
+      <c r="BA6" s="69"/>
+      <c r="BB6" s="69"/>
+      <c r="BC6" s="69"/>
+      <c r="BD6" s="69"/>
+    </row>
+    <row r="7" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>24</v>
       </c>
@@ -1402,17 +1595,63 @@
       <c r="E7" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="44">
+      <c r="F7" s="43">
         <v>101044072</v>
       </c>
       <c r="G7" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+      <c r="L7" s="69"/>
+      <c r="M7" s="69"/>
+      <c r="N7" s="69"/>
+      <c r="O7" s="69"/>
+      <c r="P7" s="69"/>
+      <c r="Q7" s="69"/>
+      <c r="R7" s="69"/>
+      <c r="S7" s="69"/>
+      <c r="T7" s="69"/>
+      <c r="U7" s="69"/>
+      <c r="V7" s="69"/>
+      <c r="W7" s="69"/>
+      <c r="X7" s="69"/>
+      <c r="Y7" s="69"/>
+      <c r="Z7" s="69"/>
+      <c r="AA7" s="69"/>
+      <c r="AB7" s="69"/>
+      <c r="AC7" s="69"/>
+      <c r="AD7" s="69"/>
+      <c r="AE7" s="69"/>
+      <c r="AF7" s="69"/>
+      <c r="AG7" s="69"/>
+      <c r="AH7" s="69"/>
+      <c r="AI7" s="69"/>
+      <c r="AJ7" s="69"/>
+      <c r="AK7" s="69"/>
+      <c r="AL7" s="69"/>
+      <c r="AM7" s="69"/>
+      <c r="AN7" s="69"/>
+      <c r="AO7" s="69"/>
+      <c r="AP7" s="69"/>
+      <c r="AQ7" s="69"/>
+      <c r="AR7" s="69"/>
+      <c r="AS7" s="69"/>
+      <c r="AT7" s="69"/>
+      <c r="AU7" s="69"/>
+      <c r="AV7" s="69"/>
+      <c r="AW7" s="69"/>
+      <c r="AX7" s="69"/>
+      <c r="AY7" s="69"/>
+      <c r="AZ7" s="69"/>
+      <c r="BA7" s="69"/>
+      <c r="BB7" s="69"/>
+      <c r="BC7" s="69"/>
+      <c r="BD7" s="69"/>
+    </row>
+    <row r="8" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>7</v>
       </c>
@@ -1428,17 +1667,63 @@
       <c r="E8" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="44">
+      <c r="F8" s="43">
         <v>101044022</v>
       </c>
       <c r="G8" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H8" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="69"/>
+      <c r="N8" s="69"/>
+      <c r="O8" s="69"/>
+      <c r="P8" s="69"/>
+      <c r="Q8" s="69"/>
+      <c r="R8" s="69"/>
+      <c r="S8" s="69"/>
+      <c r="T8" s="69"/>
+      <c r="U8" s="69"/>
+      <c r="V8" s="69"/>
+      <c r="W8" s="69"/>
+      <c r="X8" s="69"/>
+      <c r="Y8" s="69"/>
+      <c r="Z8" s="69"/>
+      <c r="AA8" s="69"/>
+      <c r="AB8" s="69"/>
+      <c r="AC8" s="69"/>
+      <c r="AD8" s="69"/>
+      <c r="AE8" s="69"/>
+      <c r="AF8" s="69"/>
+      <c r="AG8" s="69"/>
+      <c r="AH8" s="69"/>
+      <c r="AI8" s="69"/>
+      <c r="AJ8" s="69"/>
+      <c r="AK8" s="69"/>
+      <c r="AL8" s="69"/>
+      <c r="AM8" s="69"/>
+      <c r="AN8" s="69"/>
+      <c r="AO8" s="69"/>
+      <c r="AP8" s="69"/>
+      <c r="AQ8" s="69"/>
+      <c r="AR8" s="69"/>
+      <c r="AS8" s="69"/>
+      <c r="AT8" s="69"/>
+      <c r="AU8" s="69"/>
+      <c r="AV8" s="69"/>
+      <c r="AW8" s="69"/>
+      <c r="AX8" s="69"/>
+      <c r="AY8" s="69"/>
+      <c r="AZ8" s="69"/>
+      <c r="BA8" s="69"/>
+      <c r="BB8" s="69"/>
+      <c r="BC8" s="69"/>
+      <c r="BD8" s="69"/>
+    </row>
+    <row r="9" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
         <v>24</v>
       </c>
@@ -1454,17 +1739,63 @@
       <c r="E9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="44">
+      <c r="F9" s="43">
         <v>101044052</v>
       </c>
       <c r="G9" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H9" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="69"/>
+      <c r="N9" s="69"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="69"/>
+      <c r="Q9" s="69"/>
+      <c r="R9" s="69"/>
+      <c r="S9" s="69"/>
+      <c r="T9" s="69"/>
+      <c r="U9" s="69"/>
+      <c r="V9" s="69"/>
+      <c r="W9" s="69"/>
+      <c r="X9" s="69"/>
+      <c r="Y9" s="69"/>
+      <c r="Z9" s="69"/>
+      <c r="AA9" s="69"/>
+      <c r="AB9" s="69"/>
+      <c r="AC9" s="69"/>
+      <c r="AD9" s="69"/>
+      <c r="AE9" s="69"/>
+      <c r="AF9" s="69"/>
+      <c r="AG9" s="69"/>
+      <c r="AH9" s="69"/>
+      <c r="AI9" s="69"/>
+      <c r="AJ9" s="69"/>
+      <c r="AK9" s="69"/>
+      <c r="AL9" s="69"/>
+      <c r="AM9" s="69"/>
+      <c r="AN9" s="69"/>
+      <c r="AO9" s="69"/>
+      <c r="AP9" s="69"/>
+      <c r="AQ9" s="69"/>
+      <c r="AR9" s="69"/>
+      <c r="AS9" s="69"/>
+      <c r="AT9" s="69"/>
+      <c r="AU9" s="69"/>
+      <c r="AV9" s="69"/>
+      <c r="AW9" s="69"/>
+      <c r="AX9" s="69"/>
+      <c r="AY9" s="69"/>
+      <c r="AZ9" s="69"/>
+      <c r="BA9" s="69"/>
+      <c r="BB9" s="69"/>
+      <c r="BC9" s="69"/>
+      <c r="BD9" s="69"/>
+    </row>
+    <row r="10" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
         <v>24</v>
       </c>
@@ -1480,17 +1811,63 @@
       <c r="E10" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="44">
+      <c r="F10" s="43">
         <v>101044062</v>
       </c>
       <c r="G10" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H10" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="69"/>
+      <c r="M10" s="69"/>
+      <c r="N10" s="69"/>
+      <c r="O10" s="69"/>
+      <c r="P10" s="69"/>
+      <c r="Q10" s="69"/>
+      <c r="R10" s="69"/>
+      <c r="S10" s="69"/>
+      <c r="T10" s="69"/>
+      <c r="U10" s="69"/>
+      <c r="V10" s="69"/>
+      <c r="W10" s="69"/>
+      <c r="X10" s="69"/>
+      <c r="Y10" s="69"/>
+      <c r="Z10" s="69"/>
+      <c r="AA10" s="69"/>
+      <c r="AB10" s="69"/>
+      <c r="AC10" s="69"/>
+      <c r="AD10" s="69"/>
+      <c r="AE10" s="69"/>
+      <c r="AF10" s="69"/>
+      <c r="AG10" s="69"/>
+      <c r="AH10" s="69"/>
+      <c r="AI10" s="69"/>
+      <c r="AJ10" s="69"/>
+      <c r="AK10" s="69"/>
+      <c r="AL10" s="69"/>
+      <c r="AM10" s="69"/>
+      <c r="AN10" s="69"/>
+      <c r="AO10" s="69"/>
+      <c r="AP10" s="69"/>
+      <c r="AQ10" s="69"/>
+      <c r="AR10" s="69"/>
+      <c r="AS10" s="69"/>
+      <c r="AT10" s="69"/>
+      <c r="AU10" s="69"/>
+      <c r="AV10" s="69"/>
+      <c r="AW10" s="69"/>
+      <c r="AX10" s="69"/>
+      <c r="AY10" s="69"/>
+      <c r="AZ10" s="69"/>
+      <c r="BA10" s="69"/>
+      <c r="BB10" s="69"/>
+      <c r="BC10" s="69"/>
+      <c r="BD10" s="69"/>
+    </row>
+    <row r="11" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>24</v>
       </c>
@@ -1506,17 +1883,63 @@
       <c r="E11" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="44">
+      <c r="F11" s="43">
         <v>101044042</v>
       </c>
       <c r="G11" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H11" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="69"/>
+      <c r="L11" s="69"/>
+      <c r="M11" s="69"/>
+      <c r="N11" s="69"/>
+      <c r="O11" s="69"/>
+      <c r="P11" s="69"/>
+      <c r="Q11" s="69"/>
+      <c r="R11" s="69"/>
+      <c r="S11" s="69"/>
+      <c r="T11" s="69"/>
+      <c r="U11" s="69"/>
+      <c r="V11" s="69"/>
+      <c r="W11" s="69"/>
+      <c r="X11" s="69"/>
+      <c r="Y11" s="69"/>
+      <c r="Z11" s="69"/>
+      <c r="AA11" s="69"/>
+      <c r="AB11" s="69"/>
+      <c r="AC11" s="69"/>
+      <c r="AD11" s="69"/>
+      <c r="AE11" s="69"/>
+      <c r="AF11" s="69"/>
+      <c r="AG11" s="69"/>
+      <c r="AH11" s="69"/>
+      <c r="AI11" s="69"/>
+      <c r="AJ11" s="69"/>
+      <c r="AK11" s="69"/>
+      <c r="AL11" s="69"/>
+      <c r="AM11" s="69"/>
+      <c r="AN11" s="69"/>
+      <c r="AO11" s="69"/>
+      <c r="AP11" s="69"/>
+      <c r="AQ11" s="69"/>
+      <c r="AR11" s="69"/>
+      <c r="AS11" s="69"/>
+      <c r="AT11" s="69"/>
+      <c r="AU11" s="69"/>
+      <c r="AV11" s="69"/>
+      <c r="AW11" s="69"/>
+      <c r="AX11" s="69"/>
+      <c r="AY11" s="69"/>
+      <c r="AZ11" s="69"/>
+      <c r="BA11" s="69"/>
+      <c r="BB11" s="69"/>
+      <c r="BC11" s="69"/>
+      <c r="BD11" s="69"/>
+    </row>
+    <row r="12" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
         <v>24</v>
       </c>
@@ -1532,252 +1955,712 @@
       <c r="E12" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="44">
+      <c r="F12" s="43">
         <v>101044082</v>
       </c>
       <c r="G12" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H12" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="69"/>
+      <c r="L12" s="69"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="69"/>
+      <c r="O12" s="69"/>
+      <c r="P12" s="69"/>
+      <c r="Q12" s="69"/>
+      <c r="R12" s="69"/>
+      <c r="S12" s="69"/>
+      <c r="T12" s="69"/>
+      <c r="U12" s="69"/>
+      <c r="V12" s="69"/>
+      <c r="W12" s="69"/>
+      <c r="X12" s="69"/>
+      <c r="Y12" s="69"/>
+      <c r="Z12" s="69"/>
+      <c r="AA12" s="69"/>
+      <c r="AB12" s="69"/>
+      <c r="AC12" s="69"/>
+      <c r="AD12" s="69"/>
+      <c r="AE12" s="69"/>
+      <c r="AF12" s="69"/>
+      <c r="AG12" s="69"/>
+      <c r="AH12" s="69"/>
+      <c r="AI12" s="69"/>
+      <c r="AJ12" s="69"/>
+      <c r="AK12" s="69"/>
+      <c r="AL12" s="69"/>
+      <c r="AM12" s="69"/>
+      <c r="AN12" s="69"/>
+      <c r="AO12" s="69"/>
+      <c r="AP12" s="69"/>
+      <c r="AQ12" s="69"/>
+      <c r="AR12" s="69"/>
+      <c r="AS12" s="69"/>
+      <c r="AT12" s="69"/>
+      <c r="AU12" s="69"/>
+      <c r="AV12" s="69"/>
+      <c r="AW12" s="69"/>
+      <c r="AX12" s="69"/>
+      <c r="AY12" s="69"/>
+      <c r="AZ12" s="69"/>
+      <c r="BA12" s="69"/>
+      <c r="BB12" s="69"/>
+      <c r="BC12" s="69"/>
+      <c r="BD12" s="69"/>
+    </row>
+    <row r="13" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="45">
+      <c r="C13" s="44">
         <v>101010202</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="45">
         <v>101020201</v>
       </c>
-      <c r="E13" s="46" t="s">
+      <c r="E13" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="44">
+      <c r="F13" s="43">
         <v>101052002</v>
       </c>
       <c r="G13" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H13" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
+      <c r="K13" s="69"/>
+      <c r="L13" s="69"/>
+      <c r="M13" s="69"/>
+      <c r="N13" s="69"/>
+      <c r="O13" s="69"/>
+      <c r="P13" s="69"/>
+      <c r="Q13" s="69"/>
+      <c r="R13" s="69"/>
+      <c r="S13" s="69"/>
+      <c r="T13" s="69"/>
+      <c r="U13" s="69"/>
+      <c r="V13" s="69"/>
+      <c r="W13" s="69"/>
+      <c r="X13" s="69"/>
+      <c r="Y13" s="69"/>
+      <c r="Z13" s="69"/>
+      <c r="AA13" s="69"/>
+      <c r="AB13" s="69"/>
+      <c r="AC13" s="69"/>
+      <c r="AD13" s="69"/>
+      <c r="AE13" s="69"/>
+      <c r="AF13" s="69"/>
+      <c r="AG13" s="69"/>
+      <c r="AH13" s="69"/>
+      <c r="AI13" s="69"/>
+      <c r="AJ13" s="69"/>
+      <c r="AK13" s="69"/>
+      <c r="AL13" s="69"/>
+      <c r="AM13" s="69"/>
+      <c r="AN13" s="69"/>
+      <c r="AO13" s="69"/>
+      <c r="AP13" s="69"/>
+      <c r="AQ13" s="69"/>
+      <c r="AR13" s="69"/>
+      <c r="AS13" s="69"/>
+      <c r="AT13" s="69"/>
+      <c r="AU13" s="69"/>
+      <c r="AV13" s="69"/>
+      <c r="AW13" s="69"/>
+      <c r="AX13" s="69"/>
+      <c r="AY13" s="69"/>
+      <c r="AZ13" s="69"/>
+      <c r="BA13" s="69"/>
+      <c r="BB13" s="69"/>
+      <c r="BC13" s="69"/>
+      <c r="BD13" s="69"/>
+    </row>
+    <row r="14" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="45">
+      <c r="C14" s="44">
         <v>101010206</v>
       </c>
-      <c r="D14" s="47">
+      <c r="D14" s="46">
         <v>101020201</v>
       </c>
-      <c r="E14" s="47" t="s">
+      <c r="E14" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="44">
+      <c r="F14" s="43">
         <v>101052002</v>
       </c>
       <c r="G14" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H14" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="69"/>
+      <c r="K14" s="69"/>
+      <c r="L14" s="69"/>
+      <c r="M14" s="69"/>
+      <c r="N14" s="69"/>
+      <c r="O14" s="69"/>
+      <c r="P14" s="69"/>
+      <c r="Q14" s="69"/>
+      <c r="R14" s="69"/>
+      <c r="S14" s="69"/>
+      <c r="T14" s="69"/>
+      <c r="U14" s="69"/>
+      <c r="V14" s="69"/>
+      <c r="W14" s="69"/>
+      <c r="X14" s="69"/>
+      <c r="Y14" s="69"/>
+      <c r="Z14" s="69"/>
+      <c r="AA14" s="69"/>
+      <c r="AB14" s="69"/>
+      <c r="AC14" s="69"/>
+      <c r="AD14" s="69"/>
+      <c r="AE14" s="69"/>
+      <c r="AF14" s="69"/>
+      <c r="AG14" s="69"/>
+      <c r="AH14" s="69"/>
+      <c r="AI14" s="69"/>
+      <c r="AJ14" s="69"/>
+      <c r="AK14" s="69"/>
+      <c r="AL14" s="69"/>
+      <c r="AM14" s="69"/>
+      <c r="AN14" s="69"/>
+      <c r="AO14" s="69"/>
+      <c r="AP14" s="69"/>
+      <c r="AQ14" s="69"/>
+      <c r="AR14" s="69"/>
+      <c r="AS14" s="69"/>
+      <c r="AT14" s="69"/>
+      <c r="AU14" s="69"/>
+      <c r="AV14" s="69"/>
+      <c r="AW14" s="69"/>
+      <c r="AX14" s="69"/>
+      <c r="AY14" s="69"/>
+      <c r="AZ14" s="69"/>
+      <c r="BA14" s="69"/>
+      <c r="BB14" s="69"/>
+      <c r="BC14" s="69"/>
+      <c r="BD14" s="69"/>
+    </row>
+    <row r="15" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="45">
+      <c r="C15" s="44">
         <v>101010207</v>
       </c>
-      <c r="D15" s="47">
+      <c r="D15" s="46">
         <v>101020201</v>
       </c>
-      <c r="E15" s="47" t="s">
+      <c r="E15" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="44">
+      <c r="F15" s="43">
         <v>101052002</v>
       </c>
       <c r="G15" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H15" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="69"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="69"/>
+      <c r="Q15" s="69"/>
+      <c r="R15" s="69"/>
+      <c r="S15" s="69"/>
+      <c r="T15" s="69"/>
+      <c r="U15" s="69"/>
+      <c r="V15" s="69"/>
+      <c r="W15" s="69"/>
+      <c r="X15" s="69"/>
+      <c r="Y15" s="69"/>
+      <c r="Z15" s="69"/>
+      <c r="AA15" s="69"/>
+      <c r="AB15" s="69"/>
+      <c r="AC15" s="69"/>
+      <c r="AD15" s="69"/>
+      <c r="AE15" s="69"/>
+      <c r="AF15" s="69"/>
+      <c r="AG15" s="69"/>
+      <c r="AH15" s="69"/>
+      <c r="AI15" s="69"/>
+      <c r="AJ15" s="69"/>
+      <c r="AK15" s="69"/>
+      <c r="AL15" s="69"/>
+      <c r="AM15" s="69"/>
+      <c r="AN15" s="69"/>
+      <c r="AO15" s="69"/>
+      <c r="AP15" s="69"/>
+      <c r="AQ15" s="69"/>
+      <c r="AR15" s="69"/>
+      <c r="AS15" s="69"/>
+      <c r="AT15" s="69"/>
+      <c r="AU15" s="69"/>
+      <c r="AV15" s="69"/>
+      <c r="AW15" s="69"/>
+      <c r="AX15" s="69"/>
+      <c r="AY15" s="69"/>
+      <c r="AZ15" s="69"/>
+      <c r="BA15" s="69"/>
+      <c r="BB15" s="69"/>
+      <c r="BC15" s="69"/>
+      <c r="BD15" s="69"/>
+    </row>
+    <row r="16" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="45">
+      <c r="C16" s="44">
         <v>101010209</v>
       </c>
-      <c r="D16" s="47">
+      <c r="D16" s="46">
         <v>101020201</v>
       </c>
-      <c r="E16" s="47" t="s">
+      <c r="E16" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="44">
+      <c r="F16" s="43">
         <v>101052002</v>
       </c>
       <c r="G16" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H16" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="H16" s="69"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="69"/>
+      <c r="L16" s="69"/>
+      <c r="M16" s="69"/>
+      <c r="N16" s="69"/>
+      <c r="O16" s="69"/>
+      <c r="P16" s="69"/>
+      <c r="Q16" s="69"/>
+      <c r="R16" s="69"/>
+      <c r="S16" s="69"/>
+      <c r="T16" s="69"/>
+      <c r="U16" s="69"/>
+      <c r="V16" s="69"/>
+      <c r="W16" s="69"/>
+      <c r="X16" s="69"/>
+      <c r="Y16" s="69"/>
+      <c r="Z16" s="69"/>
+      <c r="AA16" s="69"/>
+      <c r="AB16" s="69"/>
+      <c r="AC16" s="69"/>
+      <c r="AD16" s="69"/>
+      <c r="AE16" s="69"/>
+      <c r="AF16" s="69"/>
+      <c r="AG16" s="69"/>
+      <c r="AH16" s="69"/>
+      <c r="AI16" s="69"/>
+      <c r="AJ16" s="69"/>
+      <c r="AK16" s="69"/>
+      <c r="AL16" s="69"/>
+      <c r="AM16" s="69"/>
+      <c r="AN16" s="69"/>
+      <c r="AO16" s="69"/>
+      <c r="AP16" s="69"/>
+      <c r="AQ16" s="69"/>
+      <c r="AR16" s="69"/>
+      <c r="AS16" s="69"/>
+      <c r="AT16" s="69"/>
+      <c r="AU16" s="69"/>
+      <c r="AV16" s="69"/>
+      <c r="AW16" s="69"/>
+      <c r="AX16" s="69"/>
+      <c r="AY16" s="69"/>
+      <c r="AZ16" s="69"/>
+      <c r="BA16" s="69"/>
+      <c r="BB16" s="69"/>
+      <c r="BC16" s="69"/>
+      <c r="BD16" s="69"/>
+    </row>
+    <row r="17" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="45">
+      <c r="C17" s="44">
         <v>101010211</v>
       </c>
-      <c r="D17" s="47">
+      <c r="D17" s="46">
         <v>101020201</v>
       </c>
-      <c r="E17" s="47" t="s">
+      <c r="E17" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="44">
+      <c r="F17" s="43">
         <v>101052002</v>
       </c>
       <c r="G17" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H17" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="H17" s="69"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="69"/>
+      <c r="K17" s="69"/>
+      <c r="L17" s="69"/>
+      <c r="M17" s="69"/>
+      <c r="N17" s="69"/>
+      <c r="O17" s="69"/>
+      <c r="P17" s="69"/>
+      <c r="Q17" s="69"/>
+      <c r="R17" s="69"/>
+      <c r="S17" s="69"/>
+      <c r="T17" s="69"/>
+      <c r="U17" s="69"/>
+      <c r="V17" s="69"/>
+      <c r="W17" s="69"/>
+      <c r="X17" s="69"/>
+      <c r="Y17" s="69"/>
+      <c r="Z17" s="69"/>
+      <c r="AA17" s="69"/>
+      <c r="AB17" s="69"/>
+      <c r="AC17" s="69"/>
+      <c r="AD17" s="69"/>
+      <c r="AE17" s="69"/>
+      <c r="AF17" s="69"/>
+      <c r="AG17" s="69"/>
+      <c r="AH17" s="69"/>
+      <c r="AI17" s="69"/>
+      <c r="AJ17" s="69"/>
+      <c r="AK17" s="69"/>
+      <c r="AL17" s="69"/>
+      <c r="AM17" s="69"/>
+      <c r="AN17" s="69"/>
+      <c r="AO17" s="69"/>
+      <c r="AP17" s="69"/>
+      <c r="AQ17" s="69"/>
+      <c r="AR17" s="69"/>
+      <c r="AS17" s="69"/>
+      <c r="AT17" s="69"/>
+      <c r="AU17" s="69"/>
+      <c r="AV17" s="69"/>
+      <c r="AW17" s="69"/>
+      <c r="AX17" s="69"/>
+      <c r="AY17" s="69"/>
+      <c r="AZ17" s="69"/>
+      <c r="BA17" s="69"/>
+      <c r="BB17" s="69"/>
+      <c r="BC17" s="69"/>
+      <c r="BD17" s="69"/>
+    </row>
+    <row r="18" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="45">
+      <c r="C18" s="44">
         <v>101010214</v>
       </c>
-      <c r="D18" s="47">
+      <c r="D18" s="46">
         <v>101020201</v>
       </c>
-      <c r="E18" s="47" t="s">
+      <c r="E18" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="44">
+      <c r="F18" s="43">
         <v>101052002</v>
       </c>
       <c r="G18" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H18" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
+      <c r="K18" s="69"/>
+      <c r="L18" s="69"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="69"/>
+      <c r="O18" s="69"/>
+      <c r="P18" s="69"/>
+      <c r="Q18" s="69"/>
+      <c r="R18" s="69"/>
+      <c r="S18" s="69"/>
+      <c r="T18" s="69"/>
+      <c r="U18" s="69"/>
+      <c r="V18" s="69"/>
+      <c r="W18" s="69"/>
+      <c r="X18" s="69"/>
+      <c r="Y18" s="69"/>
+      <c r="Z18" s="69"/>
+      <c r="AA18" s="69"/>
+      <c r="AB18" s="69"/>
+      <c r="AC18" s="69"/>
+      <c r="AD18" s="69"/>
+      <c r="AE18" s="69"/>
+      <c r="AF18" s="69"/>
+      <c r="AG18" s="69"/>
+      <c r="AH18" s="69"/>
+      <c r="AI18" s="69"/>
+      <c r="AJ18" s="69"/>
+      <c r="AK18" s="69"/>
+      <c r="AL18" s="69"/>
+      <c r="AM18" s="69"/>
+      <c r="AN18" s="69"/>
+      <c r="AO18" s="69"/>
+      <c r="AP18" s="69"/>
+      <c r="AQ18" s="69"/>
+      <c r="AR18" s="69"/>
+      <c r="AS18" s="69"/>
+      <c r="AT18" s="69"/>
+      <c r="AU18" s="69"/>
+      <c r="AV18" s="69"/>
+      <c r="AW18" s="69"/>
+      <c r="AX18" s="69"/>
+      <c r="AY18" s="69"/>
+      <c r="AZ18" s="69"/>
+      <c r="BA18" s="69"/>
+      <c r="BB18" s="69"/>
+      <c r="BC18" s="69"/>
+      <c r="BD18" s="69"/>
+    </row>
+    <row r="19" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="45">
+      <c r="C19" s="44">
         <v>101010217</v>
       </c>
-      <c r="D19" s="47">
+      <c r="D19" s="46">
         <v>101020201</v>
       </c>
-      <c r="E19" s="47" t="s">
+      <c r="E19" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="44">
+      <c r="F19" s="43">
         <v>101052002</v>
       </c>
       <c r="G19" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H19" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="69"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="69"/>
+      <c r="O19" s="69"/>
+      <c r="P19" s="69"/>
+      <c r="Q19" s="69"/>
+      <c r="R19" s="69"/>
+      <c r="S19" s="69"/>
+      <c r="T19" s="69"/>
+      <c r="U19" s="69"/>
+      <c r="V19" s="69"/>
+      <c r="W19" s="69"/>
+      <c r="X19" s="69"/>
+      <c r="Y19" s="69"/>
+      <c r="Z19" s="69"/>
+      <c r="AA19" s="69"/>
+      <c r="AB19" s="69"/>
+      <c r="AC19" s="69"/>
+      <c r="AD19" s="69"/>
+      <c r="AE19" s="69"/>
+      <c r="AF19" s="69"/>
+      <c r="AG19" s="69"/>
+      <c r="AH19" s="69"/>
+      <c r="AI19" s="69"/>
+      <c r="AJ19" s="69"/>
+      <c r="AK19" s="69"/>
+      <c r="AL19" s="69"/>
+      <c r="AM19" s="69"/>
+      <c r="AN19" s="69"/>
+      <c r="AO19" s="69"/>
+      <c r="AP19" s="69"/>
+      <c r="AQ19" s="69"/>
+      <c r="AR19" s="69"/>
+      <c r="AS19" s="69"/>
+      <c r="AT19" s="69"/>
+      <c r="AU19" s="69"/>
+      <c r="AV19" s="69"/>
+      <c r="AW19" s="69"/>
+      <c r="AX19" s="69"/>
+      <c r="AY19" s="69"/>
+      <c r="AZ19" s="69"/>
+      <c r="BA19" s="69"/>
+      <c r="BB19" s="69"/>
+      <c r="BC19" s="69"/>
+      <c r="BD19" s="69"/>
+    </row>
+    <row r="20" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="45">
+      <c r="C20" s="44">
         <v>101010219</v>
       </c>
-      <c r="D20" s="47">
+      <c r="D20" s="46">
         <v>101020201</v>
       </c>
-      <c r="E20" s="47" t="s">
+      <c r="E20" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="44">
+      <c r="F20" s="43">
         <v>101052002</v>
       </c>
       <c r="G20" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H20" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="H20" s="69"/>
+      <c r="I20" s="69"/>
+      <c r="J20" s="69"/>
+      <c r="K20" s="69"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="69"/>
+      <c r="N20" s="69"/>
+      <c r="O20" s="69"/>
+      <c r="P20" s="69"/>
+      <c r="Q20" s="69"/>
+      <c r="R20" s="69"/>
+      <c r="S20" s="69"/>
+      <c r="T20" s="69"/>
+      <c r="U20" s="69"/>
+      <c r="V20" s="69"/>
+      <c r="W20" s="69"/>
+      <c r="X20" s="69"/>
+      <c r="Y20" s="69"/>
+      <c r="Z20" s="69"/>
+      <c r="AA20" s="69"/>
+      <c r="AB20" s="69"/>
+      <c r="AC20" s="69"/>
+      <c r="AD20" s="69"/>
+      <c r="AE20" s="69"/>
+      <c r="AF20" s="69"/>
+      <c r="AG20" s="69"/>
+      <c r="AH20" s="69"/>
+      <c r="AI20" s="69"/>
+      <c r="AJ20" s="69"/>
+      <c r="AK20" s="69"/>
+      <c r="AL20" s="69"/>
+      <c r="AM20" s="69"/>
+      <c r="AN20" s="69"/>
+      <c r="AO20" s="69"/>
+      <c r="AP20" s="69"/>
+      <c r="AQ20" s="69"/>
+      <c r="AR20" s="69"/>
+      <c r="AS20" s="69"/>
+      <c r="AT20" s="69"/>
+      <c r="AU20" s="69"/>
+      <c r="AV20" s="69"/>
+      <c r="AW20" s="69"/>
+      <c r="AX20" s="69"/>
+      <c r="AY20" s="69"/>
+      <c r="AZ20" s="69"/>
+      <c r="BA20" s="69"/>
+      <c r="BB20" s="69"/>
+      <c r="BC20" s="69"/>
+      <c r="BD20" s="69"/>
+    </row>
+    <row r="21" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="48" t="s">
+      <c r="B21" s="47" t="s">
         <v>75</v>
       </c>
       <c r="C21" s="29">
         <v>101010221</v>
       </c>
-      <c r="D21" s="49">
+      <c r="D21" s="48">
         <v>101020201</v>
       </c>
-      <c r="E21" s="49" t="s">
+      <c r="E21" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="44">
+      <c r="F21" s="43">
         <v>101052002</v>
       </c>
       <c r="G21" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H21" s="43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
+        <v>84</v>
+      </c>
+      <c r="H21" s="69"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="69"/>
+      <c r="K21" s="69"/>
+      <c r="L21" s="69"/>
+      <c r="M21" s="69"/>
+      <c r="N21" s="69"/>
+      <c r="O21" s="69"/>
+      <c r="P21" s="69"/>
+      <c r="Q21" s="69"/>
+      <c r="R21" s="69"/>
+      <c r="S21" s="69"/>
+      <c r="T21" s="69"/>
+      <c r="U21" s="69"/>
+      <c r="V21" s="69"/>
+      <c r="W21" s="69"/>
+      <c r="X21" s="69"/>
+      <c r="Y21" s="69"/>
+      <c r="Z21" s="69"/>
+      <c r="AA21" s="69"/>
+      <c r="AB21" s="69"/>
+      <c r="AC21" s="69"/>
+      <c r="AD21" s="69"/>
+      <c r="AE21" s="69"/>
+      <c r="AF21" s="69"/>
+      <c r="AG21" s="69"/>
+      <c r="AH21" s="69"/>
+      <c r="AI21" s="69"/>
+      <c r="AJ21" s="69"/>
+      <c r="AK21" s="69"/>
+      <c r="AL21" s="69"/>
+      <c r="AM21" s="69"/>
+      <c r="AN21" s="69"/>
+      <c r="AO21" s="69"/>
+      <c r="AP21" s="69"/>
+      <c r="AQ21" s="69"/>
+      <c r="AR21" s="69"/>
+      <c r="AS21" s="69"/>
+      <c r="AT21" s="69"/>
+      <c r="AU21" s="69"/>
+      <c r="AV21" s="69"/>
+      <c r="AW21" s="69"/>
+      <c r="AX21" s="69"/>
+      <c r="AY21" s="69"/>
+      <c r="AZ21" s="69"/>
+      <c r="BA21" s="69"/>
+      <c r="BB21" s="69"/>
+      <c r="BC21" s="69"/>
+      <c r="BD21" s="69"/>
+    </row>
+    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A22" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1788,19 +2671,16 @@
     <mergeCell ref="H2:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="G4:G21">
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="SI">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",G4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G21" xr:uid="{36543B51-5247-4ED3-ACAE-69DC0A05FC31}">
       <formula1>"SI,NO"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H21" xr:uid="{1981D13B-ED02-4002-B54B-38B3FEA0F9DE}">
-      <formula1>"NO,SI"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.38" bottom="0.27" header="0.3" footer="0.3"/>
@@ -1813,7 +2693,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1858,9 +2738,9 @@
         <v>101010101</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="57" t="s">
-        <v>87</v>
+      <c r="E3" s="51"/>
+      <c r="F3" s="56" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1876,11 +2756,11 @@
       <c r="D4" s="14">
         <v>101044012</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="68" t="s">
-        <v>85</v>
+      <c r="F4" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1896,11 +2776,11 @@
       <c r="D5" s="14">
         <v>101044012</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="68" t="s">
-        <v>85</v>
+      <c r="F5" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1916,11 +2796,11 @@
       <c r="D6" s="14">
         <v>101044012</v>
       </c>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="68" t="s">
-        <v>85</v>
+      <c r="F6" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1936,11 +2816,11 @@
       <c r="D7" s="14">
         <v>101041012</v>
       </c>
-      <c r="E7" s="53" t="s">
+      <c r="E7" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="68" t="s">
-        <v>85</v>
+      <c r="F7" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1956,11 +2836,11 @@
       <c r="D8" s="18">
         <v>101044032</v>
       </c>
-      <c r="E8" s="54" t="s">
+      <c r="E8" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="68" t="s">
-        <v>85</v>
+      <c r="F8" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1976,11 +2856,11 @@
       <c r="D9" s="14">
         <v>101044032</v>
       </c>
-      <c r="E9" s="53" t="s">
+      <c r="E9" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="68" t="s">
-        <v>85</v>
+      <c r="F9" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1996,11 +2876,11 @@
       <c r="D10" s="14">
         <v>101041082</v>
       </c>
-      <c r="E10" s="53" t="s">
+      <c r="E10" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="68" t="s">
-        <v>85</v>
+      <c r="F10" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2016,11 +2896,11 @@
       <c r="D11" s="14">
         <v>101041002</v>
       </c>
-      <c r="E11" s="53" t="s">
+      <c r="E11" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="68" t="s">
-        <v>85</v>
+      <c r="F11" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2036,11 +2916,11 @@
       <c r="D12" s="14">
         <v>101044022</v>
       </c>
-      <c r="E12" s="53" t="s">
+      <c r="E12" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="68" t="s">
-        <v>85</v>
+      <c r="F12" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2056,11 +2936,11 @@
       <c r="D13" s="14">
         <v>101044022</v>
       </c>
-      <c r="E13" s="53" t="s">
+      <c r="E13" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="68" t="s">
-        <v>85</v>
+      <c r="F13" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2076,11 +2956,11 @@
       <c r="D14" s="14">
         <v>101044052</v>
       </c>
-      <c r="E14" s="53" t="s">
+      <c r="E14" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="68" t="s">
-        <v>85</v>
+      <c r="F14" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2096,11 +2976,11 @@
       <c r="D15" s="14">
         <v>101044052</v>
       </c>
-      <c r="E15" s="53" t="s">
+      <c r="E15" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="68" t="s">
-        <v>85</v>
+      <c r="F15" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2116,11 +2996,11 @@
       <c r="D16" s="14">
         <v>101044062</v>
       </c>
-      <c r="E16" s="53" t="s">
+      <c r="E16" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="68" t="s">
-        <v>85</v>
+      <c r="F16" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2136,11 +3016,11 @@
       <c r="D17" s="14">
         <v>101044042</v>
       </c>
-      <c r="E17" s="53" t="s">
+      <c r="E17" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="68" t="s">
-        <v>85</v>
+      <c r="F17" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2156,11 +3036,11 @@
       <c r="D18" s="14">
         <v>101044082</v>
       </c>
-      <c r="E18" s="53" t="s">
+      <c r="E18" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="68" t="s">
-        <v>85</v>
+      <c r="F18" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2176,11 +3056,11 @@
       <c r="D19" s="14">
         <v>101044102</v>
       </c>
-      <c r="E19" s="53" t="s">
+      <c r="E19" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="68" t="s">
-        <v>85</v>
+      <c r="F19" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2196,11 +3076,11 @@
       <c r="D20" s="14">
         <v>101044092</v>
       </c>
-      <c r="E20" s="53" t="s">
+      <c r="E20" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="68" t="s">
-        <v>85</v>
+      <c r="F20" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2212,8 +3092,8 @@
         <v>101010201</v>
       </c>
       <c r="D21" s="22"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="68"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="57"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
@@ -2228,11 +3108,11 @@
       <c r="D22" s="23">
         <v>101052002</v>
       </c>
-      <c r="E22" s="56" t="s">
+      <c r="E22" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="68" t="s">
-        <v>85</v>
+      <c r="F22" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2248,11 +3128,11 @@
       <c r="D23" s="23">
         <v>101052002</v>
       </c>
-      <c r="E23" s="56" t="s">
+      <c r="E23" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="68" t="s">
-        <v>85</v>
+      <c r="F23" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2268,11 +3148,11 @@
       <c r="D24" s="23">
         <v>101052002</v>
       </c>
-      <c r="E24" s="56" t="s">
+      <c r="E24" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="68" t="s">
-        <v>85</v>
+      <c r="F24" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2288,11 +3168,11 @@
       <c r="D25" s="23">
         <v>101052002</v>
       </c>
-      <c r="E25" s="56" t="s">
+      <c r="E25" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="68" t="s">
-        <v>85</v>
+      <c r="F25" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2308,11 +3188,11 @@
       <c r="D26" s="23">
         <v>101052002</v>
       </c>
-      <c r="E26" s="56" t="s">
+      <c r="E26" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F26" s="68" t="s">
-        <v>85</v>
+      <c r="F26" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2328,11 +3208,11 @@
       <c r="D27" s="23">
         <v>101052002</v>
       </c>
-      <c r="E27" s="56" t="s">
+      <c r="E27" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="68" t="s">
-        <v>85</v>
+      <c r="F27" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2348,11 +3228,11 @@
       <c r="D28" s="23">
         <v>101052002</v>
       </c>
-      <c r="E28" s="56" t="s">
+      <c r="E28" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F28" s="68" t="s">
-        <v>85</v>
+      <c r="F28" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2368,11 +3248,11 @@
       <c r="D29" s="23">
         <v>101052002</v>
       </c>
-      <c r="E29" s="56" t="s">
+      <c r="E29" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F29" s="68" t="s">
-        <v>85</v>
+      <c r="F29" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2388,11 +3268,11 @@
       <c r="D30" s="23">
         <v>101052002</v>
       </c>
-      <c r="E30" s="56" t="s">
+      <c r="E30" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F30" s="68" t="s">
-        <v>85</v>
+      <c r="F30" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2408,11 +3288,11 @@
       <c r="D31" s="23">
         <v>101052002</v>
       </c>
-      <c r="E31" s="56" t="s">
+      <c r="E31" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F31" s="68" t="s">
-        <v>85</v>
+      <c r="F31" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2428,11 +3308,11 @@
       <c r="D32" s="23">
         <v>101052002</v>
       </c>
-      <c r="E32" s="56" t="s">
+      <c r="E32" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F32" s="68" t="s">
-        <v>85</v>
+      <c r="F32" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2448,11 +3328,11 @@
       <c r="D33" s="23">
         <v>101052002</v>
       </c>
-      <c r="E33" s="56" t="s">
+      <c r="E33" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F33" s="68" t="s">
-        <v>85</v>
+      <c r="F33" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2468,11 +3348,11 @@
       <c r="D34" s="23">
         <v>101052002</v>
       </c>
-      <c r="E34" s="56" t="s">
+      <c r="E34" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F34" s="68" t="s">
-        <v>85</v>
+      <c r="F34" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2488,11 +3368,11 @@
       <c r="D35" s="23">
         <v>101052002</v>
       </c>
-      <c r="E35" s="56" t="s">
+      <c r="E35" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F35" s="68" t="s">
-        <v>85</v>
+      <c r="F35" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2508,11 +3388,11 @@
       <c r="D36" s="23">
         <v>101052002</v>
       </c>
-      <c r="E36" s="56" t="s">
+      <c r="E36" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F36" s="68" t="s">
-        <v>85</v>
+      <c r="F36" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2528,11 +3408,11 @@
       <c r="D37" s="23">
         <v>101052002</v>
       </c>
-      <c r="E37" s="56" t="s">
+      <c r="E37" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F37" s="68" t="s">
-        <v>85</v>
+      <c r="F37" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2548,11 +3428,11 @@
       <c r="D38" s="23">
         <v>101052002</v>
       </c>
-      <c r="E38" s="56" t="s">
+      <c r="E38" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F38" s="68" t="s">
-        <v>85</v>
+      <c r="F38" s="57" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2581,13 +3461,13 @@
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F38">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="SI">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",F4)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Bot5GUI --v 1.00 beta final
</commit_message>
<xml_diff>
--- a/CUENTAS DE CAJA IVSA.xlsx
+++ b/CUENTAS DE CAJA IVSA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="126" documentId="8_{E7FEFFEB-5A09-49B6-9D87-359617FDBFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B5B7978-DF3D-4E6B-8905-1BC76B74D16B}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="8_{E7FEFFEB-5A09-49B6-9D87-359617FDBFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92A107F5-2B0D-4DBE-981F-8B67329549D5}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DISTRIBUIDORAS" sheetId="1" r:id="rId1"/>
@@ -805,6 +805,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -821,6 +824,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -830,12 +836,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1208,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,15 +1221,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="62" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="61"/>
+      <c r="E1" s="62"/>
     </row>
     <row r="2" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31"/>
@@ -1245,61 +1245,61 @@
       <c r="E2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="63" t="s">
+      <c r="G2" s="64" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="68"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="69"/>
-      <c r="S2" s="69"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="69"/>
-      <c r="V2" s="69"/>
-      <c r="W2" s="69"/>
-      <c r="X2" s="69"/>
-      <c r="Y2" s="69"/>
-      <c r="Z2" s="69"/>
-      <c r="AA2" s="69"/>
-      <c r="AB2" s="69"/>
-      <c r="AC2" s="69"/>
-      <c r="AD2" s="69"/>
-      <c r="AE2" s="69"/>
-      <c r="AF2" s="69"/>
-      <c r="AG2" s="69"/>
-      <c r="AH2" s="69"/>
-      <c r="AI2" s="69"/>
-      <c r="AJ2" s="69"/>
-      <c r="AK2" s="69"/>
-      <c r="AL2" s="69"/>
-      <c r="AM2" s="69"/>
-      <c r="AN2" s="69"/>
-      <c r="AO2" s="69"/>
-      <c r="AP2" s="69"/>
-      <c r="AQ2" s="69"/>
-      <c r="AR2" s="69"/>
-      <c r="AS2" s="69"/>
-      <c r="AT2" s="69"/>
-      <c r="AU2" s="69"/>
-      <c r="AV2" s="69"/>
-      <c r="AW2" s="69"/>
-      <c r="AX2" s="69"/>
-      <c r="AY2" s="69"/>
-      <c r="AZ2" s="69"/>
-      <c r="BA2" s="69"/>
-      <c r="BB2" s="69"/>
-      <c r="BC2" s="69"/>
-      <c r="BD2" s="69"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="58"/>
+      <c r="X2" s="58"/>
+      <c r="Y2" s="58"/>
+      <c r="Z2" s="58"/>
+      <c r="AA2" s="58"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="58"/>
+      <c r="AD2" s="58"/>
+      <c r="AE2" s="58"/>
+      <c r="AF2" s="58"/>
+      <c r="AG2" s="58"/>
+      <c r="AH2" s="58"/>
+      <c r="AI2" s="58"/>
+      <c r="AJ2" s="58"/>
+      <c r="AK2" s="58"/>
+      <c r="AL2" s="58"/>
+      <c r="AM2" s="58"/>
+      <c r="AN2" s="58"/>
+      <c r="AO2" s="58"/>
+      <c r="AP2" s="58"/>
+      <c r="AQ2" s="58"/>
+      <c r="AR2" s="58"/>
+      <c r="AS2" s="58"/>
+      <c r="AT2" s="58"/>
+      <c r="AU2" s="58"/>
+      <c r="AV2" s="58"/>
+      <c r="AW2" s="58"/>
+      <c r="AX2" s="58"/>
+      <c r="AY2" s="58"/>
+      <c r="AZ2" s="58"/>
+      <c r="BA2" s="58"/>
+      <c r="BB2" s="58"/>
+      <c r="BC2" s="58"/>
+      <c r="BD2" s="58"/>
     </row>
     <row r="3" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34"/>
@@ -1311,57 +1311,57 @@
       </c>
       <c r="D3" s="37"/>
       <c r="E3" s="38"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="69"/>
-      <c r="Q3" s="69"/>
-      <c r="R3" s="69"/>
-      <c r="S3" s="69"/>
-      <c r="T3" s="69"/>
-      <c r="U3" s="69"/>
-      <c r="V3" s="69"/>
-      <c r="W3" s="69"/>
-      <c r="X3" s="69"/>
-      <c r="Y3" s="69"/>
-      <c r="Z3" s="69"/>
-      <c r="AA3" s="69"/>
-      <c r="AB3" s="69"/>
-      <c r="AC3" s="69"/>
-      <c r="AD3" s="69"/>
-      <c r="AE3" s="69"/>
-      <c r="AF3" s="69"/>
-      <c r="AG3" s="69"/>
-      <c r="AH3" s="69"/>
-      <c r="AI3" s="69"/>
-      <c r="AJ3" s="69"/>
-      <c r="AK3" s="69"/>
-      <c r="AL3" s="69"/>
-      <c r="AM3" s="69"/>
-      <c r="AN3" s="69"/>
-      <c r="AO3" s="69"/>
-      <c r="AP3" s="69"/>
-      <c r="AQ3" s="69"/>
-      <c r="AR3" s="69"/>
-      <c r="AS3" s="69"/>
-      <c r="AT3" s="69"/>
-      <c r="AU3" s="69"/>
-      <c r="AV3" s="69"/>
-      <c r="AW3" s="69"/>
-      <c r="AX3" s="69"/>
-      <c r="AY3" s="69"/>
-      <c r="AZ3" s="69"/>
-      <c r="BA3" s="69"/>
-      <c r="BB3" s="69"/>
-      <c r="BC3" s="69"/>
-      <c r="BD3" s="69"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58"/>
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58"/>
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="58"/>
+      <c r="AC3" s="58"/>
+      <c r="AD3" s="58"/>
+      <c r="AE3" s="58"/>
+      <c r="AF3" s="58"/>
+      <c r="AG3" s="58"/>
+      <c r="AH3" s="58"/>
+      <c r="AI3" s="58"/>
+      <c r="AJ3" s="58"/>
+      <c r="AK3" s="58"/>
+      <c r="AL3" s="58"/>
+      <c r="AM3" s="58"/>
+      <c r="AN3" s="58"/>
+      <c r="AO3" s="58"/>
+      <c r="AP3" s="58"/>
+      <c r="AQ3" s="58"/>
+      <c r="AR3" s="58"/>
+      <c r="AS3" s="58"/>
+      <c r="AT3" s="58"/>
+      <c r="AU3" s="58"/>
+      <c r="AV3" s="58"/>
+      <c r="AW3" s="58"/>
+      <c r="AX3" s="58"/>
+      <c r="AY3" s="58"/>
+      <c r="AZ3" s="58"/>
+      <c r="BA3" s="58"/>
+      <c r="BB3" s="58"/>
+      <c r="BC3" s="58"/>
+      <c r="BD3" s="58"/>
     </row>
     <row r="4" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
@@ -1385,55 +1385,55 @@
       <c r="G4" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="69"/>
-      <c r="O4" s="69"/>
-      <c r="P4" s="69"/>
-      <c r="Q4" s="69"/>
-      <c r="R4" s="69"/>
-      <c r="S4" s="69"/>
-      <c r="T4" s="69"/>
-      <c r="U4" s="69"/>
-      <c r="V4" s="69"/>
-      <c r="W4" s="69"/>
-      <c r="X4" s="69"/>
-      <c r="Y4" s="69"/>
-      <c r="Z4" s="69"/>
-      <c r="AA4" s="69"/>
-      <c r="AB4" s="69"/>
-      <c r="AC4" s="69"/>
-      <c r="AD4" s="69"/>
-      <c r="AE4" s="69"/>
-      <c r="AF4" s="69"/>
-      <c r="AG4" s="69"/>
-      <c r="AH4" s="69"/>
-      <c r="AI4" s="69"/>
-      <c r="AJ4" s="69"/>
-      <c r="AK4" s="69"/>
-      <c r="AL4" s="69"/>
-      <c r="AM4" s="69"/>
-      <c r="AN4" s="69"/>
-      <c r="AO4" s="69"/>
-      <c r="AP4" s="69"/>
-      <c r="AQ4" s="69"/>
-      <c r="AR4" s="69"/>
-      <c r="AS4" s="69"/>
-      <c r="AT4" s="69"/>
-      <c r="AU4" s="69"/>
-      <c r="AV4" s="69"/>
-      <c r="AW4" s="69"/>
-      <c r="AX4" s="69"/>
-      <c r="AY4" s="69"/>
-      <c r="AZ4" s="69"/>
-      <c r="BA4" s="69"/>
-      <c r="BB4" s="69"/>
-      <c r="BC4" s="69"/>
-      <c r="BD4" s="69"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="58"/>
+      <c r="P4" s="58"/>
+      <c r="Q4" s="58"/>
+      <c r="R4" s="58"/>
+      <c r="S4" s="58"/>
+      <c r="T4" s="58"/>
+      <c r="U4" s="58"/>
+      <c r="V4" s="58"/>
+      <c r="W4" s="58"/>
+      <c r="X4" s="58"/>
+      <c r="Y4" s="58"/>
+      <c r="Z4" s="58"/>
+      <c r="AA4" s="58"/>
+      <c r="AB4" s="58"/>
+      <c r="AC4" s="58"/>
+      <c r="AD4" s="58"/>
+      <c r="AE4" s="58"/>
+      <c r="AF4" s="58"/>
+      <c r="AG4" s="58"/>
+      <c r="AH4" s="58"/>
+      <c r="AI4" s="58"/>
+      <c r="AJ4" s="58"/>
+      <c r="AK4" s="58"/>
+      <c r="AL4" s="58"/>
+      <c r="AM4" s="58"/>
+      <c r="AN4" s="58"/>
+      <c r="AO4" s="58"/>
+      <c r="AP4" s="58"/>
+      <c r="AQ4" s="58"/>
+      <c r="AR4" s="58"/>
+      <c r="AS4" s="58"/>
+      <c r="AT4" s="58"/>
+      <c r="AU4" s="58"/>
+      <c r="AV4" s="58"/>
+      <c r="AW4" s="58"/>
+      <c r="AX4" s="58"/>
+      <c r="AY4" s="58"/>
+      <c r="AZ4" s="58"/>
+      <c r="BA4" s="58"/>
+      <c r="BB4" s="58"/>
+      <c r="BC4" s="58"/>
+      <c r="BD4" s="58"/>
     </row>
     <row r="5" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
@@ -1457,55 +1457,55 @@
       <c r="G5" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
-      <c r="R5" s="69"/>
-      <c r="S5" s="69"/>
-      <c r="T5" s="69"/>
-      <c r="U5" s="69"/>
-      <c r="V5" s="69"/>
-      <c r="W5" s="69"/>
-      <c r="X5" s="69"/>
-      <c r="Y5" s="69"/>
-      <c r="Z5" s="69"/>
-      <c r="AA5" s="69"/>
-      <c r="AB5" s="69"/>
-      <c r="AC5" s="69"/>
-      <c r="AD5" s="69"/>
-      <c r="AE5" s="69"/>
-      <c r="AF5" s="69"/>
-      <c r="AG5" s="69"/>
-      <c r="AH5" s="69"/>
-      <c r="AI5" s="69"/>
-      <c r="AJ5" s="69"/>
-      <c r="AK5" s="69"/>
-      <c r="AL5" s="69"/>
-      <c r="AM5" s="69"/>
-      <c r="AN5" s="69"/>
-      <c r="AO5" s="69"/>
-      <c r="AP5" s="69"/>
-      <c r="AQ5" s="69"/>
-      <c r="AR5" s="69"/>
-      <c r="AS5" s="69"/>
-      <c r="AT5" s="69"/>
-      <c r="AU5" s="69"/>
-      <c r="AV5" s="69"/>
-      <c r="AW5" s="69"/>
-      <c r="AX5" s="69"/>
-      <c r="AY5" s="69"/>
-      <c r="AZ5" s="69"/>
-      <c r="BA5" s="69"/>
-      <c r="BB5" s="69"/>
-      <c r="BC5" s="69"/>
-      <c r="BD5" s="69"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="58"/>
+      <c r="R5" s="58"/>
+      <c r="S5" s="58"/>
+      <c r="T5" s="58"/>
+      <c r="U5" s="58"/>
+      <c r="V5" s="58"/>
+      <c r="W5" s="58"/>
+      <c r="X5" s="58"/>
+      <c r="Y5" s="58"/>
+      <c r="Z5" s="58"/>
+      <c r="AA5" s="58"/>
+      <c r="AB5" s="58"/>
+      <c r="AC5" s="58"/>
+      <c r="AD5" s="58"/>
+      <c r="AE5" s="58"/>
+      <c r="AF5" s="58"/>
+      <c r="AG5" s="58"/>
+      <c r="AH5" s="58"/>
+      <c r="AI5" s="58"/>
+      <c r="AJ5" s="58"/>
+      <c r="AK5" s="58"/>
+      <c r="AL5" s="58"/>
+      <c r="AM5" s="58"/>
+      <c r="AN5" s="58"/>
+      <c r="AO5" s="58"/>
+      <c r="AP5" s="58"/>
+      <c r="AQ5" s="58"/>
+      <c r="AR5" s="58"/>
+      <c r="AS5" s="58"/>
+      <c r="AT5" s="58"/>
+      <c r="AU5" s="58"/>
+      <c r="AV5" s="58"/>
+      <c r="AW5" s="58"/>
+      <c r="AX5" s="58"/>
+      <c r="AY5" s="58"/>
+      <c r="AZ5" s="58"/>
+      <c r="BA5" s="58"/>
+      <c r="BB5" s="58"/>
+      <c r="BC5" s="58"/>
+      <c r="BD5" s="58"/>
     </row>
     <row r="6" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
@@ -1529,55 +1529,55 @@
       <c r="G6" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="69"/>
-      <c r="N6" s="69"/>
-      <c r="O6" s="69"/>
-      <c r="P6" s="69"/>
-      <c r="Q6" s="69"/>
-      <c r="R6" s="69"/>
-      <c r="S6" s="69"/>
-      <c r="T6" s="69"/>
-      <c r="U6" s="69"/>
-      <c r="V6" s="69"/>
-      <c r="W6" s="69"/>
-      <c r="X6" s="69"/>
-      <c r="Y6" s="69"/>
-      <c r="Z6" s="69"/>
-      <c r="AA6" s="69"/>
-      <c r="AB6" s="69"/>
-      <c r="AC6" s="69"/>
-      <c r="AD6" s="69"/>
-      <c r="AE6" s="69"/>
-      <c r="AF6" s="69"/>
-      <c r="AG6" s="69"/>
-      <c r="AH6" s="69"/>
-      <c r="AI6" s="69"/>
-      <c r="AJ6" s="69"/>
-      <c r="AK6" s="69"/>
-      <c r="AL6" s="69"/>
-      <c r="AM6" s="69"/>
-      <c r="AN6" s="69"/>
-      <c r="AO6" s="69"/>
-      <c r="AP6" s="69"/>
-      <c r="AQ6" s="69"/>
-      <c r="AR6" s="69"/>
-      <c r="AS6" s="69"/>
-      <c r="AT6" s="69"/>
-      <c r="AU6" s="69"/>
-      <c r="AV6" s="69"/>
-      <c r="AW6" s="69"/>
-      <c r="AX6" s="69"/>
-      <c r="AY6" s="69"/>
-      <c r="AZ6" s="69"/>
-      <c r="BA6" s="69"/>
-      <c r="BB6" s="69"/>
-      <c r="BC6" s="69"/>
-      <c r="BD6" s="69"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="58"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="58"/>
+      <c r="R6" s="58"/>
+      <c r="S6" s="58"/>
+      <c r="T6" s="58"/>
+      <c r="U6" s="58"/>
+      <c r="V6" s="58"/>
+      <c r="W6" s="58"/>
+      <c r="X6" s="58"/>
+      <c r="Y6" s="58"/>
+      <c r="Z6" s="58"/>
+      <c r="AA6" s="58"/>
+      <c r="AB6" s="58"/>
+      <c r="AC6" s="58"/>
+      <c r="AD6" s="58"/>
+      <c r="AE6" s="58"/>
+      <c r="AF6" s="58"/>
+      <c r="AG6" s="58"/>
+      <c r="AH6" s="58"/>
+      <c r="AI6" s="58"/>
+      <c r="AJ6" s="58"/>
+      <c r="AK6" s="58"/>
+      <c r="AL6" s="58"/>
+      <c r="AM6" s="58"/>
+      <c r="AN6" s="58"/>
+      <c r="AO6" s="58"/>
+      <c r="AP6" s="58"/>
+      <c r="AQ6" s="58"/>
+      <c r="AR6" s="58"/>
+      <c r="AS6" s="58"/>
+      <c r="AT6" s="58"/>
+      <c r="AU6" s="58"/>
+      <c r="AV6" s="58"/>
+      <c r="AW6" s="58"/>
+      <c r="AX6" s="58"/>
+      <c r="AY6" s="58"/>
+      <c r="AZ6" s="58"/>
+      <c r="BA6" s="58"/>
+      <c r="BB6" s="58"/>
+      <c r="BC6" s="58"/>
+      <c r="BD6" s="58"/>
     </row>
     <row r="7" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
@@ -1601,55 +1601,55 @@
       <c r="G7" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
-      <c r="O7" s="69"/>
-      <c r="P7" s="69"/>
-      <c r="Q7" s="69"/>
-      <c r="R7" s="69"/>
-      <c r="S7" s="69"/>
-      <c r="T7" s="69"/>
-      <c r="U7" s="69"/>
-      <c r="V7" s="69"/>
-      <c r="W7" s="69"/>
-      <c r="X7" s="69"/>
-      <c r="Y7" s="69"/>
-      <c r="Z7" s="69"/>
-      <c r="AA7" s="69"/>
-      <c r="AB7" s="69"/>
-      <c r="AC7" s="69"/>
-      <c r="AD7" s="69"/>
-      <c r="AE7" s="69"/>
-      <c r="AF7" s="69"/>
-      <c r="AG7" s="69"/>
-      <c r="AH7" s="69"/>
-      <c r="AI7" s="69"/>
-      <c r="AJ7" s="69"/>
-      <c r="AK7" s="69"/>
-      <c r="AL7" s="69"/>
-      <c r="AM7" s="69"/>
-      <c r="AN7" s="69"/>
-      <c r="AO7" s="69"/>
-      <c r="AP7" s="69"/>
-      <c r="AQ7" s="69"/>
-      <c r="AR7" s="69"/>
-      <c r="AS7" s="69"/>
-      <c r="AT7" s="69"/>
-      <c r="AU7" s="69"/>
-      <c r="AV7" s="69"/>
-      <c r="AW7" s="69"/>
-      <c r="AX7" s="69"/>
-      <c r="AY7" s="69"/>
-      <c r="AZ7" s="69"/>
-      <c r="BA7" s="69"/>
-      <c r="BB7" s="69"/>
-      <c r="BC7" s="69"/>
-      <c r="BD7" s="69"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
+      <c r="M7" s="58"/>
+      <c r="N7" s="58"/>
+      <c r="O7" s="58"/>
+      <c r="P7" s="58"/>
+      <c r="Q7" s="58"/>
+      <c r="R7" s="58"/>
+      <c r="S7" s="58"/>
+      <c r="T7" s="58"/>
+      <c r="U7" s="58"/>
+      <c r="V7" s="58"/>
+      <c r="W7" s="58"/>
+      <c r="X7" s="58"/>
+      <c r="Y7" s="58"/>
+      <c r="Z7" s="58"/>
+      <c r="AA7" s="58"/>
+      <c r="AB7" s="58"/>
+      <c r="AC7" s="58"/>
+      <c r="AD7" s="58"/>
+      <c r="AE7" s="58"/>
+      <c r="AF7" s="58"/>
+      <c r="AG7" s="58"/>
+      <c r="AH7" s="58"/>
+      <c r="AI7" s="58"/>
+      <c r="AJ7" s="58"/>
+      <c r="AK7" s="58"/>
+      <c r="AL7" s="58"/>
+      <c r="AM7" s="58"/>
+      <c r="AN7" s="58"/>
+      <c r="AO7" s="58"/>
+      <c r="AP7" s="58"/>
+      <c r="AQ7" s="58"/>
+      <c r="AR7" s="58"/>
+      <c r="AS7" s="58"/>
+      <c r="AT7" s="58"/>
+      <c r="AU7" s="58"/>
+      <c r="AV7" s="58"/>
+      <c r="AW7" s="58"/>
+      <c r="AX7" s="58"/>
+      <c r="AY7" s="58"/>
+      <c r="AZ7" s="58"/>
+      <c r="BA7" s="58"/>
+      <c r="BB7" s="58"/>
+      <c r="BC7" s="58"/>
+      <c r="BD7" s="58"/>
     </row>
     <row r="8" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
@@ -1673,55 +1673,55 @@
       <c r="G8" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
-      <c r="O8" s="69"/>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="69"/>
-      <c r="S8" s="69"/>
-      <c r="T8" s="69"/>
-      <c r="U8" s="69"/>
-      <c r="V8" s="69"/>
-      <c r="W8" s="69"/>
-      <c r="X8" s="69"/>
-      <c r="Y8" s="69"/>
-      <c r="Z8" s="69"/>
-      <c r="AA8" s="69"/>
-      <c r="AB8" s="69"/>
-      <c r="AC8" s="69"/>
-      <c r="AD8" s="69"/>
-      <c r="AE8" s="69"/>
-      <c r="AF8" s="69"/>
-      <c r="AG8" s="69"/>
-      <c r="AH8" s="69"/>
-      <c r="AI8" s="69"/>
-      <c r="AJ8" s="69"/>
-      <c r="AK8" s="69"/>
-      <c r="AL8" s="69"/>
-      <c r="AM8" s="69"/>
-      <c r="AN8" s="69"/>
-      <c r="AO8" s="69"/>
-      <c r="AP8" s="69"/>
-      <c r="AQ8" s="69"/>
-      <c r="AR8" s="69"/>
-      <c r="AS8" s="69"/>
-      <c r="AT8" s="69"/>
-      <c r="AU8" s="69"/>
-      <c r="AV8" s="69"/>
-      <c r="AW8" s="69"/>
-      <c r="AX8" s="69"/>
-      <c r="AY8" s="69"/>
-      <c r="AZ8" s="69"/>
-      <c r="BA8" s="69"/>
-      <c r="BB8" s="69"/>
-      <c r="BC8" s="69"/>
-      <c r="BD8" s="69"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="58"/>
+      <c r="P8" s="58"/>
+      <c r="Q8" s="58"/>
+      <c r="R8" s="58"/>
+      <c r="S8" s="58"/>
+      <c r="T8" s="58"/>
+      <c r="U8" s="58"/>
+      <c r="V8" s="58"/>
+      <c r="W8" s="58"/>
+      <c r="X8" s="58"/>
+      <c r="Y8" s="58"/>
+      <c r="Z8" s="58"/>
+      <c r="AA8" s="58"/>
+      <c r="AB8" s="58"/>
+      <c r="AC8" s="58"/>
+      <c r="AD8" s="58"/>
+      <c r="AE8" s="58"/>
+      <c r="AF8" s="58"/>
+      <c r="AG8" s="58"/>
+      <c r="AH8" s="58"/>
+      <c r="AI8" s="58"/>
+      <c r="AJ8" s="58"/>
+      <c r="AK8" s="58"/>
+      <c r="AL8" s="58"/>
+      <c r="AM8" s="58"/>
+      <c r="AN8" s="58"/>
+      <c r="AO8" s="58"/>
+      <c r="AP8" s="58"/>
+      <c r="AQ8" s="58"/>
+      <c r="AR8" s="58"/>
+      <c r="AS8" s="58"/>
+      <c r="AT8" s="58"/>
+      <c r="AU8" s="58"/>
+      <c r="AV8" s="58"/>
+      <c r="AW8" s="58"/>
+      <c r="AX8" s="58"/>
+      <c r="AY8" s="58"/>
+      <c r="AZ8" s="58"/>
+      <c r="BA8" s="58"/>
+      <c r="BB8" s="58"/>
+      <c r="BC8" s="58"/>
+      <c r="BD8" s="58"/>
     </row>
     <row r="9" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
@@ -1745,55 +1745,55 @@
       <c r="G9" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
-      <c r="K9" s="69"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="69"/>
-      <c r="N9" s="69"/>
-      <c r="O9" s="69"/>
-      <c r="P9" s="69"/>
-      <c r="Q9" s="69"/>
-      <c r="R9" s="69"/>
-      <c r="S9" s="69"/>
-      <c r="T9" s="69"/>
-      <c r="U9" s="69"/>
-      <c r="V9" s="69"/>
-      <c r="W9" s="69"/>
-      <c r="X9" s="69"/>
-      <c r="Y9" s="69"/>
-      <c r="Z9" s="69"/>
-      <c r="AA9" s="69"/>
-      <c r="AB9" s="69"/>
-      <c r="AC9" s="69"/>
-      <c r="AD9" s="69"/>
-      <c r="AE9" s="69"/>
-      <c r="AF9" s="69"/>
-      <c r="AG9" s="69"/>
-      <c r="AH9" s="69"/>
-      <c r="AI9" s="69"/>
-      <c r="AJ9" s="69"/>
-      <c r="AK9" s="69"/>
-      <c r="AL9" s="69"/>
-      <c r="AM9" s="69"/>
-      <c r="AN9" s="69"/>
-      <c r="AO9" s="69"/>
-      <c r="AP9" s="69"/>
-      <c r="AQ9" s="69"/>
-      <c r="AR9" s="69"/>
-      <c r="AS9" s="69"/>
-      <c r="AT9" s="69"/>
-      <c r="AU9" s="69"/>
-      <c r="AV9" s="69"/>
-      <c r="AW9" s="69"/>
-      <c r="AX9" s="69"/>
-      <c r="AY9" s="69"/>
-      <c r="AZ9" s="69"/>
-      <c r="BA9" s="69"/>
-      <c r="BB9" s="69"/>
-      <c r="BC9" s="69"/>
-      <c r="BD9" s="69"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="58"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="58"/>
+      <c r="Q9" s="58"/>
+      <c r="R9" s="58"/>
+      <c r="S9" s="58"/>
+      <c r="T9" s="58"/>
+      <c r="U9" s="58"/>
+      <c r="V9" s="58"/>
+      <c r="W9" s="58"/>
+      <c r="X9" s="58"/>
+      <c r="Y9" s="58"/>
+      <c r="Z9" s="58"/>
+      <c r="AA9" s="58"/>
+      <c r="AB9" s="58"/>
+      <c r="AC9" s="58"/>
+      <c r="AD9" s="58"/>
+      <c r="AE9" s="58"/>
+      <c r="AF9" s="58"/>
+      <c r="AG9" s="58"/>
+      <c r="AH9" s="58"/>
+      <c r="AI9" s="58"/>
+      <c r="AJ9" s="58"/>
+      <c r="AK9" s="58"/>
+      <c r="AL9" s="58"/>
+      <c r="AM9" s="58"/>
+      <c r="AN9" s="58"/>
+      <c r="AO9" s="58"/>
+      <c r="AP9" s="58"/>
+      <c r="AQ9" s="58"/>
+      <c r="AR9" s="58"/>
+      <c r="AS9" s="58"/>
+      <c r="AT9" s="58"/>
+      <c r="AU9" s="58"/>
+      <c r="AV9" s="58"/>
+      <c r="AW9" s="58"/>
+      <c r="AX9" s="58"/>
+      <c r="AY9" s="58"/>
+      <c r="AZ9" s="58"/>
+      <c r="BA9" s="58"/>
+      <c r="BB9" s="58"/>
+      <c r="BC9" s="58"/>
+      <c r="BD9" s="58"/>
     </row>
     <row r="10" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
@@ -1817,55 +1817,55 @@
       <c r="G10" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="69"/>
-      <c r="N10" s="69"/>
-      <c r="O10" s="69"/>
-      <c r="P10" s="69"/>
-      <c r="Q10" s="69"/>
-      <c r="R10" s="69"/>
-      <c r="S10" s="69"/>
-      <c r="T10" s="69"/>
-      <c r="U10" s="69"/>
-      <c r="V10" s="69"/>
-      <c r="W10" s="69"/>
-      <c r="X10" s="69"/>
-      <c r="Y10" s="69"/>
-      <c r="Z10" s="69"/>
-      <c r="AA10" s="69"/>
-      <c r="AB10" s="69"/>
-      <c r="AC10" s="69"/>
-      <c r="AD10" s="69"/>
-      <c r="AE10" s="69"/>
-      <c r="AF10" s="69"/>
-      <c r="AG10" s="69"/>
-      <c r="AH10" s="69"/>
-      <c r="AI10" s="69"/>
-      <c r="AJ10" s="69"/>
-      <c r="AK10" s="69"/>
-      <c r="AL10" s="69"/>
-      <c r="AM10" s="69"/>
-      <c r="AN10" s="69"/>
-      <c r="AO10" s="69"/>
-      <c r="AP10" s="69"/>
-      <c r="AQ10" s="69"/>
-      <c r="AR10" s="69"/>
-      <c r="AS10" s="69"/>
-      <c r="AT10" s="69"/>
-      <c r="AU10" s="69"/>
-      <c r="AV10" s="69"/>
-      <c r="AW10" s="69"/>
-      <c r="AX10" s="69"/>
-      <c r="AY10" s="69"/>
-      <c r="AZ10" s="69"/>
-      <c r="BA10" s="69"/>
-      <c r="BB10" s="69"/>
-      <c r="BC10" s="69"/>
-      <c r="BD10" s="69"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="58"/>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="58"/>
+      <c r="S10" s="58"/>
+      <c r="T10" s="58"/>
+      <c r="U10" s="58"/>
+      <c r="V10" s="58"/>
+      <c r="W10" s="58"/>
+      <c r="X10" s="58"/>
+      <c r="Y10" s="58"/>
+      <c r="Z10" s="58"/>
+      <c r="AA10" s="58"/>
+      <c r="AB10" s="58"/>
+      <c r="AC10" s="58"/>
+      <c r="AD10" s="58"/>
+      <c r="AE10" s="58"/>
+      <c r="AF10" s="58"/>
+      <c r="AG10" s="58"/>
+      <c r="AH10" s="58"/>
+      <c r="AI10" s="58"/>
+      <c r="AJ10" s="58"/>
+      <c r="AK10" s="58"/>
+      <c r="AL10" s="58"/>
+      <c r="AM10" s="58"/>
+      <c r="AN10" s="58"/>
+      <c r="AO10" s="58"/>
+      <c r="AP10" s="58"/>
+      <c r="AQ10" s="58"/>
+      <c r="AR10" s="58"/>
+      <c r="AS10" s="58"/>
+      <c r="AT10" s="58"/>
+      <c r="AU10" s="58"/>
+      <c r="AV10" s="58"/>
+      <c r="AW10" s="58"/>
+      <c r="AX10" s="58"/>
+      <c r="AY10" s="58"/>
+      <c r="AZ10" s="58"/>
+      <c r="BA10" s="58"/>
+      <c r="BB10" s="58"/>
+      <c r="BC10" s="58"/>
+      <c r="BD10" s="58"/>
     </row>
     <row r="11" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
@@ -1889,55 +1889,55 @@
       <c r="G11" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="69"/>
-      <c r="L11" s="69"/>
-      <c r="M11" s="69"/>
-      <c r="N11" s="69"/>
-      <c r="O11" s="69"/>
-      <c r="P11" s="69"/>
-      <c r="Q11" s="69"/>
-      <c r="R11" s="69"/>
-      <c r="S11" s="69"/>
-      <c r="T11" s="69"/>
-      <c r="U11" s="69"/>
-      <c r="V11" s="69"/>
-      <c r="W11" s="69"/>
-      <c r="X11" s="69"/>
-      <c r="Y11" s="69"/>
-      <c r="Z11" s="69"/>
-      <c r="AA11" s="69"/>
-      <c r="AB11" s="69"/>
-      <c r="AC11" s="69"/>
-      <c r="AD11" s="69"/>
-      <c r="AE11" s="69"/>
-      <c r="AF11" s="69"/>
-      <c r="AG11" s="69"/>
-      <c r="AH11" s="69"/>
-      <c r="AI11" s="69"/>
-      <c r="AJ11" s="69"/>
-      <c r="AK11" s="69"/>
-      <c r="AL11" s="69"/>
-      <c r="AM11" s="69"/>
-      <c r="AN11" s="69"/>
-      <c r="AO11" s="69"/>
-      <c r="AP11" s="69"/>
-      <c r="AQ11" s="69"/>
-      <c r="AR11" s="69"/>
-      <c r="AS11" s="69"/>
-      <c r="AT11" s="69"/>
-      <c r="AU11" s="69"/>
-      <c r="AV11" s="69"/>
-      <c r="AW11" s="69"/>
-      <c r="AX11" s="69"/>
-      <c r="AY11" s="69"/>
-      <c r="AZ11" s="69"/>
-      <c r="BA11" s="69"/>
-      <c r="BB11" s="69"/>
-      <c r="BC11" s="69"/>
-      <c r="BD11" s="69"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="58"/>
+      <c r="S11" s="58"/>
+      <c r="T11" s="58"/>
+      <c r="U11" s="58"/>
+      <c r="V11" s="58"/>
+      <c r="W11" s="58"/>
+      <c r="X11" s="58"/>
+      <c r="Y11" s="58"/>
+      <c r="Z11" s="58"/>
+      <c r="AA11" s="58"/>
+      <c r="AB11" s="58"/>
+      <c r="AC11" s="58"/>
+      <c r="AD11" s="58"/>
+      <c r="AE11" s="58"/>
+      <c r="AF11" s="58"/>
+      <c r="AG11" s="58"/>
+      <c r="AH11" s="58"/>
+      <c r="AI11" s="58"/>
+      <c r="AJ11" s="58"/>
+      <c r="AK11" s="58"/>
+      <c r="AL11" s="58"/>
+      <c r="AM11" s="58"/>
+      <c r="AN11" s="58"/>
+      <c r="AO11" s="58"/>
+      <c r="AP11" s="58"/>
+      <c r="AQ11" s="58"/>
+      <c r="AR11" s="58"/>
+      <c r="AS11" s="58"/>
+      <c r="AT11" s="58"/>
+      <c r="AU11" s="58"/>
+      <c r="AV11" s="58"/>
+      <c r="AW11" s="58"/>
+      <c r="AX11" s="58"/>
+      <c r="AY11" s="58"/>
+      <c r="AZ11" s="58"/>
+      <c r="BA11" s="58"/>
+      <c r="BB11" s="58"/>
+      <c r="BC11" s="58"/>
+      <c r="BD11" s="58"/>
     </row>
     <row r="12" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
@@ -1961,55 +1961,55 @@
       <c r="G12" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="69"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="69"/>
-      <c r="P12" s="69"/>
-      <c r="Q12" s="69"/>
-      <c r="R12" s="69"/>
-      <c r="S12" s="69"/>
-      <c r="T12" s="69"/>
-      <c r="U12" s="69"/>
-      <c r="V12" s="69"/>
-      <c r="W12" s="69"/>
-      <c r="X12" s="69"/>
-      <c r="Y12" s="69"/>
-      <c r="Z12" s="69"/>
-      <c r="AA12" s="69"/>
-      <c r="AB12" s="69"/>
-      <c r="AC12" s="69"/>
-      <c r="AD12" s="69"/>
-      <c r="AE12" s="69"/>
-      <c r="AF12" s="69"/>
-      <c r="AG12" s="69"/>
-      <c r="AH12" s="69"/>
-      <c r="AI12" s="69"/>
-      <c r="AJ12" s="69"/>
-      <c r="AK12" s="69"/>
-      <c r="AL12" s="69"/>
-      <c r="AM12" s="69"/>
-      <c r="AN12" s="69"/>
-      <c r="AO12" s="69"/>
-      <c r="AP12" s="69"/>
-      <c r="AQ12" s="69"/>
-      <c r="AR12" s="69"/>
-      <c r="AS12" s="69"/>
-      <c r="AT12" s="69"/>
-      <c r="AU12" s="69"/>
-      <c r="AV12" s="69"/>
-      <c r="AW12" s="69"/>
-      <c r="AX12" s="69"/>
-      <c r="AY12" s="69"/>
-      <c r="AZ12" s="69"/>
-      <c r="BA12" s="69"/>
-      <c r="BB12" s="69"/>
-      <c r="BC12" s="69"/>
-      <c r="BD12" s="69"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="58"/>
+      <c r="N12" s="58"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="58"/>
+      <c r="Q12" s="58"/>
+      <c r="R12" s="58"/>
+      <c r="S12" s="58"/>
+      <c r="T12" s="58"/>
+      <c r="U12" s="58"/>
+      <c r="V12" s="58"/>
+      <c r="W12" s="58"/>
+      <c r="X12" s="58"/>
+      <c r="Y12" s="58"/>
+      <c r="Z12" s="58"/>
+      <c r="AA12" s="58"/>
+      <c r="AB12" s="58"/>
+      <c r="AC12" s="58"/>
+      <c r="AD12" s="58"/>
+      <c r="AE12" s="58"/>
+      <c r="AF12" s="58"/>
+      <c r="AG12" s="58"/>
+      <c r="AH12" s="58"/>
+      <c r="AI12" s="58"/>
+      <c r="AJ12" s="58"/>
+      <c r="AK12" s="58"/>
+      <c r="AL12" s="58"/>
+      <c r="AM12" s="58"/>
+      <c r="AN12" s="58"/>
+      <c r="AO12" s="58"/>
+      <c r="AP12" s="58"/>
+      <c r="AQ12" s="58"/>
+      <c r="AR12" s="58"/>
+      <c r="AS12" s="58"/>
+      <c r="AT12" s="58"/>
+      <c r="AU12" s="58"/>
+      <c r="AV12" s="58"/>
+      <c r="AW12" s="58"/>
+      <c r="AX12" s="58"/>
+      <c r="AY12" s="58"/>
+      <c r="AZ12" s="58"/>
+      <c r="BA12" s="58"/>
+      <c r="BB12" s="58"/>
+      <c r="BC12" s="58"/>
+      <c r="BD12" s="58"/>
     </row>
     <row r="13" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
@@ -2033,55 +2033,55 @@
       <c r="G13" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H13" s="69"/>
-      <c r="I13" s="69"/>
-      <c r="J13" s="69"/>
-      <c r="K13" s="69"/>
-      <c r="L13" s="69"/>
-      <c r="M13" s="69"/>
-      <c r="N13" s="69"/>
-      <c r="O13" s="69"/>
-      <c r="P13" s="69"/>
-      <c r="Q13" s="69"/>
-      <c r="R13" s="69"/>
-      <c r="S13" s="69"/>
-      <c r="T13" s="69"/>
-      <c r="U13" s="69"/>
-      <c r="V13" s="69"/>
-      <c r="W13" s="69"/>
-      <c r="X13" s="69"/>
-      <c r="Y13" s="69"/>
-      <c r="Z13" s="69"/>
-      <c r="AA13" s="69"/>
-      <c r="AB13" s="69"/>
-      <c r="AC13" s="69"/>
-      <c r="AD13" s="69"/>
-      <c r="AE13" s="69"/>
-      <c r="AF13" s="69"/>
-      <c r="AG13" s="69"/>
-      <c r="AH13" s="69"/>
-      <c r="AI13" s="69"/>
-      <c r="AJ13" s="69"/>
-      <c r="AK13" s="69"/>
-      <c r="AL13" s="69"/>
-      <c r="AM13" s="69"/>
-      <c r="AN13" s="69"/>
-      <c r="AO13" s="69"/>
-      <c r="AP13" s="69"/>
-      <c r="AQ13" s="69"/>
-      <c r="AR13" s="69"/>
-      <c r="AS13" s="69"/>
-      <c r="AT13" s="69"/>
-      <c r="AU13" s="69"/>
-      <c r="AV13" s="69"/>
-      <c r="AW13" s="69"/>
-      <c r="AX13" s="69"/>
-      <c r="AY13" s="69"/>
-      <c r="AZ13" s="69"/>
-      <c r="BA13" s="69"/>
-      <c r="BB13" s="69"/>
-      <c r="BC13" s="69"/>
-      <c r="BD13" s="69"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="58"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="58"/>
+      <c r="Q13" s="58"/>
+      <c r="R13" s="58"/>
+      <c r="S13" s="58"/>
+      <c r="T13" s="58"/>
+      <c r="U13" s="58"/>
+      <c r="V13" s="58"/>
+      <c r="W13" s="58"/>
+      <c r="X13" s="58"/>
+      <c r="Y13" s="58"/>
+      <c r="Z13" s="58"/>
+      <c r="AA13" s="58"/>
+      <c r="AB13" s="58"/>
+      <c r="AC13" s="58"/>
+      <c r="AD13" s="58"/>
+      <c r="AE13" s="58"/>
+      <c r="AF13" s="58"/>
+      <c r="AG13" s="58"/>
+      <c r="AH13" s="58"/>
+      <c r="AI13" s="58"/>
+      <c r="AJ13" s="58"/>
+      <c r="AK13" s="58"/>
+      <c r="AL13" s="58"/>
+      <c r="AM13" s="58"/>
+      <c r="AN13" s="58"/>
+      <c r="AO13" s="58"/>
+      <c r="AP13" s="58"/>
+      <c r="AQ13" s="58"/>
+      <c r="AR13" s="58"/>
+      <c r="AS13" s="58"/>
+      <c r="AT13" s="58"/>
+      <c r="AU13" s="58"/>
+      <c r="AV13" s="58"/>
+      <c r="AW13" s="58"/>
+      <c r="AX13" s="58"/>
+      <c r="AY13" s="58"/>
+      <c r="AZ13" s="58"/>
+      <c r="BA13" s="58"/>
+      <c r="BB13" s="58"/>
+      <c r="BC13" s="58"/>
+      <c r="BD13" s="58"/>
     </row>
     <row r="14" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
@@ -2105,55 +2105,55 @@
       <c r="G14" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H14" s="69"/>
-      <c r="I14" s="69"/>
-      <c r="J14" s="69"/>
-      <c r="K14" s="69"/>
-      <c r="L14" s="69"/>
-      <c r="M14" s="69"/>
-      <c r="N14" s="69"/>
-      <c r="O14" s="69"/>
-      <c r="P14" s="69"/>
-      <c r="Q14" s="69"/>
-      <c r="R14" s="69"/>
-      <c r="S14" s="69"/>
-      <c r="T14" s="69"/>
-      <c r="U14" s="69"/>
-      <c r="V14" s="69"/>
-      <c r="W14" s="69"/>
-      <c r="X14" s="69"/>
-      <c r="Y14" s="69"/>
-      <c r="Z14" s="69"/>
-      <c r="AA14" s="69"/>
-      <c r="AB14" s="69"/>
-      <c r="AC14" s="69"/>
-      <c r="AD14" s="69"/>
-      <c r="AE14" s="69"/>
-      <c r="AF14" s="69"/>
-      <c r="AG14" s="69"/>
-      <c r="AH14" s="69"/>
-      <c r="AI14" s="69"/>
-      <c r="AJ14" s="69"/>
-      <c r="AK14" s="69"/>
-      <c r="AL14" s="69"/>
-      <c r="AM14" s="69"/>
-      <c r="AN14" s="69"/>
-      <c r="AO14" s="69"/>
-      <c r="AP14" s="69"/>
-      <c r="AQ14" s="69"/>
-      <c r="AR14" s="69"/>
-      <c r="AS14" s="69"/>
-      <c r="AT14" s="69"/>
-      <c r="AU14" s="69"/>
-      <c r="AV14" s="69"/>
-      <c r="AW14" s="69"/>
-      <c r="AX14" s="69"/>
-      <c r="AY14" s="69"/>
-      <c r="AZ14" s="69"/>
-      <c r="BA14" s="69"/>
-      <c r="BB14" s="69"/>
-      <c r="BC14" s="69"/>
-      <c r="BD14" s="69"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="58"/>
+      <c r="Q14" s="58"/>
+      <c r="R14" s="58"/>
+      <c r="S14" s="58"/>
+      <c r="T14" s="58"/>
+      <c r="U14" s="58"/>
+      <c r="V14" s="58"/>
+      <c r="W14" s="58"/>
+      <c r="X14" s="58"/>
+      <c r="Y14" s="58"/>
+      <c r="Z14" s="58"/>
+      <c r="AA14" s="58"/>
+      <c r="AB14" s="58"/>
+      <c r="AC14" s="58"/>
+      <c r="AD14" s="58"/>
+      <c r="AE14" s="58"/>
+      <c r="AF14" s="58"/>
+      <c r="AG14" s="58"/>
+      <c r="AH14" s="58"/>
+      <c r="AI14" s="58"/>
+      <c r="AJ14" s="58"/>
+      <c r="AK14" s="58"/>
+      <c r="AL14" s="58"/>
+      <c r="AM14" s="58"/>
+      <c r="AN14" s="58"/>
+      <c r="AO14" s="58"/>
+      <c r="AP14" s="58"/>
+      <c r="AQ14" s="58"/>
+      <c r="AR14" s="58"/>
+      <c r="AS14" s="58"/>
+      <c r="AT14" s="58"/>
+      <c r="AU14" s="58"/>
+      <c r="AV14" s="58"/>
+      <c r="AW14" s="58"/>
+      <c r="AX14" s="58"/>
+      <c r="AY14" s="58"/>
+      <c r="AZ14" s="58"/>
+      <c r="BA14" s="58"/>
+      <c r="BB14" s="58"/>
+      <c r="BC14" s="58"/>
+      <c r="BD14" s="58"/>
     </row>
     <row r="15" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="s">
@@ -2177,55 +2177,55 @@
       <c r="G15" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H15" s="69"/>
-      <c r="I15" s="69"/>
-      <c r="J15" s="69"/>
-      <c r="K15" s="69"/>
-      <c r="L15" s="69"/>
-      <c r="M15" s="69"/>
-      <c r="N15" s="69"/>
-      <c r="O15" s="69"/>
-      <c r="P15" s="69"/>
-      <c r="Q15" s="69"/>
-      <c r="R15" s="69"/>
-      <c r="S15" s="69"/>
-      <c r="T15" s="69"/>
-      <c r="U15" s="69"/>
-      <c r="V15" s="69"/>
-      <c r="W15" s="69"/>
-      <c r="X15" s="69"/>
-      <c r="Y15" s="69"/>
-      <c r="Z15" s="69"/>
-      <c r="AA15" s="69"/>
-      <c r="AB15" s="69"/>
-      <c r="AC15" s="69"/>
-      <c r="AD15" s="69"/>
-      <c r="AE15" s="69"/>
-      <c r="AF15" s="69"/>
-      <c r="AG15" s="69"/>
-      <c r="AH15" s="69"/>
-      <c r="AI15" s="69"/>
-      <c r="AJ15" s="69"/>
-      <c r="AK15" s="69"/>
-      <c r="AL15" s="69"/>
-      <c r="AM15" s="69"/>
-      <c r="AN15" s="69"/>
-      <c r="AO15" s="69"/>
-      <c r="AP15" s="69"/>
-      <c r="AQ15" s="69"/>
-      <c r="AR15" s="69"/>
-      <c r="AS15" s="69"/>
-      <c r="AT15" s="69"/>
-      <c r="AU15" s="69"/>
-      <c r="AV15" s="69"/>
-      <c r="AW15" s="69"/>
-      <c r="AX15" s="69"/>
-      <c r="AY15" s="69"/>
-      <c r="AZ15" s="69"/>
-      <c r="BA15" s="69"/>
-      <c r="BB15" s="69"/>
-      <c r="BC15" s="69"/>
-      <c r="BD15" s="69"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="58"/>
+      <c r="N15" s="58"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="58"/>
+      <c r="Q15" s="58"/>
+      <c r="R15" s="58"/>
+      <c r="S15" s="58"/>
+      <c r="T15" s="58"/>
+      <c r="U15" s="58"/>
+      <c r="V15" s="58"/>
+      <c r="W15" s="58"/>
+      <c r="X15" s="58"/>
+      <c r="Y15" s="58"/>
+      <c r="Z15" s="58"/>
+      <c r="AA15" s="58"/>
+      <c r="AB15" s="58"/>
+      <c r="AC15" s="58"/>
+      <c r="AD15" s="58"/>
+      <c r="AE15" s="58"/>
+      <c r="AF15" s="58"/>
+      <c r="AG15" s="58"/>
+      <c r="AH15" s="58"/>
+      <c r="AI15" s="58"/>
+      <c r="AJ15" s="58"/>
+      <c r="AK15" s="58"/>
+      <c r="AL15" s="58"/>
+      <c r="AM15" s="58"/>
+      <c r="AN15" s="58"/>
+      <c r="AO15" s="58"/>
+      <c r="AP15" s="58"/>
+      <c r="AQ15" s="58"/>
+      <c r="AR15" s="58"/>
+      <c r="AS15" s="58"/>
+      <c r="AT15" s="58"/>
+      <c r="AU15" s="58"/>
+      <c r="AV15" s="58"/>
+      <c r="AW15" s="58"/>
+      <c r="AX15" s="58"/>
+      <c r="AY15" s="58"/>
+      <c r="AZ15" s="58"/>
+      <c r="BA15" s="58"/>
+      <c r="BB15" s="58"/>
+      <c r="BC15" s="58"/>
+      <c r="BD15" s="58"/>
     </row>
     <row r="16" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
@@ -2249,55 +2249,55 @@
       <c r="G16" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H16" s="69"/>
-      <c r="I16" s="69"/>
-      <c r="J16" s="69"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="69"/>
-      <c r="N16" s="69"/>
-      <c r="O16" s="69"/>
-      <c r="P16" s="69"/>
-      <c r="Q16" s="69"/>
-      <c r="R16" s="69"/>
-      <c r="S16" s="69"/>
-      <c r="T16" s="69"/>
-      <c r="U16" s="69"/>
-      <c r="V16" s="69"/>
-      <c r="W16" s="69"/>
-      <c r="X16" s="69"/>
-      <c r="Y16" s="69"/>
-      <c r="Z16" s="69"/>
-      <c r="AA16" s="69"/>
-      <c r="AB16" s="69"/>
-      <c r="AC16" s="69"/>
-      <c r="AD16" s="69"/>
-      <c r="AE16" s="69"/>
-      <c r="AF16" s="69"/>
-      <c r="AG16" s="69"/>
-      <c r="AH16" s="69"/>
-      <c r="AI16" s="69"/>
-      <c r="AJ16" s="69"/>
-      <c r="AK16" s="69"/>
-      <c r="AL16" s="69"/>
-      <c r="AM16" s="69"/>
-      <c r="AN16" s="69"/>
-      <c r="AO16" s="69"/>
-      <c r="AP16" s="69"/>
-      <c r="AQ16" s="69"/>
-      <c r="AR16" s="69"/>
-      <c r="AS16" s="69"/>
-      <c r="AT16" s="69"/>
-      <c r="AU16" s="69"/>
-      <c r="AV16" s="69"/>
-      <c r="AW16" s="69"/>
-      <c r="AX16" s="69"/>
-      <c r="AY16" s="69"/>
-      <c r="AZ16" s="69"/>
-      <c r="BA16" s="69"/>
-      <c r="BB16" s="69"/>
-      <c r="BC16" s="69"/>
-      <c r="BD16" s="69"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="58"/>
+      <c r="N16" s="58"/>
+      <c r="O16" s="58"/>
+      <c r="P16" s="58"/>
+      <c r="Q16" s="58"/>
+      <c r="R16" s="58"/>
+      <c r="S16" s="58"/>
+      <c r="T16" s="58"/>
+      <c r="U16" s="58"/>
+      <c r="V16" s="58"/>
+      <c r="W16" s="58"/>
+      <c r="X16" s="58"/>
+      <c r="Y16" s="58"/>
+      <c r="Z16" s="58"/>
+      <c r="AA16" s="58"/>
+      <c r="AB16" s="58"/>
+      <c r="AC16" s="58"/>
+      <c r="AD16" s="58"/>
+      <c r="AE16" s="58"/>
+      <c r="AF16" s="58"/>
+      <c r="AG16" s="58"/>
+      <c r="AH16" s="58"/>
+      <c r="AI16" s="58"/>
+      <c r="AJ16" s="58"/>
+      <c r="AK16" s="58"/>
+      <c r="AL16" s="58"/>
+      <c r="AM16" s="58"/>
+      <c r="AN16" s="58"/>
+      <c r="AO16" s="58"/>
+      <c r="AP16" s="58"/>
+      <c r="AQ16" s="58"/>
+      <c r="AR16" s="58"/>
+      <c r="AS16" s="58"/>
+      <c r="AT16" s="58"/>
+      <c r="AU16" s="58"/>
+      <c r="AV16" s="58"/>
+      <c r="AW16" s="58"/>
+      <c r="AX16" s="58"/>
+      <c r="AY16" s="58"/>
+      <c r="AZ16" s="58"/>
+      <c r="BA16" s="58"/>
+      <c r="BB16" s="58"/>
+      <c r="BC16" s="58"/>
+      <c r="BD16" s="58"/>
     </row>
     <row r="17" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
@@ -2321,55 +2321,55 @@
       <c r="G17" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H17" s="69"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="69"/>
-      <c r="K17" s="69"/>
-      <c r="L17" s="69"/>
-      <c r="M17" s="69"/>
-      <c r="N17" s="69"/>
-      <c r="O17" s="69"/>
-      <c r="P17" s="69"/>
-      <c r="Q17" s="69"/>
-      <c r="R17" s="69"/>
-      <c r="S17" s="69"/>
-      <c r="T17" s="69"/>
-      <c r="U17" s="69"/>
-      <c r="V17" s="69"/>
-      <c r="W17" s="69"/>
-      <c r="X17" s="69"/>
-      <c r="Y17" s="69"/>
-      <c r="Z17" s="69"/>
-      <c r="AA17" s="69"/>
-      <c r="AB17" s="69"/>
-      <c r="AC17" s="69"/>
-      <c r="AD17" s="69"/>
-      <c r="AE17" s="69"/>
-      <c r="AF17" s="69"/>
-      <c r="AG17" s="69"/>
-      <c r="AH17" s="69"/>
-      <c r="AI17" s="69"/>
-      <c r="AJ17" s="69"/>
-      <c r="AK17" s="69"/>
-      <c r="AL17" s="69"/>
-      <c r="AM17" s="69"/>
-      <c r="AN17" s="69"/>
-      <c r="AO17" s="69"/>
-      <c r="AP17" s="69"/>
-      <c r="AQ17" s="69"/>
-      <c r="AR17" s="69"/>
-      <c r="AS17" s="69"/>
-      <c r="AT17" s="69"/>
-      <c r="AU17" s="69"/>
-      <c r="AV17" s="69"/>
-      <c r="AW17" s="69"/>
-      <c r="AX17" s="69"/>
-      <c r="AY17" s="69"/>
-      <c r="AZ17" s="69"/>
-      <c r="BA17" s="69"/>
-      <c r="BB17" s="69"/>
-      <c r="BC17" s="69"/>
-      <c r="BD17" s="69"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="58"/>
+      <c r="N17" s="58"/>
+      <c r="O17" s="58"/>
+      <c r="P17" s="58"/>
+      <c r="Q17" s="58"/>
+      <c r="R17" s="58"/>
+      <c r="S17" s="58"/>
+      <c r="T17" s="58"/>
+      <c r="U17" s="58"/>
+      <c r="V17" s="58"/>
+      <c r="W17" s="58"/>
+      <c r="X17" s="58"/>
+      <c r="Y17" s="58"/>
+      <c r="Z17" s="58"/>
+      <c r="AA17" s="58"/>
+      <c r="AB17" s="58"/>
+      <c r="AC17" s="58"/>
+      <c r="AD17" s="58"/>
+      <c r="AE17" s="58"/>
+      <c r="AF17" s="58"/>
+      <c r="AG17" s="58"/>
+      <c r="AH17" s="58"/>
+      <c r="AI17" s="58"/>
+      <c r="AJ17" s="58"/>
+      <c r="AK17" s="58"/>
+      <c r="AL17" s="58"/>
+      <c r="AM17" s="58"/>
+      <c r="AN17" s="58"/>
+      <c r="AO17" s="58"/>
+      <c r="AP17" s="58"/>
+      <c r="AQ17" s="58"/>
+      <c r="AR17" s="58"/>
+      <c r="AS17" s="58"/>
+      <c r="AT17" s="58"/>
+      <c r="AU17" s="58"/>
+      <c r="AV17" s="58"/>
+      <c r="AW17" s="58"/>
+      <c r="AX17" s="58"/>
+      <c r="AY17" s="58"/>
+      <c r="AZ17" s="58"/>
+      <c r="BA17" s="58"/>
+      <c r="BB17" s="58"/>
+      <c r="BC17" s="58"/>
+      <c r="BD17" s="58"/>
     </row>
     <row r="18" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
@@ -2393,55 +2393,55 @@
       <c r="G18" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="69"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="69"/>
-      <c r="K18" s="69"/>
-      <c r="L18" s="69"/>
-      <c r="M18" s="69"/>
-      <c r="N18" s="69"/>
-      <c r="O18" s="69"/>
-      <c r="P18" s="69"/>
-      <c r="Q18" s="69"/>
-      <c r="R18" s="69"/>
-      <c r="S18" s="69"/>
-      <c r="T18" s="69"/>
-      <c r="U18" s="69"/>
-      <c r="V18" s="69"/>
-      <c r="W18" s="69"/>
-      <c r="X18" s="69"/>
-      <c r="Y18" s="69"/>
-      <c r="Z18" s="69"/>
-      <c r="AA18" s="69"/>
-      <c r="AB18" s="69"/>
-      <c r="AC18" s="69"/>
-      <c r="AD18" s="69"/>
-      <c r="AE18" s="69"/>
-      <c r="AF18" s="69"/>
-      <c r="AG18" s="69"/>
-      <c r="AH18" s="69"/>
-      <c r="AI18" s="69"/>
-      <c r="AJ18" s="69"/>
-      <c r="AK18" s="69"/>
-      <c r="AL18" s="69"/>
-      <c r="AM18" s="69"/>
-      <c r="AN18" s="69"/>
-      <c r="AO18" s="69"/>
-      <c r="AP18" s="69"/>
-      <c r="AQ18" s="69"/>
-      <c r="AR18" s="69"/>
-      <c r="AS18" s="69"/>
-      <c r="AT18" s="69"/>
-      <c r="AU18" s="69"/>
-      <c r="AV18" s="69"/>
-      <c r="AW18" s="69"/>
-      <c r="AX18" s="69"/>
-      <c r="AY18" s="69"/>
-      <c r="AZ18" s="69"/>
-      <c r="BA18" s="69"/>
-      <c r="BB18" s="69"/>
-      <c r="BC18" s="69"/>
-      <c r="BD18" s="69"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="58"/>
+      <c r="N18" s="58"/>
+      <c r="O18" s="58"/>
+      <c r="P18" s="58"/>
+      <c r="Q18" s="58"/>
+      <c r="R18" s="58"/>
+      <c r="S18" s="58"/>
+      <c r="T18" s="58"/>
+      <c r="U18" s="58"/>
+      <c r="V18" s="58"/>
+      <c r="W18" s="58"/>
+      <c r="X18" s="58"/>
+      <c r="Y18" s="58"/>
+      <c r="Z18" s="58"/>
+      <c r="AA18" s="58"/>
+      <c r="AB18" s="58"/>
+      <c r="AC18" s="58"/>
+      <c r="AD18" s="58"/>
+      <c r="AE18" s="58"/>
+      <c r="AF18" s="58"/>
+      <c r="AG18" s="58"/>
+      <c r="AH18" s="58"/>
+      <c r="AI18" s="58"/>
+      <c r="AJ18" s="58"/>
+      <c r="AK18" s="58"/>
+      <c r="AL18" s="58"/>
+      <c r="AM18" s="58"/>
+      <c r="AN18" s="58"/>
+      <c r="AO18" s="58"/>
+      <c r="AP18" s="58"/>
+      <c r="AQ18" s="58"/>
+      <c r="AR18" s="58"/>
+      <c r="AS18" s="58"/>
+      <c r="AT18" s="58"/>
+      <c r="AU18" s="58"/>
+      <c r="AV18" s="58"/>
+      <c r="AW18" s="58"/>
+      <c r="AX18" s="58"/>
+      <c r="AY18" s="58"/>
+      <c r="AZ18" s="58"/>
+      <c r="BA18" s="58"/>
+      <c r="BB18" s="58"/>
+      <c r="BC18" s="58"/>
+      <c r="BD18" s="58"/>
     </row>
     <row r="19" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
@@ -2465,55 +2465,55 @@
       <c r="G19" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H19" s="69"/>
-      <c r="I19" s="69"/>
-      <c r="J19" s="69"/>
-      <c r="K19" s="69"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="69"/>
-      <c r="N19" s="69"/>
-      <c r="O19" s="69"/>
-      <c r="P19" s="69"/>
-      <c r="Q19" s="69"/>
-      <c r="R19" s="69"/>
-      <c r="S19" s="69"/>
-      <c r="T19" s="69"/>
-      <c r="U19" s="69"/>
-      <c r="V19" s="69"/>
-      <c r="W19" s="69"/>
-      <c r="X19" s="69"/>
-      <c r="Y19" s="69"/>
-      <c r="Z19" s="69"/>
-      <c r="AA19" s="69"/>
-      <c r="AB19" s="69"/>
-      <c r="AC19" s="69"/>
-      <c r="AD19" s="69"/>
-      <c r="AE19" s="69"/>
-      <c r="AF19" s="69"/>
-      <c r="AG19" s="69"/>
-      <c r="AH19" s="69"/>
-      <c r="AI19" s="69"/>
-      <c r="AJ19" s="69"/>
-      <c r="AK19" s="69"/>
-      <c r="AL19" s="69"/>
-      <c r="AM19" s="69"/>
-      <c r="AN19" s="69"/>
-      <c r="AO19" s="69"/>
-      <c r="AP19" s="69"/>
-      <c r="AQ19" s="69"/>
-      <c r="AR19" s="69"/>
-      <c r="AS19" s="69"/>
-      <c r="AT19" s="69"/>
-      <c r="AU19" s="69"/>
-      <c r="AV19" s="69"/>
-      <c r="AW19" s="69"/>
-      <c r="AX19" s="69"/>
-      <c r="AY19" s="69"/>
-      <c r="AZ19" s="69"/>
-      <c r="BA19" s="69"/>
-      <c r="BB19" s="69"/>
-      <c r="BC19" s="69"/>
-      <c r="BD19" s="69"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="58"/>
+      <c r="P19" s="58"/>
+      <c r="Q19" s="58"/>
+      <c r="R19" s="58"/>
+      <c r="S19" s="58"/>
+      <c r="T19" s="58"/>
+      <c r="U19" s="58"/>
+      <c r="V19" s="58"/>
+      <c r="W19" s="58"/>
+      <c r="X19" s="58"/>
+      <c r="Y19" s="58"/>
+      <c r="Z19" s="58"/>
+      <c r="AA19" s="58"/>
+      <c r="AB19" s="58"/>
+      <c r="AC19" s="58"/>
+      <c r="AD19" s="58"/>
+      <c r="AE19" s="58"/>
+      <c r="AF19" s="58"/>
+      <c r="AG19" s="58"/>
+      <c r="AH19" s="58"/>
+      <c r="AI19" s="58"/>
+      <c r="AJ19" s="58"/>
+      <c r="AK19" s="58"/>
+      <c r="AL19" s="58"/>
+      <c r="AM19" s="58"/>
+      <c r="AN19" s="58"/>
+      <c r="AO19" s="58"/>
+      <c r="AP19" s="58"/>
+      <c r="AQ19" s="58"/>
+      <c r="AR19" s="58"/>
+      <c r="AS19" s="58"/>
+      <c r="AT19" s="58"/>
+      <c r="AU19" s="58"/>
+      <c r="AV19" s="58"/>
+      <c r="AW19" s="58"/>
+      <c r="AX19" s="58"/>
+      <c r="AY19" s="58"/>
+      <c r="AZ19" s="58"/>
+      <c r="BA19" s="58"/>
+      <c r="BB19" s="58"/>
+      <c r="BC19" s="58"/>
+      <c r="BD19" s="58"/>
     </row>
     <row r="20" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
@@ -2537,55 +2537,55 @@
       <c r="G20" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H20" s="69"/>
-      <c r="I20" s="69"/>
-      <c r="J20" s="69"/>
-      <c r="K20" s="69"/>
-      <c r="L20" s="69"/>
-      <c r="M20" s="69"/>
-      <c r="N20" s="69"/>
-      <c r="O20" s="69"/>
-      <c r="P20" s="69"/>
-      <c r="Q20" s="69"/>
-      <c r="R20" s="69"/>
-      <c r="S20" s="69"/>
-      <c r="T20" s="69"/>
-      <c r="U20" s="69"/>
-      <c r="V20" s="69"/>
-      <c r="W20" s="69"/>
-      <c r="X20" s="69"/>
-      <c r="Y20" s="69"/>
-      <c r="Z20" s="69"/>
-      <c r="AA20" s="69"/>
-      <c r="AB20" s="69"/>
-      <c r="AC20" s="69"/>
-      <c r="AD20" s="69"/>
-      <c r="AE20" s="69"/>
-      <c r="AF20" s="69"/>
-      <c r="AG20" s="69"/>
-      <c r="AH20" s="69"/>
-      <c r="AI20" s="69"/>
-      <c r="AJ20" s="69"/>
-      <c r="AK20" s="69"/>
-      <c r="AL20" s="69"/>
-      <c r="AM20" s="69"/>
-      <c r="AN20" s="69"/>
-      <c r="AO20" s="69"/>
-      <c r="AP20" s="69"/>
-      <c r="AQ20" s="69"/>
-      <c r="AR20" s="69"/>
-      <c r="AS20" s="69"/>
-      <c r="AT20" s="69"/>
-      <c r="AU20" s="69"/>
-      <c r="AV20" s="69"/>
-      <c r="AW20" s="69"/>
-      <c r="AX20" s="69"/>
-      <c r="AY20" s="69"/>
-      <c r="AZ20" s="69"/>
-      <c r="BA20" s="69"/>
-      <c r="BB20" s="69"/>
-      <c r="BC20" s="69"/>
-      <c r="BD20" s="69"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="58"/>
+      <c r="L20" s="58"/>
+      <c r="M20" s="58"/>
+      <c r="N20" s="58"/>
+      <c r="O20" s="58"/>
+      <c r="P20" s="58"/>
+      <c r="Q20" s="58"/>
+      <c r="R20" s="58"/>
+      <c r="S20" s="58"/>
+      <c r="T20" s="58"/>
+      <c r="U20" s="58"/>
+      <c r="V20" s="58"/>
+      <c r="W20" s="58"/>
+      <c r="X20" s="58"/>
+      <c r="Y20" s="58"/>
+      <c r="Z20" s="58"/>
+      <c r="AA20" s="58"/>
+      <c r="AB20" s="58"/>
+      <c r="AC20" s="58"/>
+      <c r="AD20" s="58"/>
+      <c r="AE20" s="58"/>
+      <c r="AF20" s="58"/>
+      <c r="AG20" s="58"/>
+      <c r="AH20" s="58"/>
+      <c r="AI20" s="58"/>
+      <c r="AJ20" s="58"/>
+      <c r="AK20" s="58"/>
+      <c r="AL20" s="58"/>
+      <c r="AM20" s="58"/>
+      <c r="AN20" s="58"/>
+      <c r="AO20" s="58"/>
+      <c r="AP20" s="58"/>
+      <c r="AQ20" s="58"/>
+      <c r="AR20" s="58"/>
+      <c r="AS20" s="58"/>
+      <c r="AT20" s="58"/>
+      <c r="AU20" s="58"/>
+      <c r="AV20" s="58"/>
+      <c r="AW20" s="58"/>
+      <c r="AX20" s="58"/>
+      <c r="AY20" s="58"/>
+      <c r="AZ20" s="58"/>
+      <c r="BA20" s="58"/>
+      <c r="BB20" s="58"/>
+      <c r="BC20" s="58"/>
+      <c r="BD20" s="58"/>
     </row>
     <row r="21" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="28" t="s">
@@ -2609,55 +2609,55 @@
       <c r="G21" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H21" s="69"/>
-      <c r="I21" s="69"/>
-      <c r="J21" s="69"/>
-      <c r="K21" s="69"/>
-      <c r="L21" s="69"/>
-      <c r="M21" s="69"/>
-      <c r="N21" s="69"/>
-      <c r="O21" s="69"/>
-      <c r="P21" s="69"/>
-      <c r="Q21" s="69"/>
-      <c r="R21" s="69"/>
-      <c r="S21" s="69"/>
-      <c r="T21" s="69"/>
-      <c r="U21" s="69"/>
-      <c r="V21" s="69"/>
-      <c r="W21" s="69"/>
-      <c r="X21" s="69"/>
-      <c r="Y21" s="69"/>
-      <c r="Z21" s="69"/>
-      <c r="AA21" s="69"/>
-      <c r="AB21" s="69"/>
-      <c r="AC21" s="69"/>
-      <c r="AD21" s="69"/>
-      <c r="AE21" s="69"/>
-      <c r="AF21" s="69"/>
-      <c r="AG21" s="69"/>
-      <c r="AH21" s="69"/>
-      <c r="AI21" s="69"/>
-      <c r="AJ21" s="69"/>
-      <c r="AK21" s="69"/>
-      <c r="AL21" s="69"/>
-      <c r="AM21" s="69"/>
-      <c r="AN21" s="69"/>
-      <c r="AO21" s="69"/>
-      <c r="AP21" s="69"/>
-      <c r="AQ21" s="69"/>
-      <c r="AR21" s="69"/>
-      <c r="AS21" s="69"/>
-      <c r="AT21" s="69"/>
-      <c r="AU21" s="69"/>
-      <c r="AV21" s="69"/>
-      <c r="AW21" s="69"/>
-      <c r="AX21" s="69"/>
-      <c r="AY21" s="69"/>
-      <c r="AZ21" s="69"/>
-      <c r="BA21" s="69"/>
-      <c r="BB21" s="69"/>
-      <c r="BC21" s="69"/>
-      <c r="BD21" s="69"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="58"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="58"/>
+      <c r="M21" s="58"/>
+      <c r="N21" s="58"/>
+      <c r="O21" s="58"/>
+      <c r="P21" s="58"/>
+      <c r="Q21" s="58"/>
+      <c r="R21" s="58"/>
+      <c r="S21" s="58"/>
+      <c r="T21" s="58"/>
+      <c r="U21" s="58"/>
+      <c r="V21" s="58"/>
+      <c r="W21" s="58"/>
+      <c r="X21" s="58"/>
+      <c r="Y21" s="58"/>
+      <c r="Z21" s="58"/>
+      <c r="AA21" s="58"/>
+      <c r="AB21" s="58"/>
+      <c r="AC21" s="58"/>
+      <c r="AD21" s="58"/>
+      <c r="AE21" s="58"/>
+      <c r="AF21" s="58"/>
+      <c r="AG21" s="58"/>
+      <c r="AH21" s="58"/>
+      <c r="AI21" s="58"/>
+      <c r="AJ21" s="58"/>
+      <c r="AK21" s="58"/>
+      <c r="AL21" s="58"/>
+      <c r="AM21" s="58"/>
+      <c r="AN21" s="58"/>
+      <c r="AO21" s="58"/>
+      <c r="AP21" s="58"/>
+      <c r="AQ21" s="58"/>
+      <c r="AR21" s="58"/>
+      <c r="AS21" s="58"/>
+      <c r="AT21" s="58"/>
+      <c r="AU21" s="58"/>
+      <c r="AV21" s="58"/>
+      <c r="AW21" s="58"/>
+      <c r="AX21" s="58"/>
+      <c r="AY21" s="58"/>
+      <c r="AZ21" s="58"/>
+      <c r="BA21" s="58"/>
+      <c r="BB21" s="58"/>
+      <c r="BC21" s="58"/>
+      <c r="BD21" s="58"/>
     </row>
     <row r="22" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A22" s="49"/>
@@ -2692,8 +2692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2704,15 +2704,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="67" t="s">
+      <c r="B1" s="67"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="66"/>
+      <c r="E1" s="68"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>

</xml_diff>

<commit_message>
Bot5 GUI --v 1.00 beta terminada
</commit_message>
<xml_diff>
--- a/CUENTAS DE CAJA IVSA.xlsx
+++ b/CUENTAS DE CAJA IVSA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="8_{E7FEFFEB-5A09-49B6-9D87-359617FDBFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92A107F5-2B0D-4DBE-981F-8B67329549D5}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="8_{E7FEFFEB-5A09-49B6-9D87-359617FDBFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6C60DD6-342B-477E-961B-8C580FD1872A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DISTRIBUIDORAS" sheetId="1" r:id="rId1"/>
@@ -1208,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2690,10 +2690,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2703,7 +2703,7 @@
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
@@ -2714,7 +2714,7 @@
       </c>
       <c r="E1" s="68"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -2729,7 +2729,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>6</v>
@@ -2743,7 +2743,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
@@ -2762,8 +2762,9 @@
       <c r="F4" s="57" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="14"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
@@ -2782,8 +2783,9 @@
       <c r="F5" s="57" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>7</v>
       </c>
@@ -2802,8 +2804,9 @@
       <c r="F6" s="57" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>7</v>
       </c>
@@ -2814,7 +2817,7 @@
         <v>101010133</v>
       </c>
       <c r="D7" s="14">
-        <v>101041012</v>
+        <v>101044012</v>
       </c>
       <c r="E7" s="52" t="s">
         <v>16</v>
@@ -2822,8 +2825,9 @@
       <c r="F7" s="57" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>18</v>
       </c>
@@ -2833,7 +2837,7 @@
       <c r="C8" s="17">
         <v>101010108</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="14">
         <v>101044032</v>
       </c>
       <c r="E8" s="53" t="s">
@@ -2842,8 +2846,9 @@
       <c r="F8" s="57" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
@@ -2862,8 +2867,9 @@
       <c r="F9" s="57" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
@@ -2882,8 +2888,9 @@
       <c r="F10" s="57" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>7</v>
       </c>
@@ -2902,8 +2909,9 @@
       <c r="F11" s="57" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>7</v>
       </c>
@@ -2922,8 +2930,9 @@
       <c r="F12" s="57" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>7</v>
       </c>
@@ -2942,8 +2951,9 @@
       <c r="F13" s="57" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>7</v>
       </c>
@@ -2962,8 +2972,9 @@
       <c r="F14" s="57" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>7</v>
       </c>
@@ -2982,8 +2993,9 @@
       <c r="F15" s="57" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>7</v>
       </c>
@@ -3002,8 +3014,9 @@
       <c r="F16" s="57" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>7</v>
       </c>
@@ -3022,8 +3035,9 @@
       <c r="F17" s="57" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>7</v>
       </c>
@@ -3042,8 +3056,9 @@
       <c r="F18" s="57" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>45</v>
       </c>
@@ -3062,8 +3077,9 @@
       <c r="F19" s="57" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>45</v>
       </c>
@@ -3082,8 +3098,9 @@
       <c r="F20" s="57" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="20" t="s">
         <v>50</v>
@@ -3095,7 +3112,7 @@
       <c r="E21" s="54"/>
       <c r="F21" s="57"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>7</v>
       </c>
@@ -3115,7 +3132,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>7</v>
       </c>
@@ -3135,7 +3152,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>7</v>
       </c>
@@ -3155,7 +3172,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>7</v>
       </c>
@@ -3175,7 +3192,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>18</v>
       </c>
@@ -3195,7 +3212,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>7</v>
       </c>
@@ -3215,7 +3232,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>7</v>
       </c>
@@ -3235,7 +3252,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>7</v>
       </c>
@@ -3255,7 +3272,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>7</v>
       </c>
@@ -3275,7 +3292,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>7</v>
       </c>
@@ -3295,7 +3312,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>7</v>
       </c>
@@ -3471,9 +3488,12 @@
       <formula>NOT(ISERROR(SEARCH("NO",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F20 F22:F38" xr:uid="{4DDA8D3B-06EF-40B5-B0B2-CBEB1310B5C8}">
       <formula1>"SI,NO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D20" xr:uid="{6CF02B72-412D-483F-BD39-02D1D4C5A24B}">
+      <formula1>"101044032,101044042,101044012,101044082,101044052,101044022,101044062,101044102,101041002,101041012,101041082,101044092,101044072,101044002"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.38" bottom="0.27" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bot5 GUI --v 1.00 beta terminada2
</commit_message>
<xml_diff>
--- a/CUENTAS DE CAJA IVSA.xlsx
+++ b/CUENTAS DE CAJA IVSA.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="8_{E7FEFFEB-5A09-49B6-9D87-359617FDBFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6C60DD6-342B-477E-961B-8C580FD1872A}"/>
+  <xr:revisionPtr revIDLastSave="237" documentId="8_{E7FEFFEB-5A09-49B6-9D87-359617FDBFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F5410B9-5A30-4412-AD0A-992319B55787}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DISTRIBUIDORAS" sheetId="1" r:id="rId1"/>
     <sheet name="AGENCIAS" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -397,7 +398,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -617,19 +618,6 @@
       <right/>
       <top/>
       <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -693,9 +681,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -703,9 +688,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -756,15 +738,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -786,17 +762,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -807,6 +783,18 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -903,10 +891,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1208,16 +1192,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="50" customWidth="1"/>
-    <col min="2" max="2" width="47.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="30"/>
+    <col min="1" max="1" width="27.28515625" style="46" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1232,17 +1216,17 @@
       <c r="E1" s="62"/>
     </row>
     <row r="2" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31" t="s">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="30" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="59" t="s">
@@ -1252,1415 +1236,1397 @@
         <v>85</v>
       </c>
       <c r="H2" s="65"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="58"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
-      <c r="W2" s="58"/>
-      <c r="X2" s="58"/>
-      <c r="Y2" s="58"/>
-      <c r="Z2" s="58"/>
-      <c r="AA2" s="58"/>
-      <c r="AB2" s="58"/>
-      <c r="AC2" s="58"/>
-      <c r="AD2" s="58"/>
-      <c r="AE2" s="58"/>
-      <c r="AF2" s="58"/>
-      <c r="AG2" s="58"/>
-      <c r="AH2" s="58"/>
-      <c r="AI2" s="58"/>
-      <c r="AJ2" s="58"/>
-      <c r="AK2" s="58"/>
-      <c r="AL2" s="58"/>
-      <c r="AM2" s="58"/>
-      <c r="AN2" s="58"/>
-      <c r="AO2" s="58"/>
-      <c r="AP2" s="58"/>
-      <c r="AQ2" s="58"/>
-      <c r="AR2" s="58"/>
-      <c r="AS2" s="58"/>
-      <c r="AT2" s="58"/>
-      <c r="AU2" s="58"/>
-      <c r="AV2" s="58"/>
-      <c r="AW2" s="58"/>
-      <c r="AX2" s="58"/>
-      <c r="AY2" s="58"/>
-      <c r="AZ2" s="58"/>
-      <c r="BA2" s="58"/>
-      <c r="BB2" s="58"/>
-      <c r="BC2" s="58"/>
-      <c r="BD2" s="58"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="54"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="54"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
+      <c r="AF2" s="54"/>
+      <c r="AG2" s="54"/>
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="54"/>
+      <c r="AJ2" s="54"/>
+      <c r="AK2" s="54"/>
+      <c r="AL2" s="54"/>
+      <c r="AM2" s="54"/>
+      <c r="AN2" s="54"/>
+      <c r="AO2" s="54"/>
+      <c r="AP2" s="54"/>
+      <c r="AQ2" s="54"/>
+      <c r="AR2" s="54"/>
+      <c r="AS2" s="54"/>
+      <c r="AT2" s="54"/>
+      <c r="AU2" s="54"/>
+      <c r="AV2" s="54"/>
+      <c r="AW2" s="54"/>
+      <c r="AX2" s="54"/>
+      <c r="AY2" s="54"/>
+      <c r="AZ2" s="54"/>
+      <c r="BA2" s="54"/>
+      <c r="BB2" s="54"/>
+      <c r="BC2" s="54"/>
+      <c r="BD2" s="54"/>
     </row>
     <row r="3" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34"/>
-      <c r="B3" s="35" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="34">
         <v>101010101</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
       <c r="F3" s="59"/>
       <c r="G3" s="64"/>
       <c r="H3" s="65"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="58"/>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="58"/>
-      <c r="T3" s="58"/>
-      <c r="U3" s="58"/>
-      <c r="V3" s="58"/>
-      <c r="W3" s="58"/>
-      <c r="X3" s="58"/>
-      <c r="Y3" s="58"/>
-      <c r="Z3" s="58"/>
-      <c r="AA3" s="58"/>
-      <c r="AB3" s="58"/>
-      <c r="AC3" s="58"/>
-      <c r="AD3" s="58"/>
-      <c r="AE3" s="58"/>
-      <c r="AF3" s="58"/>
-      <c r="AG3" s="58"/>
-      <c r="AH3" s="58"/>
-      <c r="AI3" s="58"/>
-      <c r="AJ3" s="58"/>
-      <c r="AK3" s="58"/>
-      <c r="AL3" s="58"/>
-      <c r="AM3" s="58"/>
-      <c r="AN3" s="58"/>
-      <c r="AO3" s="58"/>
-      <c r="AP3" s="58"/>
-      <c r="AQ3" s="58"/>
-      <c r="AR3" s="58"/>
-      <c r="AS3" s="58"/>
-      <c r="AT3" s="58"/>
-      <c r="AU3" s="58"/>
-      <c r="AV3" s="58"/>
-      <c r="AW3" s="58"/>
-      <c r="AX3" s="58"/>
-      <c r="AY3" s="58"/>
-      <c r="AZ3" s="58"/>
-      <c r="BA3" s="58"/>
-      <c r="BB3" s="58"/>
-      <c r="BC3" s="58"/>
-      <c r="BD3" s="58"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="54"/>
+      <c r="AB3" s="54"/>
+      <c r="AC3" s="54"/>
+      <c r="AD3" s="54"/>
+      <c r="AE3" s="54"/>
+      <c r="AF3" s="54"/>
+      <c r="AG3" s="54"/>
+      <c r="AH3" s="54"/>
+      <c r="AI3" s="54"/>
+      <c r="AJ3" s="54"/>
+      <c r="AK3" s="54"/>
+      <c r="AL3" s="54"/>
+      <c r="AM3" s="54"/>
+      <c r="AN3" s="54"/>
+      <c r="AO3" s="54"/>
+      <c r="AP3" s="54"/>
+      <c r="AQ3" s="54"/>
+      <c r="AR3" s="54"/>
+      <c r="AS3" s="54"/>
+      <c r="AT3" s="54"/>
+      <c r="AU3" s="54"/>
+      <c r="AV3" s="54"/>
+      <c r="AW3" s="54"/>
+      <c r="AX3" s="54"/>
+      <c r="AY3" s="54"/>
+      <c r="AZ3" s="54"/>
+      <c r="BA3" s="54"/>
+      <c r="BB3" s="54"/>
+      <c r="BC3" s="54"/>
+      <c r="BD3" s="54"/>
     </row>
     <row r="4" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="38">
         <v>101010102</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="22">
         <v>101020101</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="41">
+      <c r="F4" s="58">
         <v>101044012</v>
       </c>
-      <c r="G4" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="58"/>
-      <c r="P4" s="58"/>
-      <c r="Q4" s="58"/>
-      <c r="R4" s="58"/>
-      <c r="S4" s="58"/>
-      <c r="T4" s="58"/>
-      <c r="U4" s="58"/>
-      <c r="V4" s="58"/>
-      <c r="W4" s="58"/>
-      <c r="X4" s="58"/>
-      <c r="Y4" s="58"/>
-      <c r="Z4" s="58"/>
-      <c r="AA4" s="58"/>
-      <c r="AB4" s="58"/>
-      <c r="AC4" s="58"/>
-      <c r="AD4" s="58"/>
-      <c r="AE4" s="58"/>
-      <c r="AF4" s="58"/>
-      <c r="AG4" s="58"/>
-      <c r="AH4" s="58"/>
-      <c r="AI4" s="58"/>
-      <c r="AJ4" s="58"/>
-      <c r="AK4" s="58"/>
-      <c r="AL4" s="58"/>
-      <c r="AM4" s="58"/>
-      <c r="AN4" s="58"/>
-      <c r="AO4" s="58"/>
-      <c r="AP4" s="58"/>
-      <c r="AQ4" s="58"/>
-      <c r="AR4" s="58"/>
-      <c r="AS4" s="58"/>
-      <c r="AT4" s="58"/>
-      <c r="AU4" s="58"/>
-      <c r="AV4" s="58"/>
-      <c r="AW4" s="58"/>
-      <c r="AX4" s="58"/>
-      <c r="AY4" s="58"/>
-      <c r="AZ4" s="58"/>
-      <c r="BA4" s="58"/>
-      <c r="BB4" s="58"/>
-      <c r="BC4" s="58"/>
-      <c r="BD4" s="58"/>
+      <c r="G4" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="54"/>
+      <c r="S4" s="54"/>
+      <c r="T4" s="54"/>
+      <c r="U4" s="54"/>
+      <c r="V4" s="54"/>
+      <c r="W4" s="54"/>
+      <c r="X4" s="54"/>
+      <c r="Y4" s="54"/>
+      <c r="Z4" s="54"/>
+      <c r="AA4" s="54"/>
+      <c r="AB4" s="54"/>
+      <c r="AC4" s="54"/>
+      <c r="AD4" s="54"/>
+      <c r="AE4" s="54"/>
+      <c r="AF4" s="54"/>
+      <c r="AG4" s="54"/>
+      <c r="AH4" s="54"/>
+      <c r="AI4" s="54"/>
+      <c r="AJ4" s="54"/>
+      <c r="AK4" s="54"/>
+      <c r="AL4" s="54"/>
+      <c r="AM4" s="54"/>
+      <c r="AN4" s="54"/>
+      <c r="AO4" s="54"/>
+      <c r="AP4" s="54"/>
+      <c r="AQ4" s="54"/>
+      <c r="AR4" s="54"/>
+      <c r="AS4" s="54"/>
+      <c r="AT4" s="54"/>
+      <c r="AU4" s="54"/>
+      <c r="AV4" s="54"/>
+      <c r="AW4" s="54"/>
+      <c r="AX4" s="54"/>
+      <c r="AY4" s="54"/>
+      <c r="AZ4" s="54"/>
+      <c r="BA4" s="54"/>
+      <c r="BB4" s="54"/>
+      <c r="BC4" s="54"/>
+      <c r="BD4" s="54"/>
     </row>
     <row r="5" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="40">
+      <c r="C5" s="38">
         <v>101010106</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="22">
         <v>101020101</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="43">
+      <c r="F5" s="58">
         <v>101044012</v>
       </c>
-      <c r="G5" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="58"/>
-      <c r="Q5" s="58"/>
-      <c r="R5" s="58"/>
-      <c r="S5" s="58"/>
-      <c r="T5" s="58"/>
-      <c r="U5" s="58"/>
-      <c r="V5" s="58"/>
-      <c r="W5" s="58"/>
-      <c r="X5" s="58"/>
-      <c r="Y5" s="58"/>
-      <c r="Z5" s="58"/>
-      <c r="AA5" s="58"/>
-      <c r="AB5" s="58"/>
-      <c r="AC5" s="58"/>
-      <c r="AD5" s="58"/>
-      <c r="AE5" s="58"/>
-      <c r="AF5" s="58"/>
-      <c r="AG5" s="58"/>
-      <c r="AH5" s="58"/>
-      <c r="AI5" s="58"/>
-      <c r="AJ5" s="58"/>
-      <c r="AK5" s="58"/>
-      <c r="AL5" s="58"/>
-      <c r="AM5" s="58"/>
-      <c r="AN5" s="58"/>
-      <c r="AO5" s="58"/>
-      <c r="AP5" s="58"/>
-      <c r="AQ5" s="58"/>
-      <c r="AR5" s="58"/>
-      <c r="AS5" s="58"/>
-      <c r="AT5" s="58"/>
-      <c r="AU5" s="58"/>
-      <c r="AV5" s="58"/>
-      <c r="AW5" s="58"/>
-      <c r="AX5" s="58"/>
-      <c r="AY5" s="58"/>
-      <c r="AZ5" s="58"/>
-      <c r="BA5" s="58"/>
-      <c r="BB5" s="58"/>
-      <c r="BC5" s="58"/>
-      <c r="BD5" s="58"/>
+      <c r="G5" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="54"/>
+      <c r="S5" s="54"/>
+      <c r="T5" s="54"/>
+      <c r="U5" s="54"/>
+      <c r="V5" s="54"/>
+      <c r="W5" s="54"/>
+      <c r="X5" s="54"/>
+      <c r="Y5" s="54"/>
+      <c r="Z5" s="54"/>
+      <c r="AA5" s="54"/>
+      <c r="AB5" s="54"/>
+      <c r="AC5" s="54"/>
+      <c r="AD5" s="54"/>
+      <c r="AE5" s="54"/>
+      <c r="AF5" s="54"/>
+      <c r="AG5" s="54"/>
+      <c r="AH5" s="54"/>
+      <c r="AI5" s="54"/>
+      <c r="AJ5" s="54"/>
+      <c r="AK5" s="54"/>
+      <c r="AL5" s="54"/>
+      <c r="AM5" s="54"/>
+      <c r="AN5" s="54"/>
+      <c r="AO5" s="54"/>
+      <c r="AP5" s="54"/>
+      <c r="AQ5" s="54"/>
+      <c r="AR5" s="54"/>
+      <c r="AS5" s="54"/>
+      <c r="AT5" s="54"/>
+      <c r="AU5" s="54"/>
+      <c r="AV5" s="54"/>
+      <c r="AW5" s="54"/>
+      <c r="AX5" s="54"/>
+      <c r="AY5" s="54"/>
+      <c r="AZ5" s="54"/>
+      <c r="BA5" s="54"/>
+      <c r="BB5" s="54"/>
+      <c r="BC5" s="54"/>
+      <c r="BD5" s="54"/>
     </row>
     <row r="6" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="38">
         <v>101010107</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="22">
         <v>101020101</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="43">
+      <c r="F6" s="58">
         <v>101044032</v>
       </c>
-      <c r="G6" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="58"/>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="58"/>
-      <c r="R6" s="58"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="58"/>
-      <c r="U6" s="58"/>
-      <c r="V6" s="58"/>
-      <c r="W6" s="58"/>
-      <c r="X6" s="58"/>
-      <c r="Y6" s="58"/>
-      <c r="Z6" s="58"/>
-      <c r="AA6" s="58"/>
-      <c r="AB6" s="58"/>
-      <c r="AC6" s="58"/>
-      <c r="AD6" s="58"/>
-      <c r="AE6" s="58"/>
-      <c r="AF6" s="58"/>
-      <c r="AG6" s="58"/>
-      <c r="AH6" s="58"/>
-      <c r="AI6" s="58"/>
-      <c r="AJ6" s="58"/>
-      <c r="AK6" s="58"/>
-      <c r="AL6" s="58"/>
-      <c r="AM6" s="58"/>
-      <c r="AN6" s="58"/>
-      <c r="AO6" s="58"/>
-      <c r="AP6" s="58"/>
-      <c r="AQ6" s="58"/>
-      <c r="AR6" s="58"/>
-      <c r="AS6" s="58"/>
-      <c r="AT6" s="58"/>
-      <c r="AU6" s="58"/>
-      <c r="AV6" s="58"/>
-      <c r="AW6" s="58"/>
-      <c r="AX6" s="58"/>
-      <c r="AY6" s="58"/>
-      <c r="AZ6" s="58"/>
-      <c r="BA6" s="58"/>
-      <c r="BB6" s="58"/>
-      <c r="BC6" s="58"/>
-      <c r="BD6" s="58"/>
+      <c r="G6" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="54"/>
+      <c r="S6" s="54"/>
+      <c r="T6" s="54"/>
+      <c r="U6" s="54"/>
+      <c r="V6" s="54"/>
+      <c r="W6" s="54"/>
+      <c r="X6" s="54"/>
+      <c r="Y6" s="54"/>
+      <c r="Z6" s="54"/>
+      <c r="AA6" s="54"/>
+      <c r="AB6" s="54"/>
+      <c r="AC6" s="54"/>
+      <c r="AD6" s="54"/>
+      <c r="AE6" s="54"/>
+      <c r="AF6" s="54"/>
+      <c r="AG6" s="54"/>
+      <c r="AH6" s="54"/>
+      <c r="AI6" s="54"/>
+      <c r="AJ6" s="54"/>
+      <c r="AK6" s="54"/>
+      <c r="AL6" s="54"/>
+      <c r="AM6" s="54"/>
+      <c r="AN6" s="54"/>
+      <c r="AO6" s="54"/>
+      <c r="AP6" s="54"/>
+      <c r="AQ6" s="54"/>
+      <c r="AR6" s="54"/>
+      <c r="AS6" s="54"/>
+      <c r="AT6" s="54"/>
+      <c r="AU6" s="54"/>
+      <c r="AV6" s="54"/>
+      <c r="AW6" s="54"/>
+      <c r="AX6" s="54"/>
+      <c r="AY6" s="54"/>
+      <c r="AZ6" s="54"/>
+      <c r="BA6" s="54"/>
+      <c r="BB6" s="54"/>
+      <c r="BC6" s="54"/>
+      <c r="BD6" s="54"/>
     </row>
     <row r="7" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="40">
+      <c r="C7" s="38">
         <v>101010109</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="22">
         <v>101020101</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="58">
         <v>101044072</v>
       </c>
-      <c r="G7" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="58"/>
-      <c r="R7" s="58"/>
-      <c r="S7" s="58"/>
-      <c r="T7" s="58"/>
-      <c r="U7" s="58"/>
-      <c r="V7" s="58"/>
-      <c r="W7" s="58"/>
-      <c r="X7" s="58"/>
-      <c r="Y7" s="58"/>
-      <c r="Z7" s="58"/>
-      <c r="AA7" s="58"/>
-      <c r="AB7" s="58"/>
-      <c r="AC7" s="58"/>
-      <c r="AD7" s="58"/>
-      <c r="AE7" s="58"/>
-      <c r="AF7" s="58"/>
-      <c r="AG7" s="58"/>
-      <c r="AH7" s="58"/>
-      <c r="AI7" s="58"/>
-      <c r="AJ7" s="58"/>
-      <c r="AK7" s="58"/>
-      <c r="AL7" s="58"/>
-      <c r="AM7" s="58"/>
-      <c r="AN7" s="58"/>
-      <c r="AO7" s="58"/>
-      <c r="AP7" s="58"/>
-      <c r="AQ7" s="58"/>
-      <c r="AR7" s="58"/>
-      <c r="AS7" s="58"/>
-      <c r="AT7" s="58"/>
-      <c r="AU7" s="58"/>
-      <c r="AV7" s="58"/>
-      <c r="AW7" s="58"/>
-      <c r="AX7" s="58"/>
-      <c r="AY7" s="58"/>
-      <c r="AZ7" s="58"/>
-      <c r="BA7" s="58"/>
-      <c r="BB7" s="58"/>
-      <c r="BC7" s="58"/>
-      <c r="BD7" s="58"/>
+      <c r="G7" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="54"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="54"/>
+      <c r="R7" s="54"/>
+      <c r="S7" s="54"/>
+      <c r="T7" s="54"/>
+      <c r="U7" s="54"/>
+      <c r="V7" s="54"/>
+      <c r="W7" s="54"/>
+      <c r="X7" s="54"/>
+      <c r="Y7" s="54"/>
+      <c r="Z7" s="54"/>
+      <c r="AA7" s="54"/>
+      <c r="AB7" s="54"/>
+      <c r="AC7" s="54"/>
+      <c r="AD7" s="54"/>
+      <c r="AE7" s="54"/>
+      <c r="AF7" s="54"/>
+      <c r="AG7" s="54"/>
+      <c r="AH7" s="54"/>
+      <c r="AI7" s="54"/>
+      <c r="AJ7" s="54"/>
+      <c r="AK7" s="54"/>
+      <c r="AL7" s="54"/>
+      <c r="AM7" s="54"/>
+      <c r="AN7" s="54"/>
+      <c r="AO7" s="54"/>
+      <c r="AP7" s="54"/>
+      <c r="AQ7" s="54"/>
+      <c r="AR7" s="54"/>
+      <c r="AS7" s="54"/>
+      <c r="AT7" s="54"/>
+      <c r="AU7" s="54"/>
+      <c r="AV7" s="54"/>
+      <c r="AW7" s="54"/>
+      <c r="AX7" s="54"/>
+      <c r="AY7" s="54"/>
+      <c r="AZ7" s="54"/>
+      <c r="BA7" s="54"/>
+      <c r="BB7" s="54"/>
+      <c r="BC7" s="54"/>
+      <c r="BD7" s="54"/>
     </row>
     <row r="8" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="40">
+      <c r="C8" s="38">
         <v>101010111</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="22">
         <v>101020101</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F8" s="58">
         <v>101044022</v>
       </c>
-      <c r="G8" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="58"/>
-      <c r="K8" s="58"/>
-      <c r="L8" s="58"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="58"/>
-      <c r="Q8" s="58"/>
-      <c r="R8" s="58"/>
-      <c r="S8" s="58"/>
-      <c r="T8" s="58"/>
-      <c r="U8" s="58"/>
-      <c r="V8" s="58"/>
-      <c r="W8" s="58"/>
-      <c r="X8" s="58"/>
-      <c r="Y8" s="58"/>
-      <c r="Z8" s="58"/>
-      <c r="AA8" s="58"/>
-      <c r="AB8" s="58"/>
-      <c r="AC8" s="58"/>
-      <c r="AD8" s="58"/>
-      <c r="AE8" s="58"/>
-      <c r="AF8" s="58"/>
-      <c r="AG8" s="58"/>
-      <c r="AH8" s="58"/>
-      <c r="AI8" s="58"/>
-      <c r="AJ8" s="58"/>
-      <c r="AK8" s="58"/>
-      <c r="AL8" s="58"/>
-      <c r="AM8" s="58"/>
-      <c r="AN8" s="58"/>
-      <c r="AO8" s="58"/>
-      <c r="AP8" s="58"/>
-      <c r="AQ8" s="58"/>
-      <c r="AR8" s="58"/>
-      <c r="AS8" s="58"/>
-      <c r="AT8" s="58"/>
-      <c r="AU8" s="58"/>
-      <c r="AV8" s="58"/>
-      <c r="AW8" s="58"/>
-      <c r="AX8" s="58"/>
-      <c r="AY8" s="58"/>
-      <c r="AZ8" s="58"/>
-      <c r="BA8" s="58"/>
-      <c r="BB8" s="58"/>
-      <c r="BC8" s="58"/>
-      <c r="BD8" s="58"/>
+      <c r="G8" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="54"/>
+      <c r="S8" s="54"/>
+      <c r="T8" s="54"/>
+      <c r="U8" s="54"/>
+      <c r="V8" s="54"/>
+      <c r="W8" s="54"/>
+      <c r="X8" s="54"/>
+      <c r="Y8" s="54"/>
+      <c r="Z8" s="54"/>
+      <c r="AA8" s="54"/>
+      <c r="AB8" s="54"/>
+      <c r="AC8" s="54"/>
+      <c r="AD8" s="54"/>
+      <c r="AE8" s="54"/>
+      <c r="AF8" s="54"/>
+      <c r="AG8" s="54"/>
+      <c r="AH8" s="54"/>
+      <c r="AI8" s="54"/>
+      <c r="AJ8" s="54"/>
+      <c r="AK8" s="54"/>
+      <c r="AL8" s="54"/>
+      <c r="AM8" s="54"/>
+      <c r="AN8" s="54"/>
+      <c r="AO8" s="54"/>
+      <c r="AP8" s="54"/>
+      <c r="AQ8" s="54"/>
+      <c r="AR8" s="54"/>
+      <c r="AS8" s="54"/>
+      <c r="AT8" s="54"/>
+      <c r="AU8" s="54"/>
+      <c r="AV8" s="54"/>
+      <c r="AW8" s="54"/>
+      <c r="AX8" s="54"/>
+      <c r="AY8" s="54"/>
+      <c r="AZ8" s="54"/>
+      <c r="BA8" s="54"/>
+      <c r="BB8" s="54"/>
+      <c r="BC8" s="54"/>
+      <c r="BD8" s="54"/>
     </row>
     <row r="9" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="40">
+      <c r="C9" s="38">
         <v>101010114</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="22">
         <v>101020101</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="43">
+      <c r="F9" s="58">
         <v>101044052</v>
       </c>
-      <c r="G9" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="58"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="58"/>
-      <c r="Q9" s="58"/>
-      <c r="R9" s="58"/>
-      <c r="S9" s="58"/>
-      <c r="T9" s="58"/>
-      <c r="U9" s="58"/>
-      <c r="V9" s="58"/>
-      <c r="W9" s="58"/>
-      <c r="X9" s="58"/>
-      <c r="Y9" s="58"/>
-      <c r="Z9" s="58"/>
-      <c r="AA9" s="58"/>
-      <c r="AB9" s="58"/>
-      <c r="AC9" s="58"/>
-      <c r="AD9" s="58"/>
-      <c r="AE9" s="58"/>
-      <c r="AF9" s="58"/>
-      <c r="AG9" s="58"/>
-      <c r="AH9" s="58"/>
-      <c r="AI9" s="58"/>
-      <c r="AJ9" s="58"/>
-      <c r="AK9" s="58"/>
-      <c r="AL9" s="58"/>
-      <c r="AM9" s="58"/>
-      <c r="AN9" s="58"/>
-      <c r="AO9" s="58"/>
-      <c r="AP9" s="58"/>
-      <c r="AQ9" s="58"/>
-      <c r="AR9" s="58"/>
-      <c r="AS9" s="58"/>
-      <c r="AT9" s="58"/>
-      <c r="AU9" s="58"/>
-      <c r="AV9" s="58"/>
-      <c r="AW9" s="58"/>
-      <c r="AX9" s="58"/>
-      <c r="AY9" s="58"/>
-      <c r="AZ9" s="58"/>
-      <c r="BA9" s="58"/>
-      <c r="BB9" s="58"/>
-      <c r="BC9" s="58"/>
-      <c r="BD9" s="58"/>
+      <c r="G9" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="54"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="54"/>
+      <c r="R9" s="54"/>
+      <c r="S9" s="54"/>
+      <c r="T9" s="54"/>
+      <c r="U9" s="54"/>
+      <c r="V9" s="54"/>
+      <c r="W9" s="54"/>
+      <c r="X9" s="54"/>
+      <c r="Y9" s="54"/>
+      <c r="Z9" s="54"/>
+      <c r="AA9" s="54"/>
+      <c r="AB9" s="54"/>
+      <c r="AC9" s="54"/>
+      <c r="AD9" s="54"/>
+      <c r="AE9" s="54"/>
+      <c r="AF9" s="54"/>
+      <c r="AG9" s="54"/>
+      <c r="AH9" s="54"/>
+      <c r="AI9" s="54"/>
+      <c r="AJ9" s="54"/>
+      <c r="AK9" s="54"/>
+      <c r="AL9" s="54"/>
+      <c r="AM9" s="54"/>
+      <c r="AN9" s="54"/>
+      <c r="AO9" s="54"/>
+      <c r="AP9" s="54"/>
+      <c r="AQ9" s="54"/>
+      <c r="AR9" s="54"/>
+      <c r="AS9" s="54"/>
+      <c r="AT9" s="54"/>
+      <c r="AU9" s="54"/>
+      <c r="AV9" s="54"/>
+      <c r="AW9" s="54"/>
+      <c r="AX9" s="54"/>
+      <c r="AY9" s="54"/>
+      <c r="AZ9" s="54"/>
+      <c r="BA9" s="54"/>
+      <c r="BB9" s="54"/>
+      <c r="BC9" s="54"/>
+      <c r="BD9" s="54"/>
     </row>
     <row r="10" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="40">
+      <c r="C10" s="38">
         <v>101010117</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="22">
         <v>101020101</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="58">
         <v>101044062</v>
       </c>
-      <c r="G10" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="58"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="58"/>
-      <c r="Q10" s="58"/>
-      <c r="R10" s="58"/>
-      <c r="S10" s="58"/>
-      <c r="T10" s="58"/>
-      <c r="U10" s="58"/>
-      <c r="V10" s="58"/>
-      <c r="W10" s="58"/>
-      <c r="X10" s="58"/>
-      <c r="Y10" s="58"/>
-      <c r="Z10" s="58"/>
-      <c r="AA10" s="58"/>
-      <c r="AB10" s="58"/>
-      <c r="AC10" s="58"/>
-      <c r="AD10" s="58"/>
-      <c r="AE10" s="58"/>
-      <c r="AF10" s="58"/>
-      <c r="AG10" s="58"/>
-      <c r="AH10" s="58"/>
-      <c r="AI10" s="58"/>
-      <c r="AJ10" s="58"/>
-      <c r="AK10" s="58"/>
-      <c r="AL10" s="58"/>
-      <c r="AM10" s="58"/>
-      <c r="AN10" s="58"/>
-      <c r="AO10" s="58"/>
-      <c r="AP10" s="58"/>
-      <c r="AQ10" s="58"/>
-      <c r="AR10" s="58"/>
-      <c r="AS10" s="58"/>
-      <c r="AT10" s="58"/>
-      <c r="AU10" s="58"/>
-      <c r="AV10" s="58"/>
-      <c r="AW10" s="58"/>
-      <c r="AX10" s="58"/>
-      <c r="AY10" s="58"/>
-      <c r="AZ10" s="58"/>
-      <c r="BA10" s="58"/>
-      <c r="BB10" s="58"/>
-      <c r="BC10" s="58"/>
-      <c r="BD10" s="58"/>
+      <c r="G10" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="54"/>
+      <c r="T10" s="54"/>
+      <c r="U10" s="54"/>
+      <c r="V10" s="54"/>
+      <c r="W10" s="54"/>
+      <c r="X10" s="54"/>
+      <c r="Y10" s="54"/>
+      <c r="Z10" s="54"/>
+      <c r="AA10" s="54"/>
+      <c r="AB10" s="54"/>
+      <c r="AC10" s="54"/>
+      <c r="AD10" s="54"/>
+      <c r="AE10" s="54"/>
+      <c r="AF10" s="54"/>
+      <c r="AG10" s="54"/>
+      <c r="AH10" s="54"/>
+      <c r="AI10" s="54"/>
+      <c r="AJ10" s="54"/>
+      <c r="AK10" s="54"/>
+      <c r="AL10" s="54"/>
+      <c r="AM10" s="54"/>
+      <c r="AN10" s="54"/>
+      <c r="AO10" s="54"/>
+      <c r="AP10" s="54"/>
+      <c r="AQ10" s="54"/>
+      <c r="AR10" s="54"/>
+      <c r="AS10" s="54"/>
+      <c r="AT10" s="54"/>
+      <c r="AU10" s="54"/>
+      <c r="AV10" s="54"/>
+      <c r="AW10" s="54"/>
+      <c r="AX10" s="54"/>
+      <c r="AY10" s="54"/>
+      <c r="AZ10" s="54"/>
+      <c r="BA10" s="54"/>
+      <c r="BB10" s="54"/>
+      <c r="BC10" s="54"/>
+      <c r="BD10" s="54"/>
     </row>
     <row r="11" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="38">
         <v>101010119</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="22">
         <v>101020101</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="43">
+      <c r="F11" s="58">
         <v>101044042</v>
       </c>
-      <c r="G11" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="58"/>
-      <c r="M11" s="58"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="58"/>
-      <c r="Q11" s="58"/>
-      <c r="R11" s="58"/>
-      <c r="S11" s="58"/>
-      <c r="T11" s="58"/>
-      <c r="U11" s="58"/>
-      <c r="V11" s="58"/>
-      <c r="W11" s="58"/>
-      <c r="X11" s="58"/>
-      <c r="Y11" s="58"/>
-      <c r="Z11" s="58"/>
-      <c r="AA11" s="58"/>
-      <c r="AB11" s="58"/>
-      <c r="AC11" s="58"/>
-      <c r="AD11" s="58"/>
-      <c r="AE11" s="58"/>
-      <c r="AF11" s="58"/>
-      <c r="AG11" s="58"/>
-      <c r="AH11" s="58"/>
-      <c r="AI11" s="58"/>
-      <c r="AJ11" s="58"/>
-      <c r="AK11" s="58"/>
-      <c r="AL11" s="58"/>
-      <c r="AM11" s="58"/>
-      <c r="AN11" s="58"/>
-      <c r="AO11" s="58"/>
-      <c r="AP11" s="58"/>
-      <c r="AQ11" s="58"/>
-      <c r="AR11" s="58"/>
-      <c r="AS11" s="58"/>
-      <c r="AT11" s="58"/>
-      <c r="AU11" s="58"/>
-      <c r="AV11" s="58"/>
-      <c r="AW11" s="58"/>
-      <c r="AX11" s="58"/>
-      <c r="AY11" s="58"/>
-      <c r="AZ11" s="58"/>
-      <c r="BA11" s="58"/>
-      <c r="BB11" s="58"/>
-      <c r="BC11" s="58"/>
-      <c r="BD11" s="58"/>
+      <c r="G11" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="54"/>
+      <c r="R11" s="54"/>
+      <c r="S11" s="54"/>
+      <c r="T11" s="54"/>
+      <c r="U11" s="54"/>
+      <c r="V11" s="54"/>
+      <c r="W11" s="54"/>
+      <c r="X11" s="54"/>
+      <c r="Y11" s="54"/>
+      <c r="Z11" s="54"/>
+      <c r="AA11" s="54"/>
+      <c r="AB11" s="54"/>
+      <c r="AC11" s="54"/>
+      <c r="AD11" s="54"/>
+      <c r="AE11" s="54"/>
+      <c r="AF11" s="54"/>
+      <c r="AG11" s="54"/>
+      <c r="AH11" s="54"/>
+      <c r="AI11" s="54"/>
+      <c r="AJ11" s="54"/>
+      <c r="AK11" s="54"/>
+      <c r="AL11" s="54"/>
+      <c r="AM11" s="54"/>
+      <c r="AN11" s="54"/>
+      <c r="AO11" s="54"/>
+      <c r="AP11" s="54"/>
+      <c r="AQ11" s="54"/>
+      <c r="AR11" s="54"/>
+      <c r="AS11" s="54"/>
+      <c r="AT11" s="54"/>
+      <c r="AU11" s="54"/>
+      <c r="AV11" s="54"/>
+      <c r="AW11" s="54"/>
+      <c r="AX11" s="54"/>
+      <c r="AY11" s="54"/>
+      <c r="AZ11" s="54"/>
+      <c r="BA11" s="54"/>
+      <c r="BB11" s="54"/>
+      <c r="BC11" s="54"/>
+      <c r="BD11" s="54"/>
     </row>
     <row r="12" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="40">
+      <c r="C12" s="38">
         <v>101010121</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="22">
         <v>101020101</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="43">
+      <c r="F12" s="58">
         <v>101044082</v>
       </c>
-      <c r="G12" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="58"/>
-      <c r="R12" s="58"/>
-      <c r="S12" s="58"/>
-      <c r="T12" s="58"/>
-      <c r="U12" s="58"/>
-      <c r="V12" s="58"/>
-      <c r="W12" s="58"/>
-      <c r="X12" s="58"/>
-      <c r="Y12" s="58"/>
-      <c r="Z12" s="58"/>
-      <c r="AA12" s="58"/>
-      <c r="AB12" s="58"/>
-      <c r="AC12" s="58"/>
-      <c r="AD12" s="58"/>
-      <c r="AE12" s="58"/>
-      <c r="AF12" s="58"/>
-      <c r="AG12" s="58"/>
-      <c r="AH12" s="58"/>
-      <c r="AI12" s="58"/>
-      <c r="AJ12" s="58"/>
-      <c r="AK12" s="58"/>
-      <c r="AL12" s="58"/>
-      <c r="AM12" s="58"/>
-      <c r="AN12" s="58"/>
-      <c r="AO12" s="58"/>
-      <c r="AP12" s="58"/>
-      <c r="AQ12" s="58"/>
-      <c r="AR12" s="58"/>
-      <c r="AS12" s="58"/>
-      <c r="AT12" s="58"/>
-      <c r="AU12" s="58"/>
-      <c r="AV12" s="58"/>
-      <c r="AW12" s="58"/>
-      <c r="AX12" s="58"/>
-      <c r="AY12" s="58"/>
-      <c r="AZ12" s="58"/>
-      <c r="BA12" s="58"/>
-      <c r="BB12" s="58"/>
-      <c r="BC12" s="58"/>
-      <c r="BD12" s="58"/>
+      <c r="G12" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="54"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="54"/>
+      <c r="R12" s="54"/>
+      <c r="S12" s="54"/>
+      <c r="T12" s="54"/>
+      <c r="U12" s="54"/>
+      <c r="V12" s="54"/>
+      <c r="W12" s="54"/>
+      <c r="X12" s="54"/>
+      <c r="Y12" s="54"/>
+      <c r="Z12" s="54"/>
+      <c r="AA12" s="54"/>
+      <c r="AB12" s="54"/>
+      <c r="AC12" s="54"/>
+      <c r="AD12" s="54"/>
+      <c r="AE12" s="54"/>
+      <c r="AF12" s="54"/>
+      <c r="AG12" s="54"/>
+      <c r="AH12" s="54"/>
+      <c r="AI12" s="54"/>
+      <c r="AJ12" s="54"/>
+      <c r="AK12" s="54"/>
+      <c r="AL12" s="54"/>
+      <c r="AM12" s="54"/>
+      <c r="AN12" s="54"/>
+      <c r="AO12" s="54"/>
+      <c r="AP12" s="54"/>
+      <c r="AQ12" s="54"/>
+      <c r="AR12" s="54"/>
+      <c r="AS12" s="54"/>
+      <c r="AT12" s="54"/>
+      <c r="AU12" s="54"/>
+      <c r="AV12" s="54"/>
+      <c r="AW12" s="54"/>
+      <c r="AX12" s="54"/>
+      <c r="AY12" s="54"/>
+      <c r="AZ12" s="54"/>
+      <c r="BA12" s="54"/>
+      <c r="BB12" s="54"/>
+      <c r="BC12" s="54"/>
+      <c r="BD12" s="54"/>
     </row>
     <row r="13" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="44">
+      <c r="C13" s="40">
         <v>101010202</v>
       </c>
-      <c r="D13" s="45">
+      <c r="D13" s="41">
         <v>101020201</v>
       </c>
-      <c r="E13" s="45" t="s">
+      <c r="E13" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="43">
+      <c r="F13" s="58">
         <v>101052002</v>
       </c>
-      <c r="G13" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="58"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="58"/>
-      <c r="Q13" s="58"/>
-      <c r="R13" s="58"/>
-      <c r="S13" s="58"/>
-      <c r="T13" s="58"/>
-      <c r="U13" s="58"/>
-      <c r="V13" s="58"/>
-      <c r="W13" s="58"/>
-      <c r="X13" s="58"/>
-      <c r="Y13" s="58"/>
-      <c r="Z13" s="58"/>
-      <c r="AA13" s="58"/>
-      <c r="AB13" s="58"/>
-      <c r="AC13" s="58"/>
-      <c r="AD13" s="58"/>
-      <c r="AE13" s="58"/>
-      <c r="AF13" s="58"/>
-      <c r="AG13" s="58"/>
-      <c r="AH13" s="58"/>
-      <c r="AI13" s="58"/>
-      <c r="AJ13" s="58"/>
-      <c r="AK13" s="58"/>
-      <c r="AL13" s="58"/>
-      <c r="AM13" s="58"/>
-      <c r="AN13" s="58"/>
-      <c r="AO13" s="58"/>
-      <c r="AP13" s="58"/>
-      <c r="AQ13" s="58"/>
-      <c r="AR13" s="58"/>
-      <c r="AS13" s="58"/>
-      <c r="AT13" s="58"/>
-      <c r="AU13" s="58"/>
-      <c r="AV13" s="58"/>
-      <c r="AW13" s="58"/>
-      <c r="AX13" s="58"/>
-      <c r="AY13" s="58"/>
-      <c r="AZ13" s="58"/>
-      <c r="BA13" s="58"/>
-      <c r="BB13" s="58"/>
-      <c r="BC13" s="58"/>
-      <c r="BD13" s="58"/>
+      <c r="G13" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="54"/>
+      <c r="O13" s="54"/>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="54"/>
+      <c r="S13" s="54"/>
+      <c r="T13" s="54"/>
+      <c r="U13" s="54"/>
+      <c r="V13" s="54"/>
+      <c r="W13" s="54"/>
+      <c r="X13" s="54"/>
+      <c r="Y13" s="54"/>
+      <c r="Z13" s="54"/>
+      <c r="AA13" s="54"/>
+      <c r="AB13" s="54"/>
+      <c r="AC13" s="54"/>
+      <c r="AD13" s="54"/>
+      <c r="AE13" s="54"/>
+      <c r="AF13" s="54"/>
+      <c r="AG13" s="54"/>
+      <c r="AH13" s="54"/>
+      <c r="AI13" s="54"/>
+      <c r="AJ13" s="54"/>
+      <c r="AK13" s="54"/>
+      <c r="AL13" s="54"/>
+      <c r="AM13" s="54"/>
+      <c r="AN13" s="54"/>
+      <c r="AO13" s="54"/>
+      <c r="AP13" s="54"/>
+      <c r="AQ13" s="54"/>
+      <c r="AR13" s="54"/>
+      <c r="AS13" s="54"/>
+      <c r="AT13" s="54"/>
+      <c r="AU13" s="54"/>
+      <c r="AV13" s="54"/>
+      <c r="AW13" s="54"/>
+      <c r="AX13" s="54"/>
+      <c r="AY13" s="54"/>
+      <c r="AZ13" s="54"/>
+      <c r="BA13" s="54"/>
+      <c r="BB13" s="54"/>
+      <c r="BC13" s="54"/>
+      <c r="BD13" s="54"/>
     </row>
     <row r="14" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="44">
+      <c r="C14" s="40">
         <v>101010206</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="42">
         <v>101020201</v>
       </c>
-      <c r="E14" s="46" t="s">
+      <c r="E14" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="43">
+      <c r="F14" s="58">
         <v>101052002</v>
       </c>
-      <c r="G14" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H14" s="58"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="58"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="58"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="58"/>
-      <c r="Q14" s="58"/>
-      <c r="R14" s="58"/>
-      <c r="S14" s="58"/>
-      <c r="T14" s="58"/>
-      <c r="U14" s="58"/>
-      <c r="V14" s="58"/>
-      <c r="W14" s="58"/>
-      <c r="X14" s="58"/>
-      <c r="Y14" s="58"/>
-      <c r="Z14" s="58"/>
-      <c r="AA14" s="58"/>
-      <c r="AB14" s="58"/>
-      <c r="AC14" s="58"/>
-      <c r="AD14" s="58"/>
-      <c r="AE14" s="58"/>
-      <c r="AF14" s="58"/>
-      <c r="AG14" s="58"/>
-      <c r="AH14" s="58"/>
-      <c r="AI14" s="58"/>
-      <c r="AJ14" s="58"/>
-      <c r="AK14" s="58"/>
-      <c r="AL14" s="58"/>
-      <c r="AM14" s="58"/>
-      <c r="AN14" s="58"/>
-      <c r="AO14" s="58"/>
-      <c r="AP14" s="58"/>
-      <c r="AQ14" s="58"/>
-      <c r="AR14" s="58"/>
-      <c r="AS14" s="58"/>
-      <c r="AT14" s="58"/>
-      <c r="AU14" s="58"/>
-      <c r="AV14" s="58"/>
-      <c r="AW14" s="58"/>
-      <c r="AX14" s="58"/>
-      <c r="AY14" s="58"/>
-      <c r="AZ14" s="58"/>
-      <c r="BA14" s="58"/>
-      <c r="BB14" s="58"/>
-      <c r="BC14" s="58"/>
-      <c r="BD14" s="58"/>
+      <c r="G14" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="54"/>
+      <c r="O14" s="54"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="54"/>
+      <c r="R14" s="54"/>
+      <c r="S14" s="54"/>
+      <c r="T14" s="54"/>
+      <c r="U14" s="54"/>
+      <c r="V14" s="54"/>
+      <c r="W14" s="54"/>
+      <c r="X14" s="54"/>
+      <c r="Y14" s="54"/>
+      <c r="Z14" s="54"/>
+      <c r="AA14" s="54"/>
+      <c r="AB14" s="54"/>
+      <c r="AC14" s="54"/>
+      <c r="AD14" s="54"/>
+      <c r="AE14" s="54"/>
+      <c r="AF14" s="54"/>
+      <c r="AG14" s="54"/>
+      <c r="AH14" s="54"/>
+      <c r="AI14" s="54"/>
+      <c r="AJ14" s="54"/>
+      <c r="AK14" s="54"/>
+      <c r="AL14" s="54"/>
+      <c r="AM14" s="54"/>
+      <c r="AN14" s="54"/>
+      <c r="AO14" s="54"/>
+      <c r="AP14" s="54"/>
+      <c r="AQ14" s="54"/>
+      <c r="AR14" s="54"/>
+      <c r="AS14" s="54"/>
+      <c r="AT14" s="54"/>
+      <c r="AU14" s="54"/>
+      <c r="AV14" s="54"/>
+      <c r="AW14" s="54"/>
+      <c r="AX14" s="54"/>
+      <c r="AY14" s="54"/>
+      <c r="AZ14" s="54"/>
+      <c r="BA14" s="54"/>
+      <c r="BB14" s="54"/>
+      <c r="BC14" s="54"/>
+      <c r="BD14" s="54"/>
     </row>
     <row r="15" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="44">
+      <c r="C15" s="40">
         <v>101010207</v>
       </c>
-      <c r="D15" s="46">
+      <c r="D15" s="42">
         <v>101020201</v>
       </c>
-      <c r="E15" s="46" t="s">
+      <c r="E15" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="43">
+      <c r="F15" s="58">
         <v>101052002</v>
       </c>
-      <c r="G15" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="58"/>
-      <c r="M15" s="58"/>
-      <c r="N15" s="58"/>
-      <c r="O15" s="58"/>
-      <c r="P15" s="58"/>
-      <c r="Q15" s="58"/>
-      <c r="R15" s="58"/>
-      <c r="S15" s="58"/>
-      <c r="T15" s="58"/>
-      <c r="U15" s="58"/>
-      <c r="V15" s="58"/>
-      <c r="W15" s="58"/>
-      <c r="X15" s="58"/>
-      <c r="Y15" s="58"/>
-      <c r="Z15" s="58"/>
-      <c r="AA15" s="58"/>
-      <c r="AB15" s="58"/>
-      <c r="AC15" s="58"/>
-      <c r="AD15" s="58"/>
-      <c r="AE15" s="58"/>
-      <c r="AF15" s="58"/>
-      <c r="AG15" s="58"/>
-      <c r="AH15" s="58"/>
-      <c r="AI15" s="58"/>
-      <c r="AJ15" s="58"/>
-      <c r="AK15" s="58"/>
-      <c r="AL15" s="58"/>
-      <c r="AM15" s="58"/>
-      <c r="AN15" s="58"/>
-      <c r="AO15" s="58"/>
-      <c r="AP15" s="58"/>
-      <c r="AQ15" s="58"/>
-      <c r="AR15" s="58"/>
-      <c r="AS15" s="58"/>
-      <c r="AT15" s="58"/>
-      <c r="AU15" s="58"/>
-      <c r="AV15" s="58"/>
-      <c r="AW15" s="58"/>
-      <c r="AX15" s="58"/>
-      <c r="AY15" s="58"/>
-      <c r="AZ15" s="58"/>
-      <c r="BA15" s="58"/>
-      <c r="BB15" s="58"/>
-      <c r="BC15" s="58"/>
-      <c r="BD15" s="58"/>
+      <c r="G15" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="54"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="54"/>
+      <c r="R15" s="54"/>
+      <c r="S15" s="54"/>
+      <c r="T15" s="54"/>
+      <c r="U15" s="54"/>
+      <c r="V15" s="54"/>
+      <c r="W15" s="54"/>
+      <c r="X15" s="54"/>
+      <c r="Y15" s="54"/>
+      <c r="Z15" s="54"/>
+      <c r="AA15" s="54"/>
+      <c r="AB15" s="54"/>
+      <c r="AC15" s="54"/>
+      <c r="AD15" s="54"/>
+      <c r="AE15" s="54"/>
+      <c r="AF15" s="54"/>
+      <c r="AG15" s="54"/>
+      <c r="AH15" s="54"/>
+      <c r="AI15" s="54"/>
+      <c r="AJ15" s="54"/>
+      <c r="AK15" s="54"/>
+      <c r="AL15" s="54"/>
+      <c r="AM15" s="54"/>
+      <c r="AN15" s="54"/>
+      <c r="AO15" s="54"/>
+      <c r="AP15" s="54"/>
+      <c r="AQ15" s="54"/>
+      <c r="AR15" s="54"/>
+      <c r="AS15" s="54"/>
+      <c r="AT15" s="54"/>
+      <c r="AU15" s="54"/>
+      <c r="AV15" s="54"/>
+      <c r="AW15" s="54"/>
+      <c r="AX15" s="54"/>
+      <c r="AY15" s="54"/>
+      <c r="AZ15" s="54"/>
+      <c r="BA15" s="54"/>
+      <c r="BB15" s="54"/>
+      <c r="BC15" s="54"/>
+      <c r="BD15" s="54"/>
     </row>
     <row r="16" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="40">
         <v>101010209</v>
       </c>
-      <c r="D16" s="46">
+      <c r="D16" s="42">
         <v>101020201</v>
       </c>
-      <c r="E16" s="46" t="s">
+      <c r="E16" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="43">
+      <c r="F16" s="58">
         <v>101052002</v>
       </c>
-      <c r="G16" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H16" s="58"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="58"/>
-      <c r="K16" s="58"/>
-      <c r="L16" s="58"/>
-      <c r="M16" s="58"/>
-      <c r="N16" s="58"/>
-      <c r="O16" s="58"/>
-      <c r="P16" s="58"/>
-      <c r="Q16" s="58"/>
-      <c r="R16" s="58"/>
-      <c r="S16" s="58"/>
-      <c r="T16" s="58"/>
-      <c r="U16" s="58"/>
-      <c r="V16" s="58"/>
-      <c r="W16" s="58"/>
-      <c r="X16" s="58"/>
-      <c r="Y16" s="58"/>
-      <c r="Z16" s="58"/>
-      <c r="AA16" s="58"/>
-      <c r="AB16" s="58"/>
-      <c r="AC16" s="58"/>
-      <c r="AD16" s="58"/>
-      <c r="AE16" s="58"/>
-      <c r="AF16" s="58"/>
-      <c r="AG16" s="58"/>
-      <c r="AH16" s="58"/>
-      <c r="AI16" s="58"/>
-      <c r="AJ16" s="58"/>
-      <c r="AK16" s="58"/>
-      <c r="AL16" s="58"/>
-      <c r="AM16" s="58"/>
-      <c r="AN16" s="58"/>
-      <c r="AO16" s="58"/>
-      <c r="AP16" s="58"/>
-      <c r="AQ16" s="58"/>
-      <c r="AR16" s="58"/>
-      <c r="AS16" s="58"/>
-      <c r="AT16" s="58"/>
-      <c r="AU16" s="58"/>
-      <c r="AV16" s="58"/>
-      <c r="AW16" s="58"/>
-      <c r="AX16" s="58"/>
-      <c r="AY16" s="58"/>
-      <c r="AZ16" s="58"/>
-      <c r="BA16" s="58"/>
-      <c r="BB16" s="58"/>
-      <c r="BC16" s="58"/>
-      <c r="BD16" s="58"/>
+      <c r="G16" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="54"/>
+      <c r="O16" s="54"/>
+      <c r="P16" s="54"/>
+      <c r="Q16" s="54"/>
+      <c r="R16" s="54"/>
+      <c r="S16" s="54"/>
+      <c r="T16" s="54"/>
+      <c r="U16" s="54"/>
+      <c r="V16" s="54"/>
+      <c r="W16" s="54"/>
+      <c r="X16" s="54"/>
+      <c r="Y16" s="54"/>
+      <c r="Z16" s="54"/>
+      <c r="AA16" s="54"/>
+      <c r="AB16" s="54"/>
+      <c r="AC16" s="54"/>
+      <c r="AD16" s="54"/>
+      <c r="AE16" s="54"/>
+      <c r="AF16" s="54"/>
+      <c r="AG16" s="54"/>
+      <c r="AH16" s="54"/>
+      <c r="AI16" s="54"/>
+      <c r="AJ16" s="54"/>
+      <c r="AK16" s="54"/>
+      <c r="AL16" s="54"/>
+      <c r="AM16" s="54"/>
+      <c r="AN16" s="54"/>
+      <c r="AO16" s="54"/>
+      <c r="AP16" s="54"/>
+      <c r="AQ16" s="54"/>
+      <c r="AR16" s="54"/>
+      <c r="AS16" s="54"/>
+      <c r="AT16" s="54"/>
+      <c r="AU16" s="54"/>
+      <c r="AV16" s="54"/>
+      <c r="AW16" s="54"/>
+      <c r="AX16" s="54"/>
+      <c r="AY16" s="54"/>
+      <c r="AZ16" s="54"/>
+      <c r="BA16" s="54"/>
+      <c r="BB16" s="54"/>
+      <c r="BC16" s="54"/>
+      <c r="BD16" s="54"/>
     </row>
     <row r="17" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="44">
+      <c r="C17" s="40">
         <v>101010211</v>
       </c>
-      <c r="D17" s="46">
+      <c r="D17" s="42">
         <v>101020201</v>
       </c>
-      <c r="E17" s="46" t="s">
+      <c r="E17" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="43">
+      <c r="F17" s="58">
         <v>101052002</v>
       </c>
-      <c r="G17" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="58"/>
-      <c r="L17" s="58"/>
-      <c r="M17" s="58"/>
-      <c r="N17" s="58"/>
-      <c r="O17" s="58"/>
-      <c r="P17" s="58"/>
-      <c r="Q17" s="58"/>
-      <c r="R17" s="58"/>
-      <c r="S17" s="58"/>
-      <c r="T17" s="58"/>
-      <c r="U17" s="58"/>
-      <c r="V17" s="58"/>
-      <c r="W17" s="58"/>
-      <c r="X17" s="58"/>
-      <c r="Y17" s="58"/>
-      <c r="Z17" s="58"/>
-      <c r="AA17" s="58"/>
-      <c r="AB17" s="58"/>
-      <c r="AC17" s="58"/>
-      <c r="AD17" s="58"/>
-      <c r="AE17" s="58"/>
-      <c r="AF17" s="58"/>
-      <c r="AG17" s="58"/>
-      <c r="AH17" s="58"/>
-      <c r="AI17" s="58"/>
-      <c r="AJ17" s="58"/>
-      <c r="AK17" s="58"/>
-      <c r="AL17" s="58"/>
-      <c r="AM17" s="58"/>
-      <c r="AN17" s="58"/>
-      <c r="AO17" s="58"/>
-      <c r="AP17" s="58"/>
-      <c r="AQ17" s="58"/>
-      <c r="AR17" s="58"/>
-      <c r="AS17" s="58"/>
-      <c r="AT17" s="58"/>
-      <c r="AU17" s="58"/>
-      <c r="AV17" s="58"/>
-      <c r="AW17" s="58"/>
-      <c r="AX17" s="58"/>
-      <c r="AY17" s="58"/>
-      <c r="AZ17" s="58"/>
-      <c r="BA17" s="58"/>
-      <c r="BB17" s="58"/>
-      <c r="BC17" s="58"/>
-      <c r="BD17" s="58"/>
+      <c r="G17" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="54"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="54"/>
+      <c r="P17" s="54"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="54"/>
+      <c r="S17" s="54"/>
+      <c r="T17" s="54"/>
+      <c r="U17" s="54"/>
+      <c r="V17" s="54"/>
+      <c r="W17" s="54"/>
+      <c r="X17" s="54"/>
+      <c r="Y17" s="54"/>
+      <c r="Z17" s="54"/>
+      <c r="AA17" s="54"/>
+      <c r="AB17" s="54"/>
+      <c r="AC17" s="54"/>
+      <c r="AD17" s="54"/>
+      <c r="AE17" s="54"/>
+      <c r="AF17" s="54"/>
+      <c r="AG17" s="54"/>
+      <c r="AH17" s="54"/>
+      <c r="AI17" s="54"/>
+      <c r="AJ17" s="54"/>
+      <c r="AK17" s="54"/>
+      <c r="AL17" s="54"/>
+      <c r="AM17" s="54"/>
+      <c r="AN17" s="54"/>
+      <c r="AO17" s="54"/>
+      <c r="AP17" s="54"/>
+      <c r="AQ17" s="54"/>
+      <c r="AR17" s="54"/>
+      <c r="AS17" s="54"/>
+      <c r="AT17" s="54"/>
+      <c r="AU17" s="54"/>
+      <c r="AV17" s="54"/>
+      <c r="AW17" s="54"/>
+      <c r="AX17" s="54"/>
+      <c r="AY17" s="54"/>
+      <c r="AZ17" s="54"/>
+      <c r="BA17" s="54"/>
+      <c r="BB17" s="54"/>
+      <c r="BC17" s="54"/>
+      <c r="BD17" s="54"/>
     </row>
     <row r="18" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="44">
+      <c r="C18" s="40">
         <v>101010214</v>
       </c>
-      <c r="D18" s="46">
+      <c r="D18" s="42">
         <v>101020201</v>
       </c>
-      <c r="E18" s="46" t="s">
+      <c r="E18" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="43">
+      <c r="F18" s="58">
         <v>101052002</v>
       </c>
-      <c r="G18" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="58"/>
-      <c r="K18" s="58"/>
-      <c r="L18" s="58"/>
-      <c r="M18" s="58"/>
-      <c r="N18" s="58"/>
-      <c r="O18" s="58"/>
-      <c r="P18" s="58"/>
-      <c r="Q18" s="58"/>
-      <c r="R18" s="58"/>
-      <c r="S18" s="58"/>
-      <c r="T18" s="58"/>
-      <c r="U18" s="58"/>
-      <c r="V18" s="58"/>
-      <c r="W18" s="58"/>
-      <c r="X18" s="58"/>
-      <c r="Y18" s="58"/>
-      <c r="Z18" s="58"/>
-      <c r="AA18" s="58"/>
-      <c r="AB18" s="58"/>
-      <c r="AC18" s="58"/>
-      <c r="AD18" s="58"/>
-      <c r="AE18" s="58"/>
-      <c r="AF18" s="58"/>
-      <c r="AG18" s="58"/>
-      <c r="AH18" s="58"/>
-      <c r="AI18" s="58"/>
-      <c r="AJ18" s="58"/>
-      <c r="AK18" s="58"/>
-      <c r="AL18" s="58"/>
-      <c r="AM18" s="58"/>
-      <c r="AN18" s="58"/>
-      <c r="AO18" s="58"/>
-      <c r="AP18" s="58"/>
-      <c r="AQ18" s="58"/>
-      <c r="AR18" s="58"/>
-      <c r="AS18" s="58"/>
-      <c r="AT18" s="58"/>
-      <c r="AU18" s="58"/>
-      <c r="AV18" s="58"/>
-      <c r="AW18" s="58"/>
-      <c r="AX18" s="58"/>
-      <c r="AY18" s="58"/>
-      <c r="AZ18" s="58"/>
-      <c r="BA18" s="58"/>
-      <c r="BB18" s="58"/>
-      <c r="BC18" s="58"/>
-      <c r="BD18" s="58"/>
+      <c r="G18" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="54"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="54"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="54"/>
+      <c r="T18" s="54"/>
+      <c r="U18" s="54"/>
+      <c r="V18" s="54"/>
+      <c r="W18" s="54"/>
+      <c r="X18" s="54"/>
+      <c r="Y18" s="54"/>
+      <c r="Z18" s="54"/>
+      <c r="AA18" s="54"/>
+      <c r="AB18" s="54"/>
+      <c r="AC18" s="54"/>
+      <c r="AD18" s="54"/>
+      <c r="AE18" s="54"/>
+      <c r="AF18" s="54"/>
+      <c r="AG18" s="54"/>
+      <c r="AH18" s="54"/>
+      <c r="AI18" s="54"/>
+      <c r="AJ18" s="54"/>
+      <c r="AK18" s="54"/>
+      <c r="AL18" s="54"/>
+      <c r="AM18" s="54"/>
+      <c r="AN18" s="54"/>
+      <c r="AO18" s="54"/>
+      <c r="AP18" s="54"/>
+      <c r="AQ18" s="54"/>
+      <c r="AR18" s="54"/>
+      <c r="AS18" s="54"/>
+      <c r="AT18" s="54"/>
+      <c r="AU18" s="54"/>
+      <c r="AV18" s="54"/>
+      <c r="AW18" s="54"/>
+      <c r="AX18" s="54"/>
+      <c r="AY18" s="54"/>
+      <c r="AZ18" s="54"/>
+      <c r="BA18" s="54"/>
+      <c r="BB18" s="54"/>
+      <c r="BC18" s="54"/>
+      <c r="BD18" s="54"/>
     </row>
     <row r="19" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="44">
+      <c r="C19" s="40">
         <v>101010217</v>
       </c>
-      <c r="D19" s="46">
+      <c r="D19" s="42">
         <v>101020201</v>
       </c>
-      <c r="E19" s="46" t="s">
+      <c r="E19" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="43">
+      <c r="F19" s="58">
         <v>101052002</v>
       </c>
-      <c r="G19" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="58"/>
-      <c r="K19" s="58"/>
-      <c r="L19" s="58"/>
-      <c r="M19" s="58"/>
-      <c r="N19" s="58"/>
-      <c r="O19" s="58"/>
-      <c r="P19" s="58"/>
-      <c r="Q19" s="58"/>
-      <c r="R19" s="58"/>
-      <c r="S19" s="58"/>
-      <c r="T19" s="58"/>
-      <c r="U19" s="58"/>
-      <c r="V19" s="58"/>
-      <c r="W19" s="58"/>
-      <c r="X19" s="58"/>
-      <c r="Y19" s="58"/>
-      <c r="Z19" s="58"/>
-      <c r="AA19" s="58"/>
-      <c r="AB19" s="58"/>
-      <c r="AC19" s="58"/>
-      <c r="AD19" s="58"/>
-      <c r="AE19" s="58"/>
-      <c r="AF19" s="58"/>
-      <c r="AG19" s="58"/>
-      <c r="AH19" s="58"/>
-      <c r="AI19" s="58"/>
-      <c r="AJ19" s="58"/>
-      <c r="AK19" s="58"/>
-      <c r="AL19" s="58"/>
-      <c r="AM19" s="58"/>
-      <c r="AN19" s="58"/>
-      <c r="AO19" s="58"/>
-      <c r="AP19" s="58"/>
-      <c r="AQ19" s="58"/>
-      <c r="AR19" s="58"/>
-      <c r="AS19" s="58"/>
-      <c r="AT19" s="58"/>
-      <c r="AU19" s="58"/>
-      <c r="AV19" s="58"/>
-      <c r="AW19" s="58"/>
-      <c r="AX19" s="58"/>
-      <c r="AY19" s="58"/>
-      <c r="AZ19" s="58"/>
-      <c r="BA19" s="58"/>
-      <c r="BB19" s="58"/>
-      <c r="BC19" s="58"/>
-      <c r="BD19" s="58"/>
+      <c r="G19" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="54"/>
+      <c r="O19" s="54"/>
+      <c r="P19" s="54"/>
+      <c r="Q19" s="54"/>
+      <c r="R19" s="54"/>
+      <c r="S19" s="54"/>
+      <c r="T19" s="54"/>
+      <c r="U19" s="54"/>
+      <c r="V19" s="54"/>
+      <c r="W19" s="54"/>
+      <c r="X19" s="54"/>
+      <c r="Y19" s="54"/>
+      <c r="Z19" s="54"/>
+      <c r="AA19" s="54"/>
+      <c r="AB19" s="54"/>
+      <c r="AC19" s="54"/>
+      <c r="AD19" s="54"/>
+      <c r="AE19" s="54"/>
+      <c r="AF19" s="54"/>
+      <c r="AG19" s="54"/>
+      <c r="AH19" s="54"/>
+      <c r="AI19" s="54"/>
+      <c r="AJ19" s="54"/>
+      <c r="AK19" s="54"/>
+      <c r="AL19" s="54"/>
+      <c r="AM19" s="54"/>
+      <c r="AN19" s="54"/>
+      <c r="AO19" s="54"/>
+      <c r="AP19" s="54"/>
+      <c r="AQ19" s="54"/>
+      <c r="AR19" s="54"/>
+      <c r="AS19" s="54"/>
+      <c r="AT19" s="54"/>
+      <c r="AU19" s="54"/>
+      <c r="AV19" s="54"/>
+      <c r="AW19" s="54"/>
+      <c r="AX19" s="54"/>
+      <c r="AY19" s="54"/>
+      <c r="AZ19" s="54"/>
+      <c r="BA19" s="54"/>
+      <c r="BB19" s="54"/>
+      <c r="BC19" s="54"/>
+      <c r="BD19" s="54"/>
     </row>
     <row r="20" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="44">
+      <c r="C20" s="40">
         <v>101010219</v>
       </c>
-      <c r="D20" s="46">
+      <c r="D20" s="42">
         <v>101020201</v>
       </c>
-      <c r="E20" s="46" t="s">
+      <c r="E20" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="43">
+      <c r="F20" s="58">
         <v>101052002</v>
       </c>
-      <c r="G20" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H20" s="58"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="58"/>
-      <c r="M20" s="58"/>
-      <c r="N20" s="58"/>
-      <c r="O20" s="58"/>
-      <c r="P20" s="58"/>
-      <c r="Q20" s="58"/>
-      <c r="R20" s="58"/>
-      <c r="S20" s="58"/>
-      <c r="T20" s="58"/>
-      <c r="U20" s="58"/>
-      <c r="V20" s="58"/>
-      <c r="W20" s="58"/>
-      <c r="X20" s="58"/>
-      <c r="Y20" s="58"/>
-      <c r="Z20" s="58"/>
-      <c r="AA20" s="58"/>
-      <c r="AB20" s="58"/>
-      <c r="AC20" s="58"/>
-      <c r="AD20" s="58"/>
-      <c r="AE20" s="58"/>
-      <c r="AF20" s="58"/>
-      <c r="AG20" s="58"/>
-      <c r="AH20" s="58"/>
-      <c r="AI20" s="58"/>
-      <c r="AJ20" s="58"/>
-      <c r="AK20" s="58"/>
-      <c r="AL20" s="58"/>
-      <c r="AM20" s="58"/>
-      <c r="AN20" s="58"/>
-      <c r="AO20" s="58"/>
-      <c r="AP20" s="58"/>
-      <c r="AQ20" s="58"/>
-      <c r="AR20" s="58"/>
-      <c r="AS20" s="58"/>
-      <c r="AT20" s="58"/>
-      <c r="AU20" s="58"/>
-      <c r="AV20" s="58"/>
-      <c r="AW20" s="58"/>
-      <c r="AX20" s="58"/>
-      <c r="AY20" s="58"/>
-      <c r="AZ20" s="58"/>
-      <c r="BA20" s="58"/>
-      <c r="BB20" s="58"/>
-      <c r="BC20" s="58"/>
-      <c r="BD20" s="58"/>
+      <c r="G20" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="54"/>
+      <c r="P20" s="54"/>
+      <c r="Q20" s="54"/>
+      <c r="R20" s="54"/>
+      <c r="S20" s="54"/>
+      <c r="T20" s="54"/>
+      <c r="U20" s="54"/>
+      <c r="V20" s="54"/>
+      <c r="W20" s="54"/>
+      <c r="X20" s="54"/>
+      <c r="Y20" s="54"/>
+      <c r="Z20" s="54"/>
+      <c r="AA20" s="54"/>
+      <c r="AB20" s="54"/>
+      <c r="AC20" s="54"/>
+      <c r="AD20" s="54"/>
+      <c r="AE20" s="54"/>
+      <c r="AF20" s="54"/>
+      <c r="AG20" s="54"/>
+      <c r="AH20" s="54"/>
+      <c r="AI20" s="54"/>
+      <c r="AJ20" s="54"/>
+      <c r="AK20" s="54"/>
+      <c r="AL20" s="54"/>
+      <c r="AM20" s="54"/>
+      <c r="AN20" s="54"/>
+      <c r="AO20" s="54"/>
+      <c r="AP20" s="54"/>
+      <c r="AQ20" s="54"/>
+      <c r="AR20" s="54"/>
+      <c r="AS20" s="54"/>
+      <c r="AT20" s="54"/>
+      <c r="AU20" s="54"/>
+      <c r="AV20" s="54"/>
+      <c r="AW20" s="54"/>
+      <c r="AX20" s="54"/>
+      <c r="AY20" s="54"/>
+      <c r="AZ20" s="54"/>
+      <c r="BA20" s="54"/>
+      <c r="BB20" s="54"/>
+      <c r="BC20" s="54"/>
+      <c r="BD20" s="54"/>
     </row>
     <row r="21" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="29">
+      <c r="C21" s="27">
         <v>101010221</v>
       </c>
-      <c r="D21" s="48">
+      <c r="D21" s="44">
         <v>101020201</v>
       </c>
-      <c r="E21" s="48" t="s">
+      <c r="E21" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="43">
+      <c r="F21" s="58">
         <v>101052002</v>
       </c>
-      <c r="G21" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="58"/>
-      <c r="L21" s="58"/>
-      <c r="M21" s="58"/>
-      <c r="N21" s="58"/>
-      <c r="O21" s="58"/>
-      <c r="P21" s="58"/>
-      <c r="Q21" s="58"/>
-      <c r="R21" s="58"/>
-      <c r="S21" s="58"/>
-      <c r="T21" s="58"/>
-      <c r="U21" s="58"/>
-      <c r="V21" s="58"/>
-      <c r="W21" s="58"/>
-      <c r="X21" s="58"/>
-      <c r="Y21" s="58"/>
-      <c r="Z21" s="58"/>
-      <c r="AA21" s="58"/>
-      <c r="AB21" s="58"/>
-      <c r="AC21" s="58"/>
-      <c r="AD21" s="58"/>
-      <c r="AE21" s="58"/>
-      <c r="AF21" s="58"/>
-      <c r="AG21" s="58"/>
-      <c r="AH21" s="58"/>
-      <c r="AI21" s="58"/>
-      <c r="AJ21" s="58"/>
-      <c r="AK21" s="58"/>
-      <c r="AL21" s="58"/>
-      <c r="AM21" s="58"/>
-      <c r="AN21" s="58"/>
-      <c r="AO21" s="58"/>
-      <c r="AP21" s="58"/>
-      <c r="AQ21" s="58"/>
-      <c r="AR21" s="58"/>
-      <c r="AS21" s="58"/>
-      <c r="AT21" s="58"/>
-      <c r="AU21" s="58"/>
-      <c r="AV21" s="58"/>
-      <c r="AW21" s="58"/>
-      <c r="AX21" s="58"/>
-      <c r="AY21" s="58"/>
-      <c r="AZ21" s="58"/>
-      <c r="BA21" s="58"/>
-      <c r="BB21" s="58"/>
-      <c r="BC21" s="58"/>
-      <c r="BD21" s="58"/>
+      <c r="G21" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="54"/>
+      <c r="O21" s="54"/>
+      <c r="P21" s="54"/>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="54"/>
+      <c r="S21" s="54"/>
+      <c r="T21" s="54"/>
+      <c r="U21" s="54"/>
+      <c r="V21" s="54"/>
+      <c r="W21" s="54"/>
+      <c r="X21" s="54"/>
+      <c r="Y21" s="54"/>
+      <c r="Z21" s="54"/>
+      <c r="AA21" s="54"/>
+      <c r="AB21" s="54"/>
+      <c r="AC21" s="54"/>
+      <c r="AD21" s="54"/>
+      <c r="AE21" s="54"/>
+      <c r="AF21" s="54"/>
+      <c r="AG21" s="54"/>
+      <c r="AH21" s="54"/>
+      <c r="AI21" s="54"/>
+      <c r="AJ21" s="54"/>
+      <c r="AK21" s="54"/>
+      <c r="AL21" s="54"/>
+      <c r="AM21" s="54"/>
+      <c r="AN21" s="54"/>
+      <c r="AO21" s="54"/>
+      <c r="AP21" s="54"/>
+      <c r="AQ21" s="54"/>
+      <c r="AR21" s="54"/>
+      <c r="AS21" s="54"/>
+      <c r="AT21" s="54"/>
+      <c r="AU21" s="54"/>
+      <c r="AV21" s="54"/>
+      <c r="AW21" s="54"/>
+      <c r="AX21" s="54"/>
+      <c r="AY21" s="54"/>
+      <c r="AZ21" s="54"/>
+      <c r="BA21" s="54"/>
+      <c r="BB21" s="54"/>
+      <c r="BC21" s="54"/>
+      <c r="BD21" s="54"/>
     </row>
     <row r="22" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
+      <c r="A22" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2685,6 +2651,18 @@
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.38" bottom="0.27" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{50EF1DB0-88D6-4C93-AB37-ABB00C223944}">
+          <x14:formula1>
+            <xm:f>Hoja1!$A$1:$A$26</xm:f>
+          </x14:formula1>
+          <xm:sqref>F4:F21</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2692,8 +2670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2738,8 +2716,8 @@
         <v>101010101</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="56" t="s">
+      <c r="E3" s="47"/>
+      <c r="F3" s="52" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2756,13 +2734,13 @@
       <c r="D4" s="14">
         <v>101044012</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="G4" s="14"/>
+      <c r="F4" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="55"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -2777,13 +2755,13 @@
       <c r="D5" s="14">
         <v>101044012</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="G5" s="14"/>
+      <c r="F5" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="55"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
@@ -2798,13 +2776,13 @@
       <c r="D6" s="14">
         <v>101044012</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="G6" s="14"/>
+      <c r="F6" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="55"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -2817,15 +2795,15 @@
         <v>101010133</v>
       </c>
       <c r="D7" s="14">
-        <v>101044012</v>
-      </c>
-      <c r="E7" s="52" t="s">
+        <v>101041012</v>
+      </c>
+      <c r="E7" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" s="14"/>
+      <c r="F7" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="55"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
@@ -2840,13 +2818,13 @@
       <c r="D8" s="14">
         <v>101044032</v>
       </c>
-      <c r="E8" s="53" t="s">
+      <c r="E8" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="G8" s="18"/>
+      <c r="F8" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="55"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
@@ -2861,13 +2839,13 @@
       <c r="D9" s="14">
         <v>101044032</v>
       </c>
-      <c r="E9" s="52" t="s">
+      <c r="E9" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="G9" s="14"/>
+      <c r="F9" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" s="55"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -2880,15 +2858,15 @@
         <v>101010134</v>
       </c>
       <c r="D10" s="14">
-        <v>101041082</v>
-      </c>
-      <c r="E10" s="52" t="s">
+        <v>101044082</v>
+      </c>
+      <c r="E10" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" s="14"/>
+      <c r="F10" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="55"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
@@ -2903,13 +2881,13 @@
       <c r="D11" s="14">
         <v>101041002</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="E11" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="G11" s="14"/>
+      <c r="F11" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" s="55"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
@@ -2924,13 +2902,13 @@
       <c r="D12" s="14">
         <v>101044022</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="E12" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12" s="14"/>
+      <c r="F12" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="55"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
@@ -2945,13 +2923,13 @@
       <c r="D13" s="14">
         <v>101044022</v>
       </c>
-      <c r="E13" s="52" t="s">
+      <c r="E13" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="14"/>
+      <c r="F13" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="55"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
@@ -2966,13 +2944,13 @@
       <c r="D14" s="14">
         <v>101044052</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="G14" s="14"/>
+      <c r="F14" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="55"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
@@ -2987,13 +2965,13 @@
       <c r="D15" s="14">
         <v>101044052</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="E15" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="G15" s="14"/>
+      <c r="F15" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G15" s="55"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
@@ -3008,13 +2986,13 @@
       <c r="D16" s="14">
         <v>101044062</v>
       </c>
-      <c r="E16" s="52" t="s">
+      <c r="E16" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" s="14"/>
+      <c r="F16" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="55"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
@@ -3029,13 +3007,13 @@
       <c r="D17" s="14">
         <v>101044042</v>
       </c>
-      <c r="E17" s="52" t="s">
+      <c r="E17" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="G17" s="14"/>
+      <c r="F17" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="55"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
@@ -3050,13 +3028,13 @@
       <c r="D18" s="14">
         <v>101044082</v>
       </c>
-      <c r="E18" s="52" t="s">
+      <c r="E18" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="G18" s="14"/>
+      <c r="F18" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="55"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -3071,13 +3049,13 @@
       <c r="D19" s="14">
         <v>101044102</v>
       </c>
-      <c r="E19" s="52" t="s">
+      <c r="E19" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="G19" s="14"/>
+      <c r="F19" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="55"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
@@ -3092,25 +3070,26 @@
       <c r="D20" s="14">
         <v>101044092</v>
       </c>
-      <c r="E20" s="52" t="s">
+      <c r="E20" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="G20" s="14"/>
+      <c r="F20" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="55"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="20" t="s">
+      <c r="A21" s="18"/>
+      <c r="B21" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="20">
         <v>101010201</v>
       </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="57"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="56"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
@@ -3122,15 +3101,16 @@
       <c r="C22" s="6">
         <v>101010203</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="14">
         <v>101052002</v>
       </c>
-      <c r="E22" s="55" t="s">
+      <c r="E22" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="57" t="s">
-        <v>84</v>
-      </c>
+      <c r="F22" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" s="57"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
@@ -3142,13 +3122,13 @@
       <c r="C23" s="6">
         <v>101010204</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="14">
         <v>101052002</v>
       </c>
-      <c r="E23" s="55" t="s">
+      <c r="E23" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="57" t="s">
+      <c r="F23" s="53" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3162,13 +3142,13 @@
       <c r="C24" s="6">
         <v>101010205</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="14">
         <v>101052002</v>
       </c>
-      <c r="E24" s="55" t="s">
+      <c r="E24" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="57" t="s">
+      <c r="F24" s="53" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3182,13 +3162,13 @@
       <c r="C25" s="6">
         <v>101010233</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="14">
         <v>101052002</v>
       </c>
-      <c r="E25" s="55" t="s">
+      <c r="E25" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="57" t="s">
+      <c r="F25" s="53" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3202,13 +3182,13 @@
       <c r="C26" s="17">
         <v>101010208</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="14">
         <v>101052002</v>
       </c>
-      <c r="E26" s="55" t="s">
+      <c r="E26" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F26" s="57" t="s">
+      <c r="F26" s="53" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3222,13 +3202,13 @@
       <c r="C27" s="6">
         <v>101010232</v>
       </c>
-      <c r="D27" s="23">
+      <c r="D27" s="14">
         <v>101052002</v>
       </c>
-      <c r="E27" s="55" t="s">
+      <c r="E27" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="57" t="s">
+      <c r="F27" s="53" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3242,13 +3222,13 @@
       <c r="C28" s="6">
         <v>101010234</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="14">
         <v>101052002</v>
       </c>
-      <c r="E28" s="55" t="s">
+      <c r="E28" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F28" s="57" t="s">
+      <c r="F28" s="53" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3262,13 +3242,13 @@
       <c r="C29" s="6">
         <v>101010210</v>
       </c>
-      <c r="D29" s="23">
+      <c r="D29" s="14">
         <v>101052002</v>
       </c>
-      <c r="E29" s="55" t="s">
+      <c r="E29" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F29" s="57" t="s">
+      <c r="F29" s="53" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3282,13 +3262,13 @@
       <c r="C30" s="6">
         <v>101010212</v>
       </c>
-      <c r="D30" s="23">
+      <c r="D30" s="14">
         <v>101052002</v>
       </c>
-      <c r="E30" s="55" t="s">
+      <c r="E30" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F30" s="57" t="s">
+      <c r="F30" s="53" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3302,13 +3282,13 @@
       <c r="C31" s="6">
         <v>101010213</v>
       </c>
-      <c r="D31" s="23">
+      <c r="D31" s="14">
         <v>101052002</v>
       </c>
-      <c r="E31" s="55" t="s">
+      <c r="E31" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F31" s="57" t="s">
+      <c r="F31" s="53" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3322,13 +3302,13 @@
       <c r="C32" s="6">
         <v>101010215</v>
       </c>
-      <c r="D32" s="23">
+      <c r="D32" s="14">
         <v>101052002</v>
       </c>
-      <c r="E32" s="55" t="s">
+      <c r="E32" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F32" s="57" t="s">
+      <c r="F32" s="53" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3342,13 +3322,13 @@
       <c r="C33" s="6">
         <v>101010216</v>
       </c>
-      <c r="D33" s="23">
+      <c r="D33" s="14">
         <v>101052002</v>
       </c>
-      <c r="E33" s="55" t="s">
+      <c r="E33" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F33" s="57" t="s">
+      <c r="F33" s="53" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3362,13 +3342,13 @@
       <c r="C34" s="6">
         <v>101010218</v>
       </c>
-      <c r="D34" s="23">
+      <c r="D34" s="14">
         <v>101052002</v>
       </c>
-      <c r="E34" s="55" t="s">
+      <c r="E34" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F34" s="57" t="s">
+      <c r="F34" s="53" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3382,13 +3362,13 @@
       <c r="C35" s="6">
         <v>101010220</v>
       </c>
-      <c r="D35" s="23">
+      <c r="D35" s="14">
         <v>101052002</v>
       </c>
-      <c r="E35" s="55" t="s">
+      <c r="E35" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F35" s="57" t="s">
+      <c r="F35" s="53" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3402,13 +3382,13 @@
       <c r="C36" s="6">
         <v>101010222</v>
       </c>
-      <c r="D36" s="23">
+      <c r="D36" s="14">
         <v>101052002</v>
       </c>
-      <c r="E36" s="55" t="s">
+      <c r="E36" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F36" s="57" t="s">
+      <c r="F36" s="53" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3422,13 +3402,13 @@
       <c r="C37" s="6">
         <v>101010236</v>
       </c>
-      <c r="D37" s="23">
+      <c r="D37" s="14">
         <v>101052002</v>
       </c>
-      <c r="E37" s="55" t="s">
+      <c r="E37" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F37" s="57" t="s">
+      <c r="F37" s="53" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3442,13 +3422,13 @@
       <c r="C38" s="6">
         <v>101010237</v>
       </c>
-      <c r="D38" s="23">
+      <c r="D38" s="14">
         <v>101052002</v>
       </c>
-      <c r="E38" s="55" t="s">
+      <c r="E38" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F38" s="57" t="s">
+      <c r="F38" s="53" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3492,11 +3472,173 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F20 F22:F38" xr:uid="{4DDA8D3B-06EF-40B5-B0B2-CBEB1310B5C8}">
       <formula1>"SI,NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D20" xr:uid="{6CF02B72-412D-483F-BD39-02D1D4C5A24B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G20" xr:uid="{6CF02B72-412D-483F-BD39-02D1D4C5A24B}">
       <formula1>"101044032,101044042,101044012,101044082,101044052,101044022,101044062,101044102,101041002,101041012,101041082,101044092,101044072,101044002"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.38" bottom="0.27" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DE757339-8787-490F-892F-3451C25EEE25}">
+          <x14:formula1>
+            <xm:f>Hoja1!$A$1:$A$26</xm:f>
+          </x14:formula1>
+          <xm:sqref>D22:D38 D4:D20</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EDB91D8-B6A7-47AC-8AE5-E5652C735329}">
+  <dimension ref="A1:A26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>101052002</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>101044002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>101044012</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>101044022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>101044032</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>101044042</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>101044052</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>101044062</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>101044072</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>101044082</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>101051002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>101041032</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>101041022</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>101041012</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>101041002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>101043002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>101042022</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>101051012</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>101041042</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>101041052</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>101041082</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>101043042</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>101042012</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>101045012</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <v>101044092</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>101044102</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A25" xr:uid="{9F1E8086-2992-4260-B7D0-122C2D5EBCD7}">
+      <formula1>"101052002,101044002,101044012,101044022,101044032,101044042,101044052,101044062,101044072,101044082,101051002,101041032,101041022,101041012,101041002,101043002,101042022,101051012,101041042,101041052,101041082,101043042,101042012,101045012,101044092"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>